<commit_message>
Missile launcher rebalanced again.
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Acceleration</t>
   </si>
@@ -106,6 +106,18 @@
   <si>
     <t>Time to Regen after Combat</t>
   </si>
+  <si>
+    <t>Time to Top Speed</t>
+  </si>
+  <si>
+    <t>Time to Kill Vanilla</t>
+  </si>
+  <si>
+    <t>Time to Kill StatMax</t>
+  </si>
+  <si>
+    <t>Time to Kill AbsMax</t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -200,17 +218,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="27">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -220,6 +236,30 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2096,16 +2136,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2128,23 +2168,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="22">
   <autoFilter ref="A1:F37"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Stat Level" dataDxfId="1"/>
-    <tableColumn id="2" name="0-1 Value" dataDxfId="2">
+    <tableColumn id="1" name="Stat Level" dataDxfId="11"/>
+    <tableColumn id="2" name="0-1 Value" dataDxfId="12">
       <calculatedColumnFormula>0 + ((1 - 0) * ((Table1[[#This Row],[Stat Level]] - 1) / (36 - 1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Smooth Stop" dataDxfId="19">
+    <tableColumn id="3" name="Smooth Stop" dataDxfId="26">
       <calculatedColumnFormula>1-((1-B2)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Smooth Start" dataDxfId="18">
+    <tableColumn id="4" name="Smooth Start" dataDxfId="25">
       <calculatedColumnFormula>B2^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Smooth Step" dataDxfId="17">
+    <tableColumn id="5" name="Smooth Step" dataDxfId="24">
       <calculatedColumnFormula>B2*B2*(3 - 2*B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Selected Blend" dataDxfId="16">
+    <tableColumn id="6" name="Selected Blend" dataDxfId="23">
       <calculatedColumnFormula>Table1[[#This Row],[Smooth Stop]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2153,47 +2193,81 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="H1:S37"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Top Speed" dataDxfId="0">
+    <tableColumn id="1" name="Top Speed" dataDxfId="10">
       <calculatedColumnFormula>H$39 + ((H$40 - H$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Acceleration" dataDxfId="14">
-      <calculatedColumnFormula>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
+    <tableColumn id="2" name="Acceleration" dataDxfId="5">
+      <calculatedColumnFormula>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Handling" dataDxfId="13">
+    <tableColumn id="3" name="Handling" dataDxfId="21">
       <calculatedColumnFormula>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Braking" dataDxfId="12">
+    <tableColumn id="4" name="Braking" dataDxfId="20">
       <calculatedColumnFormula>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Damage" dataDxfId="11">
+    <tableColumn id="5" name="Damage" dataDxfId="19">
       <calculatedColumnFormula>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Shield Disruption" dataDxfId="10">
+    <tableColumn id="6" name="Shield Disruption" dataDxfId="18">
       <calculatedColumnFormula>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Shot Homing" dataDxfId="9">
+    <tableColumn id="7" name="Shot Homing" dataDxfId="17">
       <calculatedColumnFormula>N$39 + ((N$40 - N$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Rate of Fire" dataDxfId="8">
+    <tableColumn id="8" name="Rate of Fire" dataDxfId="16">
       <calculatedColumnFormula>O$39 + ((O$40 - O$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="HP" dataDxfId="7">
-      <calculatedColumnFormula>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
+    <tableColumn id="9" name="HP" dataDxfId="4">
+      <calculatedColumnFormula>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Shield Capacity" dataDxfId="6">
-      <calculatedColumnFormula>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
+    <tableColumn id="10" name="Shield Capacity" dataDxfId="3">
+      <calculatedColumnFormula>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Shield Regen" dataDxfId="5">
+    <tableColumn id="11" name="Shield Regen" dataDxfId="15">
       <calculatedColumnFormula>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Shot Deflection" dataDxfId="4">
+    <tableColumn id="12" name="Shot Deflection" dataDxfId="14">
       <calculatedColumnFormula>S$39 + ((S$40 - S$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="U1:AC37" totalsRowShown="0">
+  <autoFilter ref="U1:AC37"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Time To Pop Shield" dataDxfId="9">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Time To Deplete HP" dataDxfId="8">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Time to Kill" dataDxfId="7">
+      <calculatedColumnFormula>U2 + V2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Time to Kill Vanilla" dataDxfId="2">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Time to Kill StatMax" dataDxfId="1">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Time to Regen Shield">
+      <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Time to Regen after Combat">
+      <calculatedColumnFormula>AA2 + $U$43</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Time to Top Speed" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2494,10 +2568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,14 +2595,17 @@
     <col min="18" max="18" width="14.7109375" customWidth="1"/>
     <col min="19" max="19" width="16.85546875" customWidth="1"/>
     <col min="20" max="20" width="22.42578125" customWidth="1"/>
-    <col min="21" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="19.85546875" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" customWidth="1"/>
-    <col min="25" max="25" width="27.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="20.5703125" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" customWidth="1"/>
+    <col min="25" max="26" width="20.85546875" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" customWidth="1"/>
+    <col min="28" max="28" width="27.85546875" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2593,13 +2670,25 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2629,12 +2718,12 @@
         <v>2</v>
       </c>
       <c r="I2" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.2</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.05</v>
       </c>
       <c r="J2" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="K2" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2642,7 +2731,7 @@
       </c>
       <c r="L2" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M2" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2657,11 +2746,11 @@
         <v>3</v>
       </c>
       <c r="P2" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>50</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>20</v>
       </c>
       <c r="Q2" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
         <v>30</v>
       </c>
       <c r="R2" s="2">
@@ -2674,7 +2763,7 @@
       </c>
       <c r="U2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -2682,18 +2771,31 @@
       </c>
       <c r="W2" s="2">
         <f>U2 + V2</f>
-        <v>5.3333333333333339</v>
-      </c>
-      <c r="X2">
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="X2" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>0.69863125305523921</v>
+      </c>
+      <c r="Y2" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.11507904554848752</v>
+      </c>
+      <c r="Z2" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.1</v>
+      </c>
+      <c r="AA2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3</v>
       </c>
-      <c r="Y2">
-        <f>X2 + $U$43</f>
+      <c r="AB2">
+        <f>AA2 + $U$43</f>
         <v>6</v>
       </c>
+      <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2723,12 +2825,12 @@
         <v>2.0312303206997084</v>
       </c>
       <c r="I3" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.30138775510204086</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>9.7877551020408182E-2</v>
       </c>
       <c r="J3" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.30138775510204086</v>
+        <v>9.7877551020408182E-2</v>
       </c>
       <c r="K3" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2736,7 +2838,7 @@
       </c>
       <c r="L3" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>7.534693877551021</v>
+        <v>4.7036734693877555</v>
       </c>
       <c r="M3" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2751,12 +2853,12 @@
         <v>3.3942857142857141</v>
       </c>
       <c r="P3" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>103.51020408163266</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>22.354285714285716</v>
       </c>
       <c r="Q3" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>70.555102040816337</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>31.729679300291544</v>
       </c>
       <c r="R3" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2768,26 +2870,39 @@
       </c>
       <c r="U3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.7587631460870901</v>
+        <v>1.9873763669320765</v>
       </c>
       <c r="V3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>4.0473350332505262</v>
+        <v>1.4001521637759056</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" ref="W3:W37" si="2">U3 + V3</f>
-        <v>6.8060981793376163</v>
-      </c>
-      <c r="X3">
+        <v>3.3875285307079821</v>
+      </c>
+      <c r="X3" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>0.75569496496659661</v>
+      </c>
+      <c r="Y3" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.12447862146710684</v>
+      </c>
+      <c r="Z3" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.10816793002915452</v>
+      </c>
+      <c r="AA3">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.7581612258494346</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y37" si="3">X3 + $U$43</f>
-        <v>8.7581612258494346</v>
-      </c>
+        <v>2.589530788997811</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB37" si="3">AA3 + $U$43</f>
+        <v>5.589530788997811</v>
+      </c>
+      <c r="AC3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2817,12 +2932,12 @@
         <v>2.1224956268221575</v>
       </c>
       <c r="I4" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.39983673469387759</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.14436734693877551</v>
       </c>
       <c r="J4" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.39983673469387759</v>
+        <v>0.14436734693877551</v>
       </c>
       <c r="K4" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2830,7 +2945,7 @@
       </c>
       <c r="L4" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>9.9959183673469383</v>
+        <v>7.3289795918367346</v>
       </c>
       <c r="M4" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2845,12 +2960,12 @@
         <v>3.7771428571428571</v>
       </c>
       <c r="P4" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>155.46938775510205</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>29.234285714285711</v>
       </c>
       <c r="Q4" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>109.93469387755101</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>36.784373177842568</v>
       </c>
       <c r="R4" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2862,26 +2977,39 @@
       </c>
       <c r="U4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.9117136328452937</v>
+        <v>1.3287902618908081</v>
       </c>
       <c r="V4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>4.1177386305441912</v>
+        <v>1.0560526336187734</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="2"/>
-        <v>7.0294522633894854</v>
-      </c>
-      <c r="X4">
+        <v>2.3848428955095815</v>
+      </c>
+      <c r="X4" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>0.92245396773667987</v>
+      </c>
+      <c r="Y4" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.15194728507394584</v>
+      </c>
+      <c r="Z4" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.13203731778425656</v>
+      </c>
+      <c r="AA4">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.6127755794234027</v>
-      </c>
-      <c r="Y4">
+        <v>2.5472502624565938</v>
+      </c>
+      <c r="AB4">
         <f t="shared" si="3"/>
-        <v>10.612775579423403</v>
-      </c>
+        <v>5.5472502624565934</v>
+      </c>
+      <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2911,12 +3039,12 @@
         <v>2.2701574344023325</v>
       </c>
       <c r="I5" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.49534693877551039</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.18946938775510208</v>
       </c>
       <c r="J5" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.49534693877551039</v>
+        <v>0.18946938775510208</v>
       </c>
       <c r="K5" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2924,7 +3052,7 @@
       </c>
       <c r="L5" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>12.383673469387759</v>
+        <v>9.8759183673469426</v>
       </c>
       <c r="M5" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2939,12 +3067,12 @@
         <v>4.1485714285714295</v>
       </c>
       <c r="P5" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>205.87755102040825</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>40.36571428571429</v>
       </c>
       <c r="Q5" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>148.13877551020414</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>44.962565597667641</v>
       </c>
       <c r="R5" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2956,26 +3084,39 @@
       </c>
       <c r="U5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.8835048513540751</v>
+        <v>1.0974254333412115</v>
       </c>
       <c r="V5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>4.0073837191353814</v>
+        <v>0.98522761998317643</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="2"/>
-        <v>6.8908885704894569</v>
-      </c>
-      <c r="X5">
+        <v>2.0826530533243881</v>
+      </c>
+      <c r="X5" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>1.1922600619195056</v>
+      </c>
+      <c r="Y5" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.19638994014547601</v>
+      </c>
+      <c r="Z5" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.17065655976676386</v>
+      </c>
+      <c r="AA5">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>8.9438146870379516</v>
-      </c>
-      <c r="Y5">
+        <v>2.7145955079912691</v>
+      </c>
+      <c r="AB5">
         <f t="shared" si="3"/>
-        <v>11.943814687037952</v>
-      </c>
+        <v>5.7145955079912696</v>
+      </c>
+      <c r="AC5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3005,12 +3146,12 @@
         <v>2.4705772594752187</v>
       </c>
       <c r="I6" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.58791836734693881</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.23318367346938779</v>
       </c>
       <c r="J6" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.58791836734693881</v>
+        <v>0.23318367346938779</v>
       </c>
       <c r="K6" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3018,7 +3159,7 @@
       </c>
       <c r="L6" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>14.69795918367347</v>
+        <v>12.344489795918369</v>
       </c>
       <c r="M6" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3033,12 +3174,12 @@
         <v>4.5085714285714289</v>
       </c>
       <c r="P6" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>254.73469387755105</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>55.474285714285713</v>
       </c>
       <c r="Q6" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>185.16734693877552</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>56.06274052478134</v>
       </c>
       <c r="R6" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3050,26 +3191,39 @@
       </c>
       <c r="U6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.7942702861372473</v>
+        <v>1.0073078630937322</v>
       </c>
       <c r="V6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.8440772507566372</v>
+        <v>0.99673479527473108</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="2"/>
-        <v>6.6383475368938845</v>
-      </c>
-      <c r="X6">
+        <v>2.0040426583684634</v>
+      </c>
+      <c r="X6" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>1.55846504806909</v>
+      </c>
+      <c r="Y6" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.25671149045816888</v>
+      </c>
+      <c r="Z6" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.22307405247813411</v>
+      </c>
+      <c r="AA6">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>9.9443226654975891</v>
-      </c>
-      <c r="Y6">
+        <v>3.0108223210371392</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="3"/>
-        <v>12.944322665497589</v>
-      </c>
+        <v>6.0108223210371392</v>
+      </c>
+      <c r="AC6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -3099,12 +3253,12 @@
         <v>2.7201166180758016</v>
       </c>
       <c r="I7" s="5">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.67755102040816295</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.27551020408163251</v>
       </c>
       <c r="J7" s="5">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.67755102040816295</v>
+        <v>0.27551020408163251</v>
       </c>
       <c r="K7" s="5">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3112,7 +3266,7 @@
       </c>
       <c r="L7" s="5">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>16.938775510204074</v>
+        <v>14.734693877551013</v>
       </c>
       <c r="M7" s="5">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3127,12 +3281,12 @@
         <v>4.8571428571428559</v>
       </c>
       <c r="P7" s="5">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>302.04081632653049</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>74.285714285714278</v>
       </c>
       <c r="Q7" s="5">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>221.02040816326519</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>69.883381924198247</v>
       </c>
       <c r="R7" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3144,26 +3298,39 @@
       </c>
       <c r="U7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.6863926293408933</v>
+        <v>0.97645429362880953</v>
       </c>
       <c r="V7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.6711552090715815</v>
+        <v>1.0379664331106411</v>
       </c>
       <c r="W7" s="12">
         <f t="shared" si="2"/>
-        <v>6.3575478384124748</v>
-      </c>
-      <c r="X7" s="1">
+        <v>2.0144207267394507</v>
+      </c>
+      <c r="X7" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.0144207267394507</v>
+      </c>
+      <c r="Y7" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.33181683978849608</v>
+      </c>
+      <c r="Z7" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.28833819241982506</v>
+      </c>
+      <c r="AA7" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>10.722772277227719</v>
-      </c>
-      <c r="Y7" s="1">
+        <v>3.390381895332391</v>
+      </c>
+      <c r="AB7" s="13">
         <f t="shared" si="3"/>
-        <v>13.722772277227719</v>
-      </c>
+        <v>6.390381895332391</v>
+      </c>
+      <c r="AC7" s="12"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3193,12 +3360,12 @@
         <v>3.0151370262390671</v>
       </c>
       <c r="I8" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.76424489795918382</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.31644897959183682</v>
       </c>
       <c r="J8" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.76424489795918382</v>
+        <v>0.31644897959183682</v>
       </c>
       <c r="K8" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3206,7 +3373,7 @@
       </c>
       <c r="L8" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>19.106122448979598</v>
+        <v>17.046530612244901</v>
       </c>
       <c r="M8" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3221,12 +3388,12 @@
         <v>5.1942857142857148</v>
       </c>
       <c r="P8" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>347.79591836734704</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>96.525714285714287</v>
       </c>
       <c r="Q8" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>255.69795918367353</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>86.222973760932945</v>
       </c>
       <c r="R8" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3238,26 +3405,39 @@
       </c>
       <c r="U8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.5764924281362123</v>
+        <v>0.97378069384373522</v>
       </c>
       <c r="V8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.5045002043464328</v>
+        <v>1.0901372677254313</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="2"/>
-        <v>6.0809926324826451</v>
-      </c>
-      <c r="X8">
+        <v>2.0639179615691665</v>
+      </c>
+      <c r="X8" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.5534788984846033</v>
+      </c>
+      <c r="Y8" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.42061089191292911</v>
+      </c>
+      <c r="Z8" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.36549737609329447</v>
+      </c>
+      <c r="AA8">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>11.344802607750815</v>
-      </c>
-      <c r="Y8">
+        <v>3.8255394008382049</v>
+      </c>
+      <c r="AB8">
         <f t="shared" si="3"/>
-        <v>14.344802607750815</v>
-      </c>
+        <v>6.8255394008382044</v>
+      </c>
+      <c r="AC8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3287,12 +3467,12 @@
         <v>3.3520000000000003</v>
       </c>
       <c r="I9" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.84799999999999986</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.35599999999999987</v>
       </c>
       <c r="J9" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.84799999999999986</v>
+        <v>0.35599999999999987</v>
       </c>
       <c r="K9" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3300,7 +3480,7 @@
       </c>
       <c r="L9" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>21.199999999999996</v>
+        <v>19.279999999999994</v>
       </c>
       <c r="M9" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3315,12 +3495,12 @@
         <v>5.52</v>
       </c>
       <c r="P9" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>391.99999999999989</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>121.92000000000002</v>
       </c>
       <c r="Q9" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>289.19999999999993</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>104.88000000000001</v>
       </c>
       <c r="R9" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3332,26 +3512,39 @@
       </c>
       <c r="U9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.4712879409351927</v>
+        <v>0.98547717842323701</v>
       </c>
       <c r="V9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.3497402242275087</v>
+        <v>1.1455890312105363</v>
       </c>
       <c r="W9" s="2">
         <f t="shared" si="2"/>
-        <v>5.8210281651627014</v>
-      </c>
-      <c r="X9">
+        <v>2.1310662096337731</v>
+      </c>
+      <c r="X9" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>3.1689913638585656</v>
+      </c>
+      <c r="Y9" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.52199855060793943</v>
+      </c>
+      <c r="Z9" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.45360000000000006</v>
+      </c>
+      <c r="AA9">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>11.852459016393443</v>
-      </c>
-      <c r="Y9">
+        <v>4.2983606557377065</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="3"/>
-        <v>14.852459016393443</v>
-      </c>
+        <v>7.2983606557377065</v>
+      </c>
+      <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -3381,12 +3574,12 @@
         <v>3.7270670553935856</v>
       </c>
       <c r="I10" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.92881632653061219</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.39416326530612239</v>
       </c>
       <c r="J10" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>0.92881632653061219</v>
+        <v>0.39416326530612239</v>
       </c>
       <c r="K10" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3394,7 +3587,7 @@
       </c>
       <c r="L10" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>23.220408163265304</v>
+        <v>21.435102040816325</v>
       </c>
       <c r="M10" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3409,12 +3602,12 @@
         <v>5.8342857142857145</v>
       </c>
       <c r="P10" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>434.65306122448976</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>150.19428571428571</v>
       </c>
       <c r="Q10" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>321.52653061224487</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>125.65294460641398</v>
       </c>
       <c r="R10" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3426,26 +3619,39 @@
       </c>
       <c r="U10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.3733362440257491</v>
+        <v>1.0047532549941964</v>
       </c>
       <c r="V10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.2083755633369138</v>
+        <v>1.2009921289600543</v>
       </c>
       <c r="W10" s="2">
         <f t="shared" si="2"/>
-        <v>5.5817118073626624</v>
-      </c>
-      <c r="X10">
+        <v>2.2057453839542509</v>
+      </c>
+      <c r="X10" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>3.8543099234153519</v>
+      </c>
+      <c r="Y10" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.6348847196499986</v>
+      </c>
+      <c r="Z10" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.55169446064139938</v>
+      </c>
+      <c r="AA10">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.273917108133375</v>
-      </c>
-      <c r="Y10">
+        <v>4.7966611761563458</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="3"/>
-        <v>15.273917108133375</v>
-      </c>
+        <v>7.7966611761563458</v>
+      </c>
+      <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -3475,12 +3681,12 @@
         <v>4.1366997084548096</v>
       </c>
       <c r="I11" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.0066938775510204</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.43093877551020399</v>
       </c>
       <c r="J11" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.0066938775510204</v>
+        <v>0.43093877551020399</v>
       </c>
       <c r="K11" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3488,7 +3694,7 @@
       </c>
       <c r="L11" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>25.167346938775506</v>
+        <v>23.511836734693873</v>
       </c>
       <c r="M11" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3503,12 +3709,12 @@
         <v>6.137142857142857</v>
       </c>
       <c r="P11" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>475.75510204081627</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>181.07428571428568</v>
       </c>
       <c r="Q11" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>352.67755102040809</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>148.34029154518947</v>
       </c>
       <c r="R11" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3520,26 +3726,39 @@
       </c>
       <c r="U11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.2833587324252478</v>
+        <v>1.0280313013644693</v>
       </c>
       <c r="V11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.0802061645196734</v>
+        <v>1.2548851808734056</v>
       </c>
       <c r="W11" s="2">
         <f t="shared" si="2"/>
-        <v>5.3635648969449212</v>
-      </c>
-      <c r="X11">
+        <v>2.2829164822378747</v>
+      </c>
+      <c r="X11" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>4.6027863777089806</v>
+      </c>
+      <c r="Y11" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.75817430281557807</v>
+      </c>
+      <c r="Z11" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.6588291545189503</v>
+      </c>
+      <c r="AA11">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.628763519438758</v>
-      </c>
-      <c r="Y11">
+        <v>5.3118052365640782</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="3"/>
-        <v>15.628763519438758</v>
-      </c>
+        <v>8.3118052365640782</v>
+      </c>
+      <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -3569,12 +3788,12 @@
         <v>4.5772594752186588</v>
       </c>
       <c r="I12" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.0816326530612246</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.46632653061224488</v>
       </c>
       <c r="J12" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.0816326530612246</v>
+        <v>0.46632653061224488</v>
       </c>
       <c r="K12" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3582,7 +3801,7 @@
       </c>
       <c r="L12" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>27.04081632653061</v>
+        <v>25.510204081632651</v>
       </c>
       <c r="M12" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3597,12 +3816,12 @@
         <v>6.4285714285714288</v>
       </c>
       <c r="P12" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>515.30612244897952</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>214.28571428571428</v>
       </c>
       <c r="Q12" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>382.65306122448976</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>172.74052478134112</v>
       </c>
       <c r="R12" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3614,26 +3833,39 @@
       </c>
       <c r="U12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.2012578616352201</v>
+        <v>1.0533333333333335</v>
       </c>
       <c r="V12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.9643605870020964</v>
+        <v>1.3066666666666666</v>
       </c>
       <c r="W12" s="2">
         <f t="shared" si="2"/>
-        <v>5.165618448637316</v>
-      </c>
-      <c r="X12">
+        <v>2.3600000000000003</v>
+      </c>
+      <c r="X12" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>5.4077725272934698</v>
+      </c>
+      <c r="Y12" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>0.89077220388114986</v>
+      </c>
+      <c r="Z12" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.77405247813411071</v>
+      </c>
+      <c r="AA12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.931034482758619</v>
-      </c>
-      <c r="Y12">
+        <v>5.8374384236453203</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="3"/>
-        <v>15.931034482758619</v>
-      </c>
+        <v>8.8374384236453203</v>
+      </c>
+      <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -3663,12 +3895,12 @@
         <v>5.0451078717201163</v>
       </c>
       <c r="I13" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.1536326530612244</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.50032653061224486</v>
       </c>
       <c r="J13" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.1536326530612244</v>
+        <v>0.50032653061224486</v>
       </c>
       <c r="K13" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3676,7 +3908,7 @@
       </c>
       <c r="L13" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>28.840816326530607</v>
+        <v>27.430204081632649</v>
       </c>
       <c r="M13" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3691,12 +3923,12 @@
         <v>6.7085714285714282</v>
       </c>
       <c r="P13" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>553.30612244897952</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>249.5542857142857</v>
       </c>
       <c r="Q13" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>411.45306122448972</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>198.65212827988339</v>
       </c>
       <c r="R13" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3708,26 +3940,39 @@
       </c>
       <c r="U13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.126584777934597</v>
+        <v>1.079528556901223</v>
       </c>
       <c r="V13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.8597487500427947</v>
+        <v>1.356144433278339</v>
       </c>
       <c r="W13" s="2">
         <f t="shared" si="2"/>
-        <v>4.9863335279773917</v>
-      </c>
-      <c r="X13">
+        <v>2.4356729901795617</v>
+      </c>
+      <c r="X13" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>6.2626201727228334</v>
+      </c>
+      <c r="Y13" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.0315833266231849</v>
+      </c>
+      <c r="Z13" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>0.8964128279883381</v>
+      </c>
+      <c r="AA13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.191049463491233</v>
-      </c>
-      <c r="Y13">
+        <v>6.3687217258010254</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="3"/>
-        <v>16.191049463491233</v>
-      </c>
+        <v>9.3687217258010254</v>
+      </c>
+      <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -3757,12 +4002,12 @@
         <v>5.5366064139941686</v>
       </c>
       <c r="I14" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.2226938775510203</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.53293877551020408</v>
       </c>
       <c r="J14" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.2226938775510203</v>
+        <v>0.53293877551020408</v>
       </c>
       <c r="K14" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3770,7 +4015,7 @@
       </c>
       <c r="L14" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>30.567346938775508</v>
+        <v>29.271836734693874</v>
       </c>
       <c r="M14" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3785,12 +4030,12 @@
         <v>6.9771428571428569</v>
       </c>
       <c r="P14" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>589.75510204081627</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>286.60571428571427</v>
       </c>
       <c r="Q14" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>439.07755102040812</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>225.8735860058309</v>
       </c>
       <c r="R14" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3802,26 +4047,39 @@
       </c>
       <c r="U14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0587607114513244</v>
+        <v>1.1059560211771715</v>
       </c>
       <c r="V14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.7652623793630604</v>
+        <v>1.4033217474569475</v>
       </c>
       <c r="W14" s="2">
         <f t="shared" si="2"/>
-        <v>4.8240230908143849</v>
-      </c>
-      <c r="X14">
+        <v>2.509277768634119</v>
+      </c>
+      <c r="X14" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>7.1606811145510889</v>
+      </c>
+      <c r="Y14" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.1795125748181547</v>
+      </c>
+      <c r="Z14" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.0249586005830904</v>
+      </c>
+      <c r="AA14">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.41656273384884</v>
-      </c>
-      <c r="Y14">
+        <v>6.9018494102554975</v>
+      </c>
+      <c r="AB14">
         <f t="shared" si="3"/>
-        <v>16.416562733848842</v>
-      </c>
+        <v>9.9018494102554975</v>
+      </c>
+      <c r="AC14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -3851,12 +4109,12 @@
         <v>6.0481166180758024</v>
       </c>
       <c r="I15" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.2888163265306123</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.56416326530612249</v>
       </c>
       <c r="J15" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.2888163265306123</v>
+        <v>0.56416326530612249</v>
       </c>
       <c r="K15" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3864,7 +4122,7 @@
       </c>
       <c r="L15" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>32.220408163265304</v>
+        <v>31.035102040816327</v>
       </c>
       <c r="M15" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3879,12 +4137,12 @@
         <v>7.2342857142857149</v>
       </c>
       <c r="P15" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>624.65306122448987</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>325.16571428571433</v>
       </c>
       <c r="Q15" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>465.52653061224493</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>254.20338192419828</v>
       </c>
       <c r="R15" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3896,26 +4154,39 @@
       </c>
       <c r="U15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9971824542486525</v>
+        <v>1.1322243467112985</v>
       </c>
       <c r="V15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.6798604415295717</v>
+        <v>1.4482912683665183</v>
       </c>
       <c r="W15" s="2">
         <f t="shared" si="2"/>
-        <v>4.6770428957782242</v>
-      </c>
-      <c r="X15">
+        <v>2.5805156150778168</v>
+      </c>
+      <c r="X15" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>8.0953071533322536</v>
+      </c>
+      <c r="Y15" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.3334648522425316</v>
+      </c>
+      <c r="Z15" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.1587381924198252</v>
+      </c>
+      <c r="AA15">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.61351157794223</v>
-      </c>
-      <c r="Y15">
+        <v>7.4337346110561677</v>
+      </c>
+      <c r="AB15">
         <f t="shared" si="3"/>
-        <v>16.61351157794223</v>
-      </c>
+        <v>10.433734611056167</v>
+      </c>
+      <c r="AC15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -3945,12 +4216,12 @@
         <v>6.5760000000000014</v>
       </c>
       <c r="I16" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.3520000000000001</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.59400000000000008</v>
       </c>
       <c r="J16" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.3520000000000001</v>
+        <v>0.59400000000000008</v>
       </c>
       <c r="K16" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3958,7 +4229,7 @@
       </c>
       <c r="L16" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>33.799999999999997</v>
+        <v>32.72</v>
       </c>
       <c r="M16" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3973,12 +4244,12 @@
         <v>7.48</v>
       </c>
       <c r="P16" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>658</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>364.96000000000009</v>
       </c>
       <c r="Q16" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>490.8</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>283.44000000000005</v>
       </c>
       <c r="R16" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3990,26 +4261,39 @@
       </c>
       <c r="U16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9412713982849732</v>
+        <v>1.1581004929199956</v>
       </c>
       <c r="V16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.6026010188906117</v>
+        <v>1.4911810467685633</v>
       </c>
       <c r="W16" s="2">
         <f t="shared" si="2"/>
-        <v>4.5438724171755851</v>
-      </c>
-      <c r="X16">
+        <v>2.649281539688559</v>
+      </c>
+      <c r="X16" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>9.059850089620344</v>
+      </c>
+      <c r="Y16" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.4923450626727868</v>
+      </c>
+      <c r="Z16" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.2968000000000004</v>
+      </c>
+      <c r="AA16">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.786516853932584</v>
-      </c>
-      <c r="Y16">
+        <v>7.96179775280899</v>
+      </c>
+      <c r="AB16">
         <f t="shared" si="3"/>
-        <v>16.786516853932582</v>
-      </c>
+        <v>10.961797752808991</v>
+      </c>
+      <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -4039,12 +4323,12 @@
         <v>7.1166180758017488</v>
       </c>
       <c r="I17" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.4122448979591837</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.62244897959183687</v>
       </c>
       <c r="J17" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.4122448979591837</v>
+        <v>0.62244897959183687</v>
       </c>
       <c r="K17" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4052,7 +4336,7 @@
       </c>
       <c r="L17" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>35.306122448979593</v>
+        <v>34.326530612244902</v>
       </c>
       <c r="M17" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4067,12 +4351,12 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="P17" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>689.79591836734699</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>405.71428571428567</v>
       </c>
       <c r="Q17" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>514.89795918367349</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>313.38192419825072</v>
       </c>
       <c r="R17" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4084,26 +4368,39 @@
       </c>
       <c r="U17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8904945407835578</v>
+        <v>1.1834456335050862</v>
       </c>
       <c r="V17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.5326482551916074</v>
+        <v>1.5321266569780239</v>
       </c>
       <c r="W17" s="2">
         <f t="shared" si="2"/>
-        <v>4.4231427959751652</v>
-      </c>
-      <c r="X17">
+        <v>2.7155722904831103</v>
+      </c>
+      <c r="X17" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>10.047661723969373</v>
+      </c>
+      <c r="Y17" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.6550581098853905</v>
+      </c>
+      <c r="Z17" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.4381924198250728</v>
+      </c>
+      <c r="AA17">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.939226519337018</v>
-      </c>
-      <c r="Y17">
+        <v>8.4838200473559588</v>
+      </c>
+      <c r="AB17">
         <f t="shared" si="3"/>
-        <v>16.939226519337019</v>
-      </c>
+        <v>11.483820047355959</v>
+      </c>
+      <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -4133,12 +4430,12 @@
         <v>7.6663323615160346</v>
       </c>
       <c r="I18" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.469551020408163</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.64951020408163262</v>
       </c>
       <c r="J18" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.469551020408163</v>
+        <v>0.64951020408163262</v>
       </c>
       <c r="K18" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4146,7 +4443,7 @@
       </c>
       <c r="L18" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>36.738775510204079</v>
+        <v>35.854693877551014</v>
       </c>
       <c r="M18" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4161,12 +4458,12 @@
         <v>7.9371428571428568</v>
       </c>
       <c r="P18" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>720.04081632653049</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>447.15428571428572</v>
       </c>
       <c r="Q18" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>537.82040816326526</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>343.82763848396502</v>
       </c>
       <c r="R18" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4178,26 +4475,39 @@
       </c>
       <c r="U18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8443715037182093</v>
+        <v>1.2081770127940334</v>
       </c>
       <c r="V18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.4692680734857952</v>
+        <v>1.5712568412313095</v>
       </c>
       <c r="W18" s="2">
         <f t="shared" si="2"/>
-        <v>4.3136395772040048</v>
-      </c>
-      <c r="X18">
+        <v>2.7794338540253429</v>
+      </c>
+      <c r="X18" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>11.052093856933363</v>
+      </c>
+      <c r="Y18" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.8205088976568162</v>
+      </c>
+      <c r="Z18" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.5819638483965015</v>
+      </c>
+      <c r="AA18">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.074556718649861</v>
-      </c>
-      <c r="Y18">
+        <v>8.9978392895291002</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="3"/>
-        <v>17.074556718649859</v>
-      </c>
+        <v>11.9978392895291</v>
+      </c>
+      <c r="AC18" s="2"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -4227,12 +4537,12 @@
         <v>8.2215043731778419</v>
       </c>
       <c r="I19" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.5239183673469388</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.67518367346938779</v>
       </c>
       <c r="J19" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.5239183673469388</v>
+        <v>0.67518367346938779</v>
       </c>
       <c r="K19" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4240,7 +4550,7 @@
       </c>
       <c r="L19" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>38.097959183673474</v>
+        <v>37.304489795918371</v>
       </c>
       <c r="M19" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4255,12 +4565,12 @@
         <v>8.1485714285714295</v>
       </c>
       <c r="P19" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>748.73469387755108</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>489.00571428571425</v>
       </c>
       <c r="Q19" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>559.56734693877559</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>374.5756268221574</v>
       </c>
       <c r="R19" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4272,26 +4582,39 @@
       </c>
       <c r="U19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8024746879931337</v>
+        <v>1.2322446279270998</v>
       </c>
       <c r="V19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.4118193120447313</v>
+        <v>1.6086862606795251</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="2"/>
-        <v>4.2142940000378655</v>
-      </c>
-      <c r="X19">
+        <v>2.8409308886066249</v>
+      </c>
+      <c r="X19" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>12.066498289066327</v>
+      </c>
+      <c r="Y19" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>1.9876023297635341</v>
+      </c>
+      <c r="Z19" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.7271626822157433</v>
+      </c>
+      <c r="AA19">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.194864361151378</v>
-      </c>
-      <c r="Y19">
+        <v>9.5020737804336886</v>
+      </c>
+      <c r="AB19">
         <f t="shared" si="3"/>
-        <v>17.194864361151378</v>
-      </c>
+        <v>12.502073780433689</v>
+      </c>
+      <c r="AC19" s="2"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -4321,12 +4644,12 @@
         <v>8.7784956268221563</v>
       </c>
       <c r="I20" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.5753469387755101</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.69946938775510203</v>
       </c>
       <c r="J20" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.5753469387755101</v>
+        <v>0.69946938775510203</v>
       </c>
       <c r="K20" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4334,7 +4657,7 @@
       </c>
       <c r="L20" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>39.383673469387752</v>
+        <v>38.675918367346938</v>
       </c>
       <c r="M20" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4349,12 +4672,12 @@
         <v>8.3485714285714288</v>
       </c>
       <c r="P20" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>775.87755102040808</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>530.99428571428575</v>
       </c>
       <c r="Q20" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>580.13877551020403</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>405.42437317784254</v>
       </c>
       <c r="R20" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4366,26 +4689,39 @@
       </c>
       <c r="U20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7644262271010198</v>
+        <v>1.2556166088922824</v>
       </c>
       <c r="V20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.3597434921245646</v>
+        <v>1.6445119940465125</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" si="2"/>
-        <v>4.1241697192255842</v>
-      </c>
-      <c r="X20">
+        <v>2.9001286029387949</v>
+      </c>
+      <c r="X20" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>13.084226820922284</v>
+      </c>
+      <c r="Y20" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.1552433099820165</v>
+      </c>
+      <c r="Z20" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>1.8728373177842566</v>
+      </c>
+      <c r="AA20">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.302072851680418</v>
-      </c>
-      <c r="Y20">
+        <v>9.9948653077652878</v>
+      </c>
+      <c r="AB20">
         <f t="shared" si="3"/>
-        <v>17.302072851680418</v>
-      </c>
+        <v>12.994865307765288</v>
+      </c>
+      <c r="AC20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -4415,12 +4751,12 @@
         <v>9.3336676384839645</v>
       </c>
       <c r="I21" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.6238367346938773</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.72236734693877547</v>
       </c>
       <c r="J21" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.6238367346938773</v>
+        <v>0.72236734693877547</v>
       </c>
       <c r="K21" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4428,7 +4764,7 @@
       </c>
       <c r="L21" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>40.595918367346933</v>
+        <v>39.968979591836728</v>
       </c>
       <c r="M21" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4443,12 +4779,12 @@
         <v>8.5371428571428574</v>
       </c>
       <c r="P21" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>801.46938775510193</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>572.84571428571428</v>
       </c>
       <c r="Q21" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>599.53469387755092</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>436.17236151603493</v>
       </c>
       <c r="R21" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4460,26 +4796,39 @@
       </c>
       <c r="U21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7298936344614331</v>
+        <v>1.2782698130457373</v>
       </c>
       <c r="V21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.3125547299459921</v>
+        <v>1.6788119759787488</v>
       </c>
       <c r="W21" s="2">
         <f t="shared" si="2"/>
-        <v>4.0424483644074254</v>
-      </c>
-      <c r="X21">
+        <v>2.9570817890244863</v>
+      </c>
+      <c r="X21" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>14.098631253055249</v>
+      </c>
+      <c r="Y21" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.3223367420887349</v>
+      </c>
+      <c r="Z21" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.0180361516034986</v>
+      </c>
+      <c r="AA21">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.397765144089393</v>
-      </c>
-      <c r="Y21">
+        <v>10.474635225586018</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="3"/>
-        <v>17.397765144089391</v>
-      </c>
+        <v>13.474635225586018</v>
+      </c>
+      <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -4509,12 +4858,12 @@
         <v>9.8833819241982503</v>
       </c>
       <c r="I22" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.6693877551020408</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.7438775510204082</v>
       </c>
       <c r="J22" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.6693877551020408</v>
+        <v>0.7438775510204082</v>
       </c>
       <c r="K22" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4522,7 +4871,7 @@
       </c>
       <c r="L22" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>41.734693877551024</v>
+        <v>41.183673469387756</v>
       </c>
       <c r="M22" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4537,12 +4886,12 @@
         <v>8.7142857142857153</v>
       </c>
       <c r="P22" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>825.51020408163265</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>614.28571428571422</v>
       </c>
       <c r="Q22" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>617.75510204081638</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>466.61807580174923</v>
       </c>
       <c r="R22" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4554,26 +4903,39 @@
       </c>
       <c r="U22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6985851136318086</v>
+        <v>1.3001835935596027</v>
       </c>
       <c r="V22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.2698304541264172</v>
+        <v>1.7116443808997706</v>
       </c>
       <c r="W22" s="2">
         <f t="shared" si="2"/>
-        <v>3.9684155677582256</v>
-      </c>
-      <c r="X22">
+        <v>3.011827974459373</v>
+      </c>
+      <c r="X22" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>15.103063386019237</v>
+      </c>
+      <c r="Y22" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.4877875298601602</v>
+      </c>
+      <c r="Z22" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.1618075801749268</v>
+      </c>
+      <c r="AA22">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.483253588516748</v>
-      </c>
-      <c r="Y22">
+        <v>10.93984962406015</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="3"/>
-        <v>17.483253588516746</v>
-      </c>
+        <v>13.93984962406015</v>
+      </c>
+      <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -4603,12 +4965,12 @@
         <v>10.423999999999999</v>
       </c>
       <c r="I23" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.712</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.76400000000000001</v>
       </c>
       <c r="J23" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.712</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="K23" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4616,7 +4978,7 @@
       </c>
       <c r="L23" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>42.8</v>
+        <v>42.32</v>
       </c>
       <c r="M23" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4631,12 +4993,12 @@
         <v>8.879999999999999</v>
       </c>
       <c r="P23" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>848</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>655.04</v>
       </c>
       <c r="Q23" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>634.79999999999995</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>496.56</v>
       </c>
       <c r="R23" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4648,26 +5010,39 @@
       </c>
       <c r="U23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.670245011366507</v>
+        <v>1.3213355132069691</v>
       </c>
       <c r="V23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.2312031657826057</v>
+        <v>1.7430473952213084</v>
       </c>
       <c r="W23" s="2">
         <f t="shared" si="2"/>
-        <v>3.9014481771491125</v>
-      </c>
-      <c r="X23">
+        <v>3.0643829084282777</v>
+      </c>
+      <c r="X23" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.090875020368269</v>
+      </c>
+      <c r="Y23" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.6505005770727648</v>
+      </c>
+      <c r="Z23" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.3031999999999999</v>
+      </c>
+      <c r="AA23">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.559633027522935</v>
-      </c>
-      <c r="Y23">
+        <v>11.388990825688072</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="3"/>
-        <v>17.559633027522935</v>
-      </c>
+        <v>14.388990825688072</v>
+      </c>
+      <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -4697,12 +5072,12 @@
         <v>10.951883381924198</v>
       </c>
       <c r="I24" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.7516734693877551</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.78273469387755101</v>
       </c>
       <c r="J24" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.7516734693877551</v>
+        <v>0.78273469387755101</v>
       </c>
       <c r="K24" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4710,7 +5085,7 @@
       </c>
       <c r="L24" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>43.791836734693881</v>
+        <v>43.377959183673468</v>
       </c>
       <c r="M24" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4725,12 +5100,12 @@
         <v>9.0342857142857156</v>
       </c>
       <c r="P24" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>868.9387755102041</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>694.83428571428567</v>
       </c>
       <c r="Q24" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>650.66938775510209</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>525.79661807580169</v>
       </c>
       <c r="R24" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4742,26 +5117,39 @@
       </c>
       <c r="U24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6446496337313452</v>
+        <v>1.3416982440122429</v>
       </c>
       <c r="V24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.1963532721408789</v>
+        <v>1.7730390591594845</v>
       </c>
       <c r="W24" s="2">
         <f t="shared" si="2"/>
-        <v>3.8410029058722239</v>
-      </c>
-      <c r="X24">
+        <v>3.1147373031717276</v>
+      </c>
+      <c r="X24" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>17.055417956656356</v>
+      </c>
+      <c r="Y24" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.8093807875030192</v>
+      </c>
+      <c r="Z24" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.4412618075801746</v>
+      </c>
+      <c r="AA24">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.627821618645624</v>
-      </c>
-      <c r="Y24">
+        <v>11.82053325642975</v>
+      </c>
+      <c r="AB24">
         <f t="shared" si="3"/>
-        <v>17.627821618645626</v>
-      </c>
+        <v>14.82053325642975</v>
+      </c>
+      <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -4791,12 +5179,12 @@
         <v>11.46339358600583</v>
       </c>
       <c r="I25" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.7884081632653062</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.80008163265306131</v>
       </c>
       <c r="J25" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.7884081632653062</v>
+        <v>0.80008163265306131</v>
       </c>
       <c r="K25" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4804,7 +5192,7 @@
       </c>
       <c r="L25" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>44.710204081632654</v>
+        <v>44.357551020408167</v>
       </c>
       <c r="M25" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4819,12 +5207,12 @@
         <v>9.1771428571428579</v>
       </c>
       <c r="P25" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>888.32653061224494</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>733.39428571428573</v>
       </c>
       <c r="Q25" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>665.36326530612246</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>554.12641399416907</v>
       </c>
       <c r="R25" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4836,26 +5224,39 @@
       </c>
       <c r="U25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6216035084791351</v>
+        <v>1.3612371702108845</v>
       </c>
       <c r="V25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.1650029297201407</v>
+        <v>1.8016169901351289</v>
       </c>
       <c r="W25" s="2">
         <f t="shared" si="2"/>
-        <v>3.7866064381992759</v>
-      </c>
-      <c r="X25">
+        <v>3.1628541603460132</v>
+      </c>
+      <c r="X25" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>17.990043995437521</v>
+      </c>
+      <c r="Y25" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>2.9633330649273959</v>
+      </c>
+      <c r="Z25" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.5750413994169099</v>
+      </c>
+      <c r="AA25">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.688592539196252</v>
-      </c>
-      <c r="Y25">
+        <v>12.232922276858121</v>
+      </c>
+      <c r="AB25">
         <f t="shared" si="3"/>
-        <v>17.68859253919625</v>
-      </c>
+        <v>15.232922276858121</v>
+      </c>
+      <c r="AC25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -4885,12 +5286,12 @@
         <v>11.954892128279884</v>
       </c>
       <c r="I26" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.822204081632653</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.81604081632653069</v>
       </c>
       <c r="J26" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.822204081632653</v>
+        <v>0.81604081632653069</v>
       </c>
       <c r="K26" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4898,7 +5299,7 @@
       </c>
       <c r="L26" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>45.55510204081633</v>
+        <v>45.258775510204082</v>
       </c>
       <c r="M26" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4913,12 +5314,12 @@
         <v>9.3085714285714296</v>
       </c>
       <c r="P26" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>906.16326530612253</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>770.4457142857143</v>
       </c>
       <c r="Q26" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>678.88163265306127</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>581.3478717201167</v>
       </c>
       <c r="R26" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4930,26 +5331,39 @@
       </c>
       <c r="U26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6009361062750898</v>
+        <v>1.3799083780285579</v>
       </c>
       <c r="V26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.1369107953905746</v>
+        <v>1.8287578705902487</v>
       </c>
       <c r="W26" s="2">
         <f t="shared" si="2"/>
-        <v>3.7378469016656641</v>
-      </c>
-      <c r="X26">
+        <v>3.2086662486188064</v>
+      </c>
+      <c r="X26" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>18.88810493726578</v>
+      </c>
+      <c r="Y26" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.1112623131223662</v>
+      </c>
+      <c r="Z26" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.703587172011662</v>
+      </c>
+      <c r="AA26">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.742598829994684</v>
-      </c>
-      <c r="Y26">
+        <v>12.624554916808066</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="3"/>
-        <v>17.742598829994684</v>
-      </c>
+        <v>15.624554916808066</v>
+      </c>
+      <c r="AC26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -4979,12 +5393,12 @@
         <v>12.422740524781341</v>
       </c>
       <c r="I27" s="5">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.8530612244897959</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.83061224489795926</v>
       </c>
       <c r="J27" s="5">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.8530612244897959</v>
+        <v>0.83061224489795926</v>
       </c>
       <c r="K27" s="5">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4992,7 +5406,7 @@
       </c>
       <c r="L27" s="5">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>46.326530612244902</v>
+        <v>46.081632653061227</v>
       </c>
       <c r="M27" s="5">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5007,12 +5421,12 @@
         <v>9.4285714285714288</v>
       </c>
       <c r="P27" s="5">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>922.44897959183675</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>805.71428571428567</v>
       </c>
       <c r="Q27" s="5">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>691.22448979591843</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>607.25947521865885</v>
       </c>
       <c r="R27" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5024,26 +5438,39 @@
       </c>
       <c r="U27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5824989987985583</v>
+        <v>1.3976568161687735</v>
       </c>
       <c r="V27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.1118675744226403</v>
+        <v>1.8544166196956275</v>
       </c>
       <c r="W27" s="12">
         <f t="shared" si="2"/>
-        <v>3.6943665732211985</v>
-      </c>
-      <c r="X27" s="1">
+        <v>3.2520734358644008</v>
+      </c>
+      <c r="X27" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>19.742952582695139</v>
+      </c>
+      <c r="Y27" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.2520734358644008</v>
+      </c>
+      <c r="Z27" s="12">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.8259475218658894</v>
+      </c>
+      <c r="AA27" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.790393013100436</v>
-      </c>
-      <c r="Y27" s="1">
+        <v>12.993761696818463</v>
+      </c>
+      <c r="AB27" s="13">
         <f t="shared" si="3"/>
-        <v>17.790393013100434</v>
-      </c>
+        <v>15.993761696818463</v>
+      </c>
+      <c r="AC27" s="12"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -5073,12 +5500,12 @@
         <v>12.86330029154519</v>
       </c>
       <c r="I28" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.8809795918367347</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.84379591836734691</v>
       </c>
       <c r="J28" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.8809795918367347</v>
+        <v>0.84379591836734691</v>
       </c>
       <c r="K28" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5086,7 +5513,7 @@
       </c>
       <c r="L28" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>47.024489795918363</v>
+        <v>46.826122448979589</v>
       </c>
       <c r="M28" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5101,12 +5528,12 @@
         <v>9.5371428571428574</v>
       </c>
       <c r="P28" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>937.18367346938771</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>838.92571428571432</v>
       </c>
       <c r="Q28" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>702.39183673469381</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>631.65970845481047</v>
       </c>
       <c r="R28" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5118,26 +5545,39 @@
       </c>
       <c r="U28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5661634166987848</v>
+        <v>1.4144144712517011</v>
       </c>
       <c r="V28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0896922591507034</v>
+        <v>1.8785251848555637</v>
       </c>
       <c r="W28" s="2">
         <f t="shared" si="2"/>
-        <v>3.6558556758494882</v>
-      </c>
-      <c r="X28">
+        <v>3.292939656107265</v>
+      </c>
+      <c r="X28" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>20.547938732279629</v>
+      </c>
+      <c r="Y28" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.3846713369299728</v>
+      </c>
+      <c r="Z28" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>2.9411708454810492</v>
+      </c>
+      <c r="AA28">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.832442682296154</v>
-      </c>
-      <c r="Y28">
+        <v>13.338788878764744</v>
+      </c>
+      <c r="AB28">
         <f t="shared" si="3"/>
-        <v>17.832442682296154</v>
-      </c>
+        <v>16.338788878764746</v>
+      </c>
+      <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -5167,12 +5607,12 @@
         <v>13.272932944606413</v>
       </c>
       <c r="I29" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9059591836734695</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.85559183673469397</v>
       </c>
       <c r="J29" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9059591836734695</v>
+        <v>0.85559183673469397</v>
       </c>
       <c r="K29" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5180,7 +5620,7 @@
       </c>
       <c r="L29" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>47.648979591836735</v>
+        <v>47.492244897959182</v>
       </c>
       <c r="M29" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5195,12 +5635,12 @@
         <v>9.6342857142857135</v>
       </c>
       <c r="P29" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>950.36734693877554</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>869.80571428571432</v>
       </c>
       <c r="Q29" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>712.38367346938776</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>654.34705539358606</v>
       </c>
       <c r="R29" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5212,26 +5652,39 @@
       </c>
       <c r="U29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5518181657447248</v>
+        <v>1.4300984376210013</v>
       </c>
       <c r="V29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0702289623339962</v>
+        <v>1.9009908928001755</v>
       </c>
       <c r="W29" s="2">
         <f t="shared" si="2"/>
-        <v>3.6220471280787212</v>
-      </c>
-      <c r="X29">
+        <v>3.3310893304211771</v>
+      </c>
+      <c r="X29" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>21.296415186573263</v>
+      </c>
+      <c r="Y29" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.5079609200955524</v>
+      </c>
+      <c r="Z29" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.0483055393586005</v>
+      </c>
+      <c r="AA29">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.86914295450673</v>
-      </c>
-      <c r="Y29">
+        <v>13.657780590511891</v>
+      </c>
+      <c r="AB29">
         <f t="shared" si="3"/>
-        <v>17.869142954506728</v>
-      </c>
+        <v>16.657780590511891</v>
+      </c>
+      <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -5261,12 +5714,12 @@
         <v>13.648000000000001</v>
       </c>
       <c r="I30" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9279999999999999</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.86599999999999999</v>
       </c>
       <c r="J30" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9279999999999999</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="K30" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5274,7 +5727,7 @@
       </c>
       <c r="L30" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>48.199999999999996</v>
+        <v>48.08</v>
       </c>
       <c r="M30" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5289,12 +5742,12 @@
         <v>9.7199999999999989</v>
       </c>
       <c r="P30" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>962</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>898.08000000000015</v>
       </c>
       <c r="Q30" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>721.19999999999993</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>675.12000000000012</v>
       </c>
       <c r="R30" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5306,26 +5759,39 @@
       </c>
       <c r="U30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5393678602530609</v>
+        <v>1.4446087796060068</v>
       </c>
       <c r="V30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0533442617352256</v>
+        <v>1.9216942955157048</v>
       </c>
       <c r="W30" s="2">
         <f t="shared" si="2"/>
-        <v>3.5927121219882867</v>
-      </c>
-      <c r="X30">
+        <v>3.3663030751217118</v>
+      </c>
+      <c r="X30" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>21.98173374613005</v>
+      </c>
+      <c r="Y30" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.6208470891376123</v>
+      </c>
+      <c r="Z30" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.1464000000000008</v>
+      </c>
+      <c r="AA30">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.900826446280991</v>
-      </c>
-      <c r="Y30">
+        <v>13.948760330578516</v>
+      </c>
+      <c r="AB30">
         <f t="shared" si="3"/>
-        <v>17.900826446280991</v>
-      </c>
+        <v>16.948760330578516</v>
+      </c>
+      <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -5355,12 +5821,12 @@
         <v>13.984862973760933</v>
       </c>
       <c r="I31" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9471020408163264</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.87502040816326532</v>
       </c>
       <c r="J31" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9471020408163264</v>
+        <v>0.87502040816326532</v>
       </c>
       <c r="K31" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5368,7 +5834,7 @@
       </c>
       <c r="L31" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>48.67755102040816</v>
+        <v>48.589387755102038</v>
       </c>
       <c r="M31" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5383,12 +5849,12 @@
         <v>9.7942857142857136</v>
       </c>
       <c r="P31" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>972.08163265306121</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>923.47428571428577</v>
       </c>
       <c r="Q31" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>728.84081632653056</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>693.77702623906714</v>
       </c>
       <c r="R31" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5400,26 +5866,39 @@
       </c>
       <c r="U31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5287314362332791</v>
+        <v>1.4578260915421213</v>
       </c>
       <c r="V31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0389249848981206</v>
+        <v>1.940486435361731</v>
       </c>
       <c r="W31" s="2">
         <f t="shared" si="2"/>
-        <v>3.5676564211313995</v>
-      </c>
-      <c r="X31">
+        <v>3.3983125269038523</v>
+      </c>
+      <c r="X31" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>22.597246211504007</v>
+      </c>
+      <c r="Y31" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.7222347478326223</v>
+      </c>
+      <c r="Z31" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.2345026239067058</v>
+      </c>
+      <c r="AA31">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.927771275706402</v>
-      </c>
-      <c r="Y31">
+        <v>14.209611388444362</v>
+      </c>
+      <c r="AB31">
         <f t="shared" si="3"/>
-        <v>17.927771275706402</v>
-      </c>
+        <v>17.209611388444362</v>
+      </c>
+      <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -5449,12 +5928,12 @@
         <v>14.279883381924199</v>
       </c>
       <c r="I32" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.963265306122449</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.88265306122448983</v>
       </c>
       <c r="J32" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.963265306122449</v>
+        <v>0.88265306122448983</v>
       </c>
       <c r="K32" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5462,7 +5941,7 @@
       </c>
       <c r="L32" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.08163265306122</v>
+        <v>49.020408163265301</v>
       </c>
       <c r="M32" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5477,12 +5956,12 @@
         <v>9.8571428571428577</v>
       </c>
       <c r="P32" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>980.61224489795916</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>945.71428571428578</v>
       </c>
       <c r="Q32" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>735.30612244897952</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>710.11661807580174</v>
       </c>
       <c r="R32" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5494,26 +5973,39 @@
       </c>
       <c r="U32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5198409111452589</v>
+        <v>1.469608659450458</v>
       </c>
       <c r="V32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0268763747024616</v>
+        <v>1.9571854372563928</v>
       </c>
       <c r="W32" s="2">
         <f t="shared" si="2"/>
-        <v>3.5467172858477207</v>
-      </c>
-      <c r="X32">
+        <v>3.4267940967068506</v>
+      </c>
+      <c r="X32" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>23.136304383249161</v>
+      </c>
+      <c r="Y32" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.8110287999570547</v>
+      </c>
+      <c r="Z32" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.3116618075801751</v>
+      </c>
+      <c r="AA32">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.950207468879666</v>
-      </c>
-      <c r="Y32">
+        <v>14.438055720213397</v>
+      </c>
+      <c r="AB32">
         <f t="shared" si="3"/>
-        <v>17.950207468879668</v>
-      </c>
+        <v>17.438055720213399</v>
+      </c>
+      <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -5543,12 +6035,12 @@
         <v>14.529422740524781</v>
       </c>
       <c r="I33" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9764897959183672</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.88889795918367343</v>
       </c>
       <c r="J33" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9764897959183672</v>
+        <v>0.88889795918367343</v>
       </c>
       <c r="K33" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5556,7 +6048,7 @@
       </c>
       <c r="L33" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.412244897959184</v>
+        <v>49.373061224489796</v>
       </c>
       <c r="M33" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5571,12 +6063,12 @@
         <v>9.9085714285714275</v>
       </c>
       <c r="P33" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>987.59183673469386</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>964.52571428571434</v>
       </c>
       <c r="Q33" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>740.59591836734694</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>723.93725947521864</v>
       </c>
       <c r="R33" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5588,26 +6080,39 @@
       </c>
       <c r="U33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5126403619241111</v>
+        <v>1.4797891196774609</v>
       </c>
       <c r="V33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0171205866823074</v>
+        <v>1.9715723137164893</v>
       </c>
       <c r="W33" s="2">
         <f t="shared" si="2"/>
-        <v>3.5297609486064188</v>
-      </c>
-      <c r="X33">
+        <v>3.4513614333939504</v>
+      </c>
+      <c r="X33" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>23.592260061919522</v>
+      </c>
+      <c r="Y33" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.8861341492873822</v>
+      </c>
+      <c r="Z33" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.3769259475218658</v>
+      </c>
+      <c r="AA33">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.968322059066161</v>
-      </c>
-      <c r="Y33">
+        <v>14.631630801140782</v>
+      </c>
+      <c r="AB33">
         <f t="shared" si="3"/>
-        <v>17.968322059066161</v>
-      </c>
+        <v>17.63163080114078</v>
+      </c>
+      <c r="AC33" s="2"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -5637,12 +6142,12 @@
         <v>14.729842565597666</v>
       </c>
       <c r="I34" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9867755102040816</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.89375510204081632</v>
       </c>
       <c r="J34" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9867755102040816</v>
+        <v>0.89375510204081632</v>
       </c>
       <c r="K34" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5650,7 +6155,7 @@
       </c>
       <c r="L34" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.669387755102044</v>
+        <v>49.647346938775513</v>
       </c>
       <c r="M34" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5665,12 +6170,12 @@
         <v>9.9485714285714284</v>
       </c>
       <c r="P34" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>993.0204081632653</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>979.63428571428562</v>
       </c>
       <c r="Q34" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>744.7102040816327</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>735.03743440233234</v>
       </c>
       <c r="R34" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5682,26 +6187,39 @@
       </c>
       <c r="U34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.507085097588627</v>
+        <v>1.48817049443232</v>
       </c>
       <c r="V34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0095954782703425</v>
+        <v>1.9833858400962756</v>
       </c>
       <c r="W34" s="2">
         <f t="shared" si="2"/>
-        <v>3.5166805758589694</v>
-      </c>
-      <c r="X34">
+        <v>3.4715563345285956</v>
+      </c>
+      <c r="X34" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>23.958465048069105</v>
+      </c>
+      <c r="Y34" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.946455699600075</v>
+      </c>
+      <c r="Z34" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.4293434402332359</v>
+      </c>
+      <c r="AA34">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.982263097388735</v>
-      </c>
-      <c r="Y34">
+        <v>14.787663937310841</v>
+      </c>
+      <c r="AB34">
         <f t="shared" si="3"/>
-        <v>17.982263097388735</v>
-      </c>
+        <v>17.787663937310839</v>
+      </c>
+      <c r="AC34" s="2"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -5731,12 +6249,12 @@
         <v>14.877504373177842</v>
       </c>
       <c r="I35" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9941224489795917</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.8972244897959184</v>
       </c>
       <c r="J35" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.9941224489795917</v>
+        <v>0.8972244897959184</v>
       </c>
       <c r="K35" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5744,7 +6262,7 @@
       </c>
       <c r="L35" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.853061224489792</v>
+        <v>49.843265306122447</v>
       </c>
       <c r="M35" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5759,12 +6277,12 @@
         <v>9.9771428571428569</v>
       </c>
       <c r="P35" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>996.89795918367338</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>990.76571428571435</v>
       </c>
       <c r="Q35" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>747.64897959183668</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>743.21562682215745</v>
       </c>
       <c r="R35" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5776,26 +6294,39 @@
       </c>
       <c r="U35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5031410071367599</v>
+        <v>1.4945214617074702</v>
       </c>
       <c r="V35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0042536581779196</v>
+        <v>1.9923163212474411</v>
       </c>
       <c r="W35" s="2">
         <f t="shared" si="2"/>
-        <v>3.5073946653146795</v>
-      </c>
-      <c r="X35">
+        <v>3.4868377829549111</v>
+      </c>
+      <c r="X35" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>24.228271142251934</v>
+      </c>
+      <c r="Y35" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>3.9908983546716055</v>
+      </c>
+      <c r="Z35" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.4679626822157434</v>
+      </c>
+      <c r="AA35">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.992142740219348</v>
-      </c>
-      <c r="Y35">
+        <v>14.903243458129692</v>
+      </c>
+      <c r="AB35">
         <f t="shared" si="3"/>
-        <v>17.99214274021935</v>
-      </c>
+        <v>17.903243458129694</v>
+      </c>
+      <c r="AC35" s="2"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -5825,12 +6356,12 @@
         <v>14.968769679300292</v>
       </c>
       <c r="I36" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.998530612244898</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.89930612244897956</v>
       </c>
       <c r="J36" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>1.998530612244898</v>
+        <v>0.89930612244897956</v>
       </c>
       <c r="K36" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5838,7 +6369,7 @@
       </c>
       <c r="L36" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.963265306122452</v>
+        <v>49.960816326530612</v>
       </c>
       <c r="M36" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5853,12 +6384,12 @@
         <v>9.9942857142857147</v>
       </c>
       <c r="P36" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>999.22448979591832</v>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>997.64571428571435</v>
       </c>
       <c r="Q36" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>749.41224489795923</v>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
+        <v>748.27032069970846</v>
       </c>
       <c r="R36" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5870,26 +6401,39 @@
       </c>
       <c r="U36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5007840674907584</v>
+        <v>1.4985706865149699</v>
       </c>
       <c r="V36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0010617711970879</v>
+        <v>1.9979980250423997</v>
       </c>
       <c r="W36" s="2">
         <f t="shared" si="2"/>
-        <v>3.5018458386878466</v>
-      </c>
-      <c r="X36">
+        <v>3.4965687115573694</v>
+      </c>
+      <c r="X36" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>24.395030145022016</v>
+      </c>
+      <c r="Y36" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>4.0183670182784441</v>
+      </c>
+      <c r="Z36" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.4918320699708456</v>
+      </c>
+      <c r="AA36">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.998039536023528</v>
-      </c>
-      <c r="Y36">
+        <v>14.975186127383482</v>
+      </c>
+      <c r="AB36">
         <f t="shared" si="3"/>
-        <v>17.998039536023526</v>
-      </c>
+        <v>17.975186127383481</v>
+      </c>
+      <c r="AC36" s="2"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -5919,12 +6463,12 @@
         <v>15</v>
       </c>
       <c r="I37" s="2">
-        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>2</v>
+        <f>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</f>
+        <v>0.9</v>
       </c>
       <c r="J37" s="2">
         <f>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="K37" s="2">
         <f>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5947,11 +6491,11 @@
         <v>10</v>
       </c>
       <c r="P37" s="2">
-        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
+        <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
         <v>1000</v>
       </c>
       <c r="Q37" s="2">
-        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
+        <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
         <v>750</v>
       </c>
       <c r="R37" s="2">
@@ -5974,16 +6518,29 @@
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="X37">
+      <c r="X37" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>24.452093856933374</v>
+      </c>
+      <c r="Y37" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
+        <v>4.0277665941970637</v>
+      </c>
+      <c r="Z37" s="2">
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
+        <v>3.5</v>
+      </c>
+      <c r="AA37">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>15</v>
       </c>
-      <c r="Y37">
+      <c r="AB37">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
+      <c r="AC37" s="2"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G39" s="8" t="s">
         <v>7</v>
       </c>
@@ -5991,16 +6548,16 @@
         <v>2</v>
       </c>
       <c r="I39" s="9">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="J39" s="9">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="K39" s="9">
         <v>0.97</v>
       </c>
       <c r="L39" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M39" s="9">
         <v>0</v>
@@ -6012,7 +6569,7 @@
         <v>3</v>
       </c>
       <c r="P39" s="9">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="Q39" s="9">
         <v>30</v>
@@ -6024,7 +6581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
         <v>8</v>
       </c>
@@ -6032,10 +6589,10 @@
         <v>15</v>
       </c>
       <c r="I40" s="11">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="J40" s="11">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="K40" s="11">
         <v>0.95</v>
@@ -6065,12 +6622,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T43" t="s">
         <v>25</v>
       </c>
@@ -6082,9 +6639,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pumped up the bass (More rumble for hull damage)
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -259,7 +259,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -301,7 +301,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2168,23 +2168,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A1:F37"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Stat Level" dataDxfId="11"/>
-    <tableColumn id="2" name="0-1 Value" dataDxfId="12">
+    <tableColumn id="1" name="Stat Level" dataDxfId="25"/>
+    <tableColumn id="2" name="0-1 Value" dataDxfId="24">
       <calculatedColumnFormula>0 + ((1 - 0) * ((Table1[[#This Row],[Stat Level]] - 1) / (36 - 1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Smooth Stop" dataDxfId="26">
+    <tableColumn id="3" name="Smooth Stop" dataDxfId="23">
       <calculatedColumnFormula>1-((1-B2)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Smooth Start" dataDxfId="25">
+    <tableColumn id="4" name="Smooth Start" dataDxfId="22">
       <calculatedColumnFormula>B2^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Smooth Step" dataDxfId="24">
+    <tableColumn id="5" name="Smooth Step" dataDxfId="21">
       <calculatedColumnFormula>B2*B2*(3 - 2*B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Selected Blend" dataDxfId="23">
+    <tableColumn id="6" name="Selected Blend" dataDxfId="20">
       <calculatedColumnFormula>Table1[[#This Row],[Smooth Stop]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2193,43 +2193,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="H1:S37"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Top Speed" dataDxfId="10">
+    <tableColumn id="1" name="Top Speed" dataDxfId="18">
       <calculatedColumnFormula>H$39 + ((H$40 - H$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Acceleration" dataDxfId="5">
+    <tableColumn id="2" name="Acceleration" dataDxfId="17">
       <calculatedColumnFormula>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Handling" dataDxfId="21">
+    <tableColumn id="3" name="Handling" dataDxfId="16">
       <calculatedColumnFormula>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Braking" dataDxfId="20">
+    <tableColumn id="4" name="Braking" dataDxfId="15">
       <calculatedColumnFormula>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Damage" dataDxfId="19">
+    <tableColumn id="5" name="Damage" dataDxfId="14">
       <calculatedColumnFormula>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Shield Disruption" dataDxfId="18">
+    <tableColumn id="6" name="Shield Disruption" dataDxfId="13">
       <calculatedColumnFormula>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Shot Homing" dataDxfId="17">
+    <tableColumn id="7" name="Shot Homing" dataDxfId="12">
       <calculatedColumnFormula>N$39 + ((N$40 - N$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Rate of Fire" dataDxfId="16">
+    <tableColumn id="8" name="Rate of Fire" dataDxfId="11">
       <calculatedColumnFormula>O$39 + ((O$40 - O$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="HP" dataDxfId="4">
+    <tableColumn id="9" name="HP" dataDxfId="10">
       <calculatedColumnFormula>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Shield Capacity" dataDxfId="3">
+    <tableColumn id="10" name="Shield Capacity" dataDxfId="9">
       <calculatedColumnFormula>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Shield Regen" dataDxfId="15">
+    <tableColumn id="11" name="Shield Regen" dataDxfId="8">
       <calculatedColumnFormula>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Shot Deflection" dataDxfId="14">
+    <tableColumn id="12" name="Shot Deflection" dataDxfId="7">
       <calculatedColumnFormula>S$39 + ((S$40 - S$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2241,22 +2241,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="U1:AC37" totalsRowShown="0">
   <autoFilter ref="U1:AC37"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Time To Pop Shield" dataDxfId="9">
+    <tableColumn id="1" name="Time To Pop Shield" dataDxfId="6">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Time To Deplete HP" dataDxfId="8">
+    <tableColumn id="2" name="Time To Deplete HP" dataDxfId="5">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Time to Kill" dataDxfId="7">
+    <tableColumn id="3" name="Time to Kill" dataDxfId="4">
       <calculatedColumnFormula>U2 + V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Time to Kill Vanilla" dataDxfId="2">
+    <tableColumn id="7" name="Time to Kill Vanilla" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Time to Kill StatMax" dataDxfId="1">
+    <tableColumn id="9" name="Time to Kill StatMax" dataDxfId="2">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="0">
+    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="1">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Time to Regen Shield">
@@ -2265,7 +2265,7 @@
     <tableColumn id="5" name="Time to Regen after Combat">
       <calculatedColumnFormula>AA2 + $U$43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Time to Top Speed" dataDxfId="6"/>
+    <tableColumn id="6" name="Time to Top Speed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2571,7 +2571,7 @@
   <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed death funtionality bugs.
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -2570,8 +2570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,7 +2858,7 @@
       </c>
       <c r="Q3" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>31.729679300291544</v>
+        <v>30.888862973760933</v>
       </c>
       <c r="R3" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="U3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9873763669320765</v>
+        <v>1.9347121568572454</v>
       </c>
       <c r="V3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -2878,27 +2878,27 @@
       </c>
       <c r="W3" s="2">
         <f t="shared" ref="W3:W37" si="2">U3 + V3</f>
-        <v>3.3875285307079821</v>
+        <v>3.3348643206331507</v>
       </c>
       <c r="X3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>0.75569496496659661</v>
+        <v>0.74394655369072893</v>
       </c>
       <c r="Y3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.12447862146710684</v>
+        <v>0.12254341466033228</v>
       </c>
       <c r="Z3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.10816793002915452</v>
+        <v>0.1064862973760933</v>
       </c>
       <c r="AA3">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.589530788997811</v>
+        <v>2.5209098696107355</v>
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AB37" si="3">AA3 + $U$43</f>
-        <v>5.589530788997811</v>
+        <v>5.520909869610735</v>
       </c>
       <c r="AC3" s="2"/>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="Q4" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>36.784373177842568</v>
+        <v>33.486413994169098</v>
       </c>
       <c r="R4" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="U4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3287902618908081</v>
+        <v>1.2096555405733769</v>
       </c>
       <c r="V4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -2985,27 +2985,27 @@
       </c>
       <c r="W4" s="2">
         <f t="shared" si="2"/>
-        <v>2.3848428955095815</v>
+        <v>2.2657081741921505</v>
       </c>
       <c r="X4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>0.92245396773667987</v>
+        <v>0.87637282059638322</v>
       </c>
       <c r="Y4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.15194728507394584</v>
+        <v>0.14435676517164558</v>
       </c>
       <c r="Z4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.13203731778425656</v>
+        <v>0.12544139941690963</v>
       </c>
       <c r="AA4">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.5472502624565938</v>
+        <v>2.3188726479851409</v>
       </c>
       <c r="AB4">
         <f t="shared" si="3"/>
-        <v>5.5472502624565934</v>
+        <v>5.3188726479851409</v>
       </c>
       <c r="AC4" s="2"/>
     </row>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="Q5" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>44.962565597667641</v>
+        <v>37.689096209912535</v>
       </c>
       <c r="R5" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="U5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0974254333412115</v>
+        <v>0.91989796824555337</v>
       </c>
       <c r="V5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3092,27 +3092,27 @@
       </c>
       <c r="W5" s="2">
         <f t="shared" si="2"/>
-        <v>2.0826530533243881</v>
+        <v>1.9051255882287297</v>
       </c>
       <c r="X5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.1922600619195056</v>
+        <v>1.0906306012709801</v>
       </c>
       <c r="Y5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.19638994014547601</v>
+        <v>0.17964946184609604</v>
       </c>
       <c r="Z5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.17065655976676386</v>
+        <v>0.15610962099125364</v>
       </c>
       <c r="AA5">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.7145955079912691</v>
+        <v>2.2754629303668232</v>
       </c>
       <c r="AB5">
         <f t="shared" si="3"/>
-        <v>5.7145955079912696</v>
+        <v>5.2754629303668228</v>
       </c>
       <c r="AC5" s="2"/>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="Q6" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>56.06274052478134</v>
+        <v>43.393352769679296</v>
       </c>
       <c r="R6" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="U6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0073078630937322</v>
+        <v>0.77967050917849545</v>
       </c>
       <c r="V6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3199,27 +3199,27 @@
       </c>
       <c r="W6" s="2">
         <f t="shared" si="2"/>
-        <v>2.0040426583684634</v>
+        <v>1.7764053044532266</v>
       </c>
       <c r="X6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.55846504806909</v>
+        <v>1.3814404432132972</v>
       </c>
       <c r="Y6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.25671149045816888</v>
+        <v>0.22755186944735215</v>
       </c>
       <c r="Z6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.22307405247813411</v>
+        <v>0.19773527696793003</v>
       </c>
       <c r="AA6">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.0108223210371392</v>
+        <v>2.3304189891651528</v>
       </c>
       <c r="AB6">
         <f t="shared" si="3"/>
-        <v>6.0108223210371392</v>
+        <v>5.3304189891651532</v>
       </c>
       <c r="AC6" s="2"/>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="Q7" s="5">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>69.883381924198247</v>
+        <v>50.495626822157433</v>
       </c>
       <c r="R7" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="U7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.97645429362880953</v>
+        <v>0.70555646081147183</v>
       </c>
       <c r="V7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3306,27 +3306,27 @@
       </c>
       <c r="W7" s="12">
         <f t="shared" si="2"/>
-        <v>2.0144207267394507</v>
+        <v>1.7435228939221128</v>
       </c>
       <c r="X7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.0144207267394507</v>
+        <v>1.7435228939221128</v>
       </c>
       <c r="Y7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.33181683978849608</v>
+        <v>0.28719435273908256</v>
       </c>
       <c r="Z7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.28833819241982506</v>
+        <v>0.2495626822157434</v>
       </c>
       <c r="AA7" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.390381895332391</v>
+        <v>2.4497878359264504</v>
       </c>
       <c r="AB7" s="13">
         <f t="shared" si="3"/>
-        <v>6.390381895332391</v>
+        <v>5.4497878359264504</v>
       </c>
       <c r="AC7" s="12"/>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="Q8" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>86.222973760932945</v>
+        <v>58.892361516034981</v>
       </c>
       <c r="R8" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="U8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.97378069384373522</v>
+        <v>0.66511559689634292</v>
       </c>
       <c r="V8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3413,27 +3413,27 @@
       </c>
       <c r="W8" s="2">
         <f t="shared" si="2"/>
-        <v>2.0639179615691665</v>
+        <v>1.7552528646217742</v>
       </c>
       <c r="X8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.5534788984846033</v>
+        <v>2.1715985008962049</v>
       </c>
       <c r="Y8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.42061089191292911</v>
+        <v>0.35770727648495582</v>
       </c>
       <c r="Z8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.36549737609329447</v>
+        <v>0.31083615160349853</v>
       </c>
       <c r="AA8">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.8255394008382049</v>
+        <v>2.6129352718994148</v>
       </c>
       <c r="AB8">
         <f t="shared" si="3"/>
-        <v>6.8255394008382044</v>
+        <v>5.6129352718994152</v>
       </c>
       <c r="AC8" s="2"/>
     </row>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="Q9" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>104.88000000000001</v>
+        <v>68.480000000000018</v>
       </c>
       <c r="R9" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="U9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.98547717842323701</v>
+        <v>0.64345420650670559</v>
       </c>
       <c r="V9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3520,27 +3520,27 @@
       </c>
       <c r="W9" s="2">
         <f t="shared" si="2"/>
-        <v>2.1310662096337731</v>
+        <v>1.7890432377172418</v>
       </c>
       <c r="X9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.1689913638585656</v>
+        <v>2.6603878116343513</v>
       </c>
       <c r="Y9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.52199855060793943</v>
+        <v>0.43822100544864057</v>
       </c>
       <c r="Z9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.45360000000000006</v>
+        <v>0.38080000000000003</v>
       </c>
       <c r="AA9">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>4.2983606557377065</v>
+        <v>2.8065573770491818</v>
       </c>
       <c r="AB9">
         <f t="shared" si="3"/>
-        <v>7.2983606557377065</v>
+        <v>5.8065573770491818</v>
       </c>
       <c r="AC9" s="2"/>
     </row>
@@ -3607,7 +3607,7 @@
       </c>
       <c r="Q10" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>125.65294460641398</v>
+        <v>79.154985422740523</v>
       </c>
       <c r="R10" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="U10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0047532549941964</v>
+        <v>0.63294361705278346</v>
       </c>
       <c r="V10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3627,27 +3627,27 @@
       </c>
       <c r="W10" s="2">
         <f t="shared" si="2"/>
-        <v>2.2057453839542509</v>
+        <v>1.8339357460128376</v>
       </c>
       <c r="X10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.8543099234153519</v>
+        <v>3.2046113736353288</v>
       </c>
       <c r="Y10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.6348847196499986</v>
+        <v>0.52786590439380521</v>
       </c>
       <c r="Z10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.55169446064139938</v>
+        <v>0.45869854227405249</v>
       </c>
       <c r="AA10">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>4.7966611761563458</v>
+        <v>3.0216533855673777</v>
       </c>
       <c r="AB10">
         <f t="shared" si="3"/>
-        <v>7.7966611761563458</v>
+        <v>6.0216533855673777</v>
       </c>
       <c r="AC10" s="2"/>
     </row>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="Q11" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>148.34029154518947</v>
+        <v>90.813760932944604</v>
       </c>
       <c r="R11" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="U11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0280313013644693</v>
+        <v>0.62935961538983765</v>
       </c>
       <c r="V11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3734,27 +3734,27 @@
       </c>
       <c r="W11" s="2">
         <f t="shared" si="2"/>
-        <v>2.2829164822378747</v>
+        <v>1.8842447962632431</v>
       </c>
       <c r="X11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>4.6027863777089806</v>
+        <v>3.7989897343979164</v>
       </c>
       <c r="Y11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.75817430281557807</v>
+        <v>0.62577233808411825</v>
       </c>
       <c r="Z11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.6588291545189503</v>
+        <v>0.54377609329446064</v>
       </c>
       <c r="AA11">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.3118052365640782</v>
+        <v>3.2518812377333277</v>
       </c>
       <c r="AB11">
         <f t="shared" si="3"/>
-        <v>8.3118052365640782</v>
+        <v>6.2518812377333273</v>
       </c>
       <c r="AC11" s="2"/>
     </row>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="Q12" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>172.74052478134112</v>
+        <v>103.35276967930029</v>
       </c>
       <c r="R12" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="U12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0533333333333335</v>
+        <v>0.63022222222222224</v>
       </c>
       <c r="V12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3841,27 +3841,27 @@
       </c>
       <c r="W12" s="2">
         <f t="shared" si="2"/>
-        <v>2.3600000000000003</v>
+        <v>1.9368888888888889</v>
       </c>
       <c r="X12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>5.4077725272934698</v>
+        <v>4.4382434414208927</v>
       </c>
       <c r="Y12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.89077220388114986</v>
+        <v>0.73107067128324876</v>
       </c>
       <c r="Z12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.77405247813411071</v>
+        <v>0.63527696793002919</v>
       </c>
       <c r="AA12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.8374384236453203</v>
+        <v>3.4926108374384235</v>
       </c>
       <c r="AB12">
         <f t="shared" si="3"/>
-        <v>8.8374384236453203</v>
+        <v>6.4926108374384235</v>
       </c>
       <c r="AC12" s="2"/>
     </row>
@@ -3928,7 +3928,7 @@
       </c>
       <c r="Q13" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>198.65212827988339</v>
+        <v>116.66845481049562</v>
       </c>
       <c r="R13" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3940,7 +3940,7 @@
       </c>
       <c r="U13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.079528556901223</v>
+        <v>0.63400744682695642</v>
       </c>
       <c r="V13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -3948,27 +3948,27 @@
       </c>
       <c r="W13" s="2">
         <f t="shared" si="2"/>
-        <v>2.4356729901795617</v>
+        <v>1.9901518801052953</v>
       </c>
       <c r="X13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>6.2626201727228334</v>
+        <v>5.1170930422030345</v>
       </c>
       <c r="Y13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.0315833266231849</v>
+        <v>0.84289126875486475</v>
       </c>
       <c r="Z13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.8964128279883381</v>
+        <v>0.73244548104956264</v>
       </c>
       <c r="AA13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.3687217258010254</v>
+        <v>3.740352189030546</v>
       </c>
       <c r="AB13">
         <f t="shared" si="3"/>
-        <v>9.3687217258010254</v>
+        <v>6.7403521890305456</v>
       </c>
       <c r="AC13" s="2"/>
     </row>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="Q14" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>225.8735860058309</v>
+        <v>130.65725947521867</v>
       </c>
       <c r="R14" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="U14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.1059560211771715</v>
+        <v>0.63974360783998818</v>
       </c>
       <c r="V14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4055,27 +4055,27 @@
       </c>
       <c r="W14" s="2">
         <f t="shared" si="2"/>
-        <v>2.509277768634119</v>
+        <v>2.0430653552969358</v>
       </c>
       <c r="X14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>7.1606811145510889</v>
+        <v>5.830259084243119</v>
       </c>
       <c r="Y14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.1795125748181547</v>
+        <v>0.96036449526263512</v>
       </c>
       <c r="Z14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.0249586005830904</v>
+        <v>0.83452594752186593</v>
       </c>
       <c r="AA14">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.9018494102554975</v>
+        <v>3.9923956811459935</v>
       </c>
       <c r="AB14">
         <f t="shared" si="3"/>
-        <v>9.9018494102554975</v>
+        <v>6.9923956811459931</v>
       </c>
       <c r="AC14" s="2"/>
     </row>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="Q15" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>254.20338192419828</v>
+        <v>145.21562682215745</v>
       </c>
       <c r="R15" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="U15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.1322243467112985</v>
+        <v>0.64679182065334151</v>
       </c>
       <c r="V15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4162,27 +4162,27 @@
       </c>
       <c r="W15" s="2">
         <f t="shared" si="2"/>
-        <v>2.5805156150778168</v>
+        <v>2.0950830890198597</v>
       </c>
       <c r="X15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>8.0953071533322536</v>
+        <v>6.5724621150399276</v>
       </c>
       <c r="Y15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.3334648522425316</v>
+        <v>1.0826207155702283</v>
       </c>
       <c r="Z15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.1587381924198252</v>
+        <v>0.94076268221574355</v>
       </c>
       <c r="AA15">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.4337346110561677</v>
+        <v>4.2465777717150361</v>
       </c>
       <c r="AB15">
         <f t="shared" si="3"/>
-        <v>10.433734611056167</v>
+        <v>7.2465777717150361</v>
       </c>
       <c r="AC15" s="2"/>
     </row>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="Q16" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>283.44000000000005</v>
+        <v>160.24000000000004</v>
       </c>
       <c r="R16" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="U16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.1581004929199956</v>
+        <v>0.65472065687799919</v>
       </c>
       <c r="V16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4269,27 +4269,27 @@
       </c>
       <c r="W16" s="2">
         <f t="shared" si="2"/>
-        <v>2.649281539688559</v>
+        <v>2.1459017036465626</v>
       </c>
       <c r="X16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>9.059850089620344</v>
+        <v>7.3384226820922347</v>
       </c>
       <c r="Y16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.4923450626727868</v>
+        <v>1.2087902944413134</v>
       </c>
       <c r="Z16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.2968000000000004</v>
+        <v>1.0504000000000002</v>
       </c>
       <c r="AA16">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.96179775280899</v>
+        <v>4.5011235955056188</v>
       </c>
       <c r="AB16">
         <f t="shared" si="3"/>
-        <v>10.961797752808991</v>
+        <v>7.5011235955056188</v>
       </c>
       <c r="AC16" s="2"/>
     </row>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="Q17" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>313.38192419825072</v>
+        <v>175.62682215743439</v>
       </c>
       <c r="R17" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4368,7 +4368,7 @@
       </c>
       <c r="U17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.1834456335050862</v>
+        <v>0.66323160258950964</v>
       </c>
       <c r="V17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4376,27 +4376,27 @@
       </c>
       <c r="W17" s="2">
         <f t="shared" si="2"/>
-        <v>2.7155722904831103</v>
+        <v>2.1953582595675334</v>
       </c>
       <c r="X17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>10.047661723969373</v>
+        <v>8.1228613328988146</v>
       </c>
       <c r="Y17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.6550581098853905</v>
+        <v>1.3380035966395574</v>
       </c>
       <c r="Z17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.4381924198250728</v>
+        <v>1.16268221574344</v>
       </c>
       <c r="AA17">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>8.4838200473559588</v>
+        <v>4.7545382794001574</v>
       </c>
       <c r="AB17">
         <f t="shared" si="3"/>
-        <v>11.483820047355959</v>
+        <v>7.7545382794001574</v>
       </c>
       <c r="AC17" s="2"/>
     </row>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="Q18" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>343.82763848396502</v>
+        <v>191.27253644314868</v>
       </c>
       <c r="R18" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="U18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2081770127940334</v>
+        <v>0.67211316323599912</v>
       </c>
       <c r="V18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4483,27 +4483,27 @@
       </c>
       <c r="W18" s="2">
         <f t="shared" si="2"/>
-        <v>2.7794338540253429</v>
+        <v>2.2433700044673088</v>
       </c>
       <c r="X18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>11.052093856933363</v>
+        <v>8.9204986149584542</v>
       </c>
       <c r="Y18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.8205088976568162</v>
+        <v>1.4693909869286308</v>
       </c>
       <c r="Z18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.5819638483965015</v>
+        <v>1.2768536443148688</v>
       </c>
       <c r="AA18">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>8.9978392895291002</v>
+        <v>5.0055299539170512</v>
       </c>
       <c r="AB18">
         <f t="shared" si="3"/>
-        <v>11.9978392895291</v>
+        <v>8.0055299539170512</v>
       </c>
       <c r="AC18" s="2"/>
     </row>
@@ -4570,7 +4570,7 @@
       </c>
       <c r="Q19" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>374.5756268221574</v>
+        <v>207.07358600583089</v>
       </c>
       <c r="R19" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="U19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2322446279270998</v>
+        <v>0.68121173848407879</v>
       </c>
       <c r="V19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4590,27 +4590,27 @@
       </c>
       <c r="W19" s="2">
         <f t="shared" si="2"/>
-        <v>2.8409308886066249</v>
+        <v>2.2898979991636041</v>
       </c>
       <c r="X19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>12.066498289066327</v>
+        <v>9.726055075769926</v>
       </c>
       <c r="Y19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.9876023297635341</v>
+        <v>1.602082830072201</v>
       </c>
       <c r="Z19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.7271626822157433</v>
+        <v>1.3921586005830904</v>
       </c>
       <c r="AA19">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>9.5020737804336886</v>
+        <v>5.2529538798331501</v>
       </c>
       <c r="AB19">
         <f t="shared" si="3"/>
-        <v>12.502073780433689</v>
+        <v>8.2529538798331501</v>
       </c>
       <c r="AC19" s="2"/>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="Q20" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>405.42437317784254</v>
+        <v>222.92641399416908</v>
       </c>
       <c r="R20" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="U20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2556166088922824</v>
+        <v>0.69041263054278912</v>
       </c>
       <c r="V20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4697,27 +4697,27 @@
       </c>
       <c r="W20" s="2">
         <f t="shared" si="2"/>
-        <v>2.9001286029387949</v>
+        <v>2.3349246245893016</v>
       </c>
       <c r="X20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>13.084226820922284</v>
+        <v>10.53425126283201</v>
       </c>
       <c r="Y20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.1552433099820165</v>
+        <v>1.7352094908339373</v>
       </c>
       <c r="Z20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.8728373177842566</v>
+        <v>1.5078413994169098</v>
       </c>
       <c r="AA20">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>9.9948653077652878</v>
+        <v>5.4957709225771207</v>
       </c>
       <c r="AB20">
         <f t="shared" si="3"/>
-        <v>12.994865307765288</v>
+        <v>8.4957709225771207</v>
       </c>
       <c r="AC20" s="2"/>
     </row>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="Q21" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>436.17236151603493</v>
+        <v>238.72746355685129</v>
       </c>
       <c r="R21" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4796,7 +4796,7 @@
       </c>
       <c r="U21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2782698130457373</v>
+        <v>0.69962734261529058</v>
       </c>
       <c r="V21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4804,27 +4804,27 @@
       </c>
       <c r="W21" s="2">
         <f t="shared" si="2"/>
-        <v>2.9570817890244863</v>
+        <v>2.3784393185940393</v>
       </c>
       <c r="X21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>14.098631253055249</v>
+        <v>11.339807723643482</v>
       </c>
       <c r="Y21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.3223367420887349</v>
+        <v>1.8679013339775077</v>
       </c>
       <c r="Z21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.0180361516034986</v>
+        <v>1.6231463556851311</v>
       </c>
       <c r="AA21">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>10.474635225586018</v>
+        <v>5.7330159352507906</v>
       </c>
       <c r="AB21">
         <f t="shared" si="3"/>
-        <v>13.474635225586018</v>
+        <v>8.7330159352507906</v>
       </c>
       <c r="AC21" s="2"/>
     </row>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="Q22" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>466.61807580174923</v>
+        <v>254.37317784256558</v>
       </c>
       <c r="R22" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4903,7 +4903,7 @@
       </c>
       <c r="U22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3001835935596027</v>
+        <v>0.70878487059091111</v>
       </c>
       <c r="V22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -4911,27 +4911,27 @@
       </c>
       <c r="W22" s="2">
         <f t="shared" si="2"/>
-        <v>3.011827974459373</v>
+        <v>2.4204292514906816</v>
       </c>
       <c r="X22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.103063386019237</v>
+        <v>12.137445005703121</v>
       </c>
       <c r="Y22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.4877875298601602</v>
+        <v>1.9992887242665804</v>
       </c>
       <c r="Z22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.1618075801749268</v>
+        <v>1.7373177842565597</v>
       </c>
       <c r="AA22">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>10.93984962406015</v>
+        <v>5.9637730690362263</v>
       </c>
       <c r="AB22">
         <f t="shared" si="3"/>
-        <v>13.93984962406015</v>
+        <v>8.9637730690362254</v>
       </c>
       <c r="AC22" s="2"/>
     </row>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="Q23" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>496.56</v>
+        <v>269.76</v>
       </c>
       <c r="R23" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="U23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3213355132069691</v>
+        <v>0.7178255760486385</v>
       </c>
       <c r="V23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5018,27 +5018,27 @@
       </c>
       <c r="W23" s="2">
         <f t="shared" si="2"/>
-        <v>3.0643829084282777</v>
+        <v>2.4608729712699469</v>
       </c>
       <c r="X23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.090875020368269</v>
+        <v>12.921883656509703</v>
       </c>
       <c r="Y23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.6505005770727648</v>
+        <v>2.1285020264648251</v>
       </c>
       <c r="Z23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.3031999999999999</v>
+        <v>1.8495999999999999</v>
       </c>
       <c r="AA23">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>11.388990825688072</v>
+        <v>6.187155963302752</v>
       </c>
       <c r="AB23">
         <f t="shared" si="3"/>
-        <v>14.388990825688072</v>
+        <v>9.187155963302752</v>
       </c>
       <c r="AC23" s="2"/>
     </row>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="Q24" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>525.79661807580169</v>
+        <v>284.78437317784255</v>
       </c>
       <c r="R24" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="U24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3416982440122429</v>
+        <v>0.72669674980631738</v>
       </c>
       <c r="V24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5125,27 +5125,27 @@
       </c>
       <c r="W24" s="2">
         <f t="shared" si="2"/>
-        <v>3.1147373031717276</v>
+        <v>2.4997358089658017</v>
       </c>
       <c r="X24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>17.055417956656356</v>
+        <v>13.68784422356201</v>
       </c>
       <c r="Y24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.8093807875030192</v>
+        <v>2.2546716053359095</v>
       </c>
       <c r="Z24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.4412618075801746</v>
+        <v>1.9592373177842564</v>
       </c>
       <c r="AA24">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>11.82053325642975</v>
+        <v>6.4022913771858532</v>
       </c>
       <c r="AB24">
         <f t="shared" si="3"/>
-        <v>14.82053325642975</v>
+        <v>9.4022913771858541</v>
       </c>
       <c r="AC24" s="2"/>
     </row>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="Q25" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>554.12641399416907</v>
+        <v>299.34274052478133</v>
       </c>
       <c r="R25" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="U25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3612371702108845</v>
+        <v>0.73534928988137382</v>
       </c>
       <c r="V25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5232,27 +5232,27 @@
       </c>
       <c r="W25" s="2">
         <f t="shared" si="2"/>
-        <v>3.1628541603460132</v>
+        <v>2.5369662800165029</v>
       </c>
       <c r="X25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>17.990043995437521</v>
+        <v>14.430047254358817</v>
       </c>
       <c r="Y25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.9633330649273959</v>
+        <v>2.3769278256435031</v>
       </c>
       <c r="Z25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.5750413994169099</v>
+        <v>2.0654740524781343</v>
       </c>
       <c r="AA25">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.232922276858121</v>
+        <v>6.6083052287413429</v>
       </c>
       <c r="AB25">
         <f t="shared" si="3"/>
-        <v>15.232922276858121</v>
+        <v>9.6083052287413437</v>
       </c>
       <c r="AC25" s="2"/>
     </row>
@@ -5319,7 +5319,7 @@
       </c>
       <c r="Q26" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>581.3478717201167</v>
+        <v>313.33154518950437</v>
       </c>
       <c r="R26" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="U26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3799083780285579</v>
+        <v>0.74373511169537709</v>
       </c>
       <c r="V26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5339,27 +5339,27 @@
       </c>
       <c r="W26" s="2">
         <f t="shared" si="2"/>
-        <v>3.2086662486188064</v>
+        <v>2.5724929822856257</v>
       </c>
       <c r="X26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>18.88810493726578</v>
+        <v>15.143213296398901</v>
       </c>
       <c r="Y26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.1112623131223662</v>
+        <v>2.4944010521512734</v>
       </c>
       <c r="Z26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.703587172011662</v>
+        <v>2.1675545189504373</v>
       </c>
       <c r="AA26">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.624554916808066</v>
+        <v>6.8043102793324381</v>
       </c>
       <c r="AB26">
         <f t="shared" si="3"/>
-        <v>15.624554916808066</v>
+        <v>9.8043102793324373</v>
       </c>
       <c r="AC26" s="2"/>
     </row>
@@ -5426,7 +5426,7 @@
       </c>
       <c r="Q27" s="5">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>607.25947521865885</v>
+        <v>326.64723032069969</v>
       </c>
       <c r="R27" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="U27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3976568161687735</v>
+        <v>0.75180502992726195</v>
       </c>
       <c r="V27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5446,27 +5446,27 @@
       </c>
       <c r="W27" s="12">
         <f t="shared" si="2"/>
-        <v>3.2520734358644008</v>
+        <v>2.6062216496228894</v>
       </c>
       <c r="X27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>19.742952582695139</v>
+        <v>15.822062897181041</v>
       </c>
       <c r="Y27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.2520734358644008</v>
+        <v>2.6062216496228894</v>
       </c>
       <c r="Z27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.8259475218658894</v>
+        <v>2.2647230320699707</v>
       </c>
       <c r="AA27" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>12.993761696818463</v>
+        <v>6.9893948845913902</v>
       </c>
       <c r="AB27" s="13">
         <f t="shared" si="3"/>
-        <v>15.993761696818463</v>
+        <v>9.9893948845913911</v>
       </c>
       <c r="AC27" s="12"/>
     </row>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="Q28" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>631.65970845481047</v>
+        <v>339.1862390670554</v>
       </c>
       <c r="R28" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="U28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4144144712517011</v>
+        <v>0.7595069284369339</v>
       </c>
       <c r="V28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5553,27 +5553,27 @@
       </c>
       <c r="W28" s="2">
         <f t="shared" si="2"/>
-        <v>3.292939656107265</v>
+        <v>2.6380321132924975</v>
       </c>
       <c r="X28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>20.547938732279629</v>
+        <v>16.461316604204022</v>
       </c>
       <c r="Y28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.3846713369299728</v>
+        <v>2.7115199828220202</v>
       </c>
       <c r="Z28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.9411708454810492</v>
+        <v>2.3562239067055395</v>
       </c>
       <c r="AA28">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.338788878764744</v>
+        <v>7.1626123574753118</v>
       </c>
       <c r="AB28">
         <f t="shared" si="3"/>
-        <v>16.338788878764746</v>
+        <v>10.162612357475311</v>
       </c>
       <c r="AC28" s="2"/>
     </row>
@@ -5640,7 +5640,7 @@
       </c>
       <c r="Q29" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>654.34705539358606</v>
+        <v>350.84501457725946</v>
       </c>
       <c r="R29" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="U29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4300984376210013</v>
+        <v>0.76678408355067884</v>
       </c>
       <c r="V29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5660,27 +5660,27 @@
       </c>
       <c r="W29" s="2">
         <f t="shared" si="2"/>
-        <v>3.3310893304211771</v>
+        <v>2.6677749763508545</v>
       </c>
       <c r="X29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>21.296415186573263</v>
+        <v>17.055694964966609</v>
       </c>
       <c r="Y29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.5079609200955524</v>
+        <v>2.8094264165123333</v>
       </c>
       <c r="Z29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.0483055393586005</v>
+        <v>2.4413014577259475</v>
       </c>
       <c r="AA29">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.657780590511891</v>
+        <v>7.3229705717693445</v>
       </c>
       <c r="AB29">
         <f t="shared" si="3"/>
-        <v>16.657780590511891</v>
+        <v>10.322970571769345</v>
       </c>
       <c r="AC29" s="2"/>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="Q30" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>675.12000000000012</v>
+        <v>361.52000000000004</v>
       </c>
       <c r="R30" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="U30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4446087796060068</v>
+        <v>0.77357353656114991</v>
       </c>
       <c r="V30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5767,27 +5767,27 @@
       </c>
       <c r="W30" s="2">
         <f t="shared" si="2"/>
-        <v>3.3663030751217118</v>
+        <v>2.6952678320768548</v>
       </c>
       <c r="X30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>21.98173374613005</v>
+        <v>17.599918526967588</v>
       </c>
       <c r="Y30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.6208470891376123</v>
+        <v>2.8990713154574985</v>
       </c>
       <c r="Z30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.1464000000000008</v>
+        <v>2.5192000000000005</v>
       </c>
       <c r="AA30">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>13.948760330578516</v>
+        <v>7.4694214876033067</v>
       </c>
       <c r="AB30">
         <f t="shared" si="3"/>
-        <v>16.948760330578516</v>
+        <v>10.469421487603306</v>
       </c>
       <c r="AC30" s="2"/>
     </row>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="Q31" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>693.77702623906714</v>
+        <v>371.10763848396505</v>
       </c>
       <c r="R31" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="U31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4578260915421213</v>
+        <v>0.77980442950856621</v>
       </c>
       <c r="V31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5874,27 +5874,27 @@
       </c>
       <c r="W31" s="2">
         <f t="shared" si="2"/>
-        <v>3.3983125269038523</v>
+        <v>2.7202908648702975</v>
       </c>
       <c r="X31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>22.597246211504007</v>
+        <v>18.088707837705734</v>
       </c>
       <c r="Y31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.7222347478326223</v>
+        <v>2.9795850444211829</v>
       </c>
       <c r="Z31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.2345026239067058</v>
+        <v>2.5891638483965016</v>
       </c>
       <c r="AA31">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.209611388444362</v>
+        <v>7.6008503117013406</v>
       </c>
       <c r="AB31">
         <f t="shared" si="3"/>
-        <v>17.209611388444362</v>
+        <v>10.60085031170134</v>
       </c>
       <c r="AC31" s="2"/>
     </row>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="Q32" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>710.11661807580174</v>
+        <v>379.50437317784258</v>
       </c>
       <c r="R32" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="U32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.469608659450458</v>
+        <v>0.78539622778119689</v>
       </c>
       <c r="V32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -5981,27 +5981,27 @@
       </c>
       <c r="W32" s="2">
         <f t="shared" si="2"/>
-        <v>3.4267940967068506</v>
+        <v>2.7425816650375898</v>
       </c>
       <c r="X32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>23.136304383249161</v>
+        <v>18.516783444679824</v>
       </c>
       <c r="Y32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.8110287999570547</v>
+        <v>3.0500979681670559</v>
       </c>
       <c r="Z32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.3116618075801751</v>
+        <v>2.6504373177842568</v>
       </c>
       <c r="AA32">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.438055720213397</v>
+        <v>7.7160640189685834</v>
       </c>
       <c r="AB32">
         <f t="shared" si="3"/>
-        <v>17.438055720213399</v>
+        <v>10.716064018968584</v>
       </c>
       <c r="AC32" s="2"/>
     </row>
@@ -6068,7 +6068,7 @@
       </c>
       <c r="Q33" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>723.93725947521864</v>
+        <v>386.60664723032073</v>
       </c>
       <c r="R33" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="U33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4797891196774609</v>
+        <v>0.79025675592540023</v>
       </c>
       <c r="V33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6088,27 +6088,27 @@
       </c>
       <c r="W33" s="2">
         <f t="shared" si="2"/>
-        <v>3.4513614333939504</v>
+        <v>2.7618290696418897</v>
       </c>
       <c r="X33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>23.592260061919522</v>
+        <v>18.878865895388643</v>
       </c>
       <c r="Y33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.8861341492873822</v>
+        <v>3.1097404514587863</v>
       </c>
       <c r="Z33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.3769259475218658</v>
+        <v>2.7022647230320702</v>
       </c>
       <c r="AA33">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.631630801140782</v>
+        <v>7.8137789615103594</v>
       </c>
       <c r="AB33">
         <f t="shared" si="3"/>
-        <v>17.63163080114078</v>
+        <v>10.813778961510359</v>
       </c>
       <c r="AC33" s="2"/>
     </row>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="Q34" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>735.03743440233234</v>
+        <v>392.31090379008742</v>
       </c>
       <c r="R34" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="U34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.48817049443232</v>
+        <v>0.79427997043334286</v>
       </c>
       <c r="V34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6195,27 +6195,27 @@
       </c>
       <c r="W34" s="2">
         <f t="shared" si="2"/>
-        <v>3.4715563345285956</v>
+        <v>2.7776658105296184</v>
       </c>
       <c r="X34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>23.958465048069105</v>
+        <v>19.169675737330955</v>
       </c>
       <c r="Y34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.946455699600075</v>
+        <v>3.1576428590600418</v>
       </c>
       <c r="Z34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.4293434402332359</v>
+        <v>2.7438903790087461</v>
       </c>
       <c r="AA34">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.787663937310841</v>
+        <v>7.8926072777608329</v>
       </c>
       <c r="AB34">
         <f t="shared" si="3"/>
-        <v>17.787663937310839</v>
+        <v>10.892607277760833</v>
       </c>
       <c r="AC34" s="2"/>
     </row>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="Q35" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>743.21562682215745</v>
+        <v>396.51358600583092</v>
       </c>
       <c r="R35" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="U35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4945214617074702</v>
+        <v>0.79734338563108109</v>
       </c>
       <c r="V35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6302,27 +6302,27 @@
       </c>
       <c r="W35" s="2">
         <f t="shared" si="2"/>
-        <v>3.4868377829549111</v>
+        <v>2.7896597068785223</v>
       </c>
       <c r="X35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>24.228271142251934</v>
+        <v>19.383933518005556</v>
       </c>
       <c r="Y35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.9908983546716055</v>
+        <v>3.1929355557344929</v>
       </c>
       <c r="Z35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.4679626822157434</v>
+        <v>2.7745586005830907</v>
       </c>
       <c r="AA35">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.903243458129692</v>
+        <v>7.9510417884619891</v>
       </c>
       <c r="AB35">
         <f t="shared" si="3"/>
-        <v>17.903243458129694</v>
+        <v>10.951041788461989</v>
       </c>
       <c r="AC35" s="2"/>
     </row>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="Q36" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>748.27032069970846</v>
+        <v>399.11113702623908</v>
       </c>
       <c r="R36" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="U36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4985706865149699</v>
+        <v>0.79930505602560964</v>
       </c>
       <c r="V36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6409,27 +6409,27 @@
       </c>
       <c r="W36" s="2">
         <f t="shared" si="2"/>
-        <v>3.4965687115573694</v>
+        <v>2.7973030810680095</v>
       </c>
       <c r="X36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>24.395030145022016</v>
+        <v>19.516359784911209</v>
       </c>
       <c r="Y36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>4.0183670182784441</v>
+        <v>3.2147489062458061</v>
       </c>
       <c r="Z36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.4918320699708456</v>
+        <v>2.793513702623907</v>
       </c>
       <c r="AA36">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>14.975186127383482</v>
+        <v>7.9874390272364471</v>
       </c>
       <c r="AB36">
         <f t="shared" si="3"/>
-        <v>17.975186127383481</v>
+        <v>10.987439027236448</v>
       </c>
       <c r="AC36" s="2"/>
     </row>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="Q37" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="R37" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6508,7 +6508,7 @@
       </c>
       <c r="U37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="V37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6516,27 +6516,27 @@
       </c>
       <c r="W37" s="2">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="X37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>24.452093856933374</v>
+        <v>19.561675085546696</v>
       </c>
       <c r="Y37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>4.0277665941970637</v>
+        <v>3.2222132753576509</v>
       </c>
       <c r="Z37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="AA37">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AB37">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="AC37" s="2"/>
     </row>
@@ -6613,7 +6613,7 @@
         <v>1000</v>
       </c>
       <c r="Q40" s="11">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="R40" s="11">
         <v>50</v>

</xml_diff>

<commit_message>
Added some more content to the paper on the process, added more helpful stat things
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Acceleration</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Time to Kill AbsMax</t>
+  </si>
+  <si>
+    <t>Time for Vanilla to Kill</t>
+  </si>
+  <si>
+    <t>Time for StatMax to Kill</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="29">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -2149,7 +2161,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2168,23 +2186,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0" dataDxfId="28">
   <autoFilter ref="A1:F37"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Stat Level" dataDxfId="25"/>
-    <tableColumn id="2" name="0-1 Value" dataDxfId="24">
+    <tableColumn id="1" name="Stat Level" dataDxfId="27"/>
+    <tableColumn id="2" name="0-1 Value" dataDxfId="26">
       <calculatedColumnFormula>0 + ((1 - 0) * ((Table1[[#This Row],[Stat Level]] - 1) / (36 - 1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Smooth Stop" dataDxfId="23">
+    <tableColumn id="3" name="Smooth Stop" dataDxfId="25">
       <calculatedColumnFormula>1-((1-B2)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Smooth Start" dataDxfId="22">
+    <tableColumn id="4" name="Smooth Start" dataDxfId="24">
       <calculatedColumnFormula>B2^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Smooth Step" dataDxfId="21">
+    <tableColumn id="5" name="Smooth Step" dataDxfId="23">
       <calculatedColumnFormula>B2*B2*(3 - 2*B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Selected Blend" dataDxfId="20">
+    <tableColumn id="6" name="Selected Blend" dataDxfId="22">
       <calculatedColumnFormula>Table1[[#This Row],[Smooth Stop]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2193,43 +2211,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:S37" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="H1:S37"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Top Speed" dataDxfId="18">
+    <tableColumn id="1" name="Top Speed" dataDxfId="20">
       <calculatedColumnFormula>H$39 + ((H$40 - H$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Acceleration" dataDxfId="17">
+    <tableColumn id="2" name="Acceleration" dataDxfId="19">
       <calculatedColumnFormula>I$39 + ((I$40 - I$39) * ((Table1[[#This Row],[Smooth Stop]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Handling" dataDxfId="16">
+    <tableColumn id="3" name="Handling" dataDxfId="18">
       <calculatedColumnFormula>J$39 + ((J$40 - J$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Braking" dataDxfId="15">
+    <tableColumn id="4" name="Braking" dataDxfId="17">
       <calculatedColumnFormula>K$39 + ((K$40 - K$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Damage" dataDxfId="14">
+    <tableColumn id="5" name="Damage" dataDxfId="16">
       <calculatedColumnFormula>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Shield Disruption" dataDxfId="13">
+    <tableColumn id="6" name="Shield Disruption" dataDxfId="15">
       <calculatedColumnFormula>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Shot Homing" dataDxfId="12">
+    <tableColumn id="7" name="Shot Homing" dataDxfId="14">
       <calculatedColumnFormula>N$39 + ((N$40 - N$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Rate of Fire" dataDxfId="11">
+    <tableColumn id="8" name="Rate of Fire" dataDxfId="13">
       <calculatedColumnFormula>O$39 + ((O$40 - O$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="HP" dataDxfId="10">
+    <tableColumn id="9" name="HP" dataDxfId="12">
       <calculatedColumnFormula>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Shield Capacity" dataDxfId="9">
+    <tableColumn id="10" name="Shield Capacity" dataDxfId="11">
       <calculatedColumnFormula>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Shield Regen" dataDxfId="8">
+    <tableColumn id="11" name="Shield Regen" dataDxfId="10">
       <calculatedColumnFormula>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Shot Deflection" dataDxfId="7">
+    <tableColumn id="12" name="Shot Deflection" dataDxfId="9">
       <calculatedColumnFormula>S$39 + ((S$40 - S$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2238,34 +2256,40 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="U1:AC37" totalsRowShown="0">
-  <autoFilter ref="U1:AC37"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Time To Pop Shield" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="U1:AE37" totalsRowShown="0">
+  <autoFilter ref="U1:AE37"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Time To Pop Shield" dataDxfId="8">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Time To Deplete HP" dataDxfId="5">
+    <tableColumn id="2" name="Time To Deplete HP" dataDxfId="7">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Time to Kill" dataDxfId="4">
+    <tableColumn id="3" name="Time to Kill" dataDxfId="6">
       <calculatedColumnFormula>U2 + V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Time to Kill Vanilla" dataDxfId="3">
+    <tableColumn id="8" name="Time to Kill Vanilla" dataDxfId="1">
+      <calculatedColumnFormula xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Time to Kill StatMax" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Time for Vanilla to Kill" dataDxfId="5">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Time to Kill StatMax" dataDxfId="2">
+    <tableColumn id="9" name="Time for StatMax to Kill" dataDxfId="4">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="1">
+    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Time to Regen Shield">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Time to Regen after Combat">
-      <calculatedColumnFormula>AA2 + $U$43</calculatedColumnFormula>
+      <calculatedColumnFormula>AC2 + $U$43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Time to Top Speed" dataDxfId="0"/>
+    <tableColumn id="6" name="Time to Top Speed" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2568,10 +2592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC43"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,14 +2622,15 @@
     <col min="21" max="21" width="20" customWidth="1"/>
     <col min="22" max="22" width="20.5703125" customWidth="1"/>
     <col min="23" max="23" width="13.140625" customWidth="1"/>
-    <col min="24" max="24" width="20.140625" customWidth="1"/>
-    <col min="25" max="26" width="20.85546875" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" customWidth="1"/>
-    <col min="28" max="28" width="27.85546875" customWidth="1"/>
-    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="24" max="25" width="22.5703125" customWidth="1"/>
+    <col min="26" max="26" width="26.140625" customWidth="1"/>
+    <col min="27" max="27" width="20.85546875" customWidth="1"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="27.85546875" customWidth="1"/>
+    <col min="30" max="30" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2676,19 +2701,25 @@
         <v>29</v>
       </c>
       <c r="Z1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2774,28 +2805,36 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="X2" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>20.796890184645285</v>
+      </c>
+      <c r="Y2" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>20.796890184645285</v>
+      </c>
+      <c r="Z2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>0.69863125305523921</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AA2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.11507904554848752</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AB2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.1</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3</v>
       </c>
-      <c r="AB2">
-        <f>AA2 + $U$43</f>
+      <c r="AD2">
+        <f>AC2 + $U$43</f>
         <v>6</v>
       </c>
-      <c r="AC2" s="2"/>
+      <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2881,28 +2920,36 @@
         <v>3.3348643206331507</v>
       </c>
       <c r="X3" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>7.8156317309389145</v>
+      </c>
+      <c r="Y3" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>7.8156317309389145</v>
+      </c>
+      <c r="Z3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>0.74394655369072893</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AA3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.12254341466033228</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AB3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.1064862973760933</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.5209098696107355</v>
       </c>
-      <c r="AB3">
-        <f t="shared" ref="AB3:AB37" si="3">AA3 + $U$43</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD37" si="3">AC3 + $U$43</f>
         <v>5.520909869610735</v>
       </c>
-      <c r="AC3" s="2"/>
+      <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2988,28 +3035,36 @@
         <v>2.2657081741921505</v>
       </c>
       <c r="X4" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>4.5075725533822961</v>
+      </c>
+      <c r="Y4" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>4.5075725533822961</v>
+      </c>
+      <c r="Z4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>0.87637282059638322</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="AA4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.14435676517164558</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AB4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.12544139941690963</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.3188726479851409</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <f t="shared" si="3"/>
         <v>5.3188726479851409</v>
       </c>
-      <c r="AC4" s="2"/>
+      <c r="AE4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -3095,28 +3150,36 @@
         <v>1.9051255882287297</v>
       </c>
       <c r="X5" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.0456050609644727</v>
+      </c>
+      <c r="Y5" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.0456050609644727</v>
+      </c>
+      <c r="Z5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>1.0906306012709801</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="AA5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.17964946184609604</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AB5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.15610962099125364</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.2754629303668232</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <f t="shared" si="3"/>
         <v>5.2754629303668228</v>
       </c>
-      <c r="AC5" s="2"/>
+      <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3202,28 +3265,36 @@
         <v>1.7764053044532266</v>
       </c>
       <c r="X6" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.242010021072379</v>
+      </c>
+      <c r="Y6" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.242010021072379</v>
+      </c>
+      <c r="Z6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>1.3814404432132972</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="AA6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.22755186944735215</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AB6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.19773527696793003</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.3304189891651528</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <f t="shared" si="3"/>
         <v>5.3304189891651532</v>
       </c>
-      <c r="AC6" s="2"/>
+      <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -3309,28 +3380,36 @@
         <v>1.7435228939221128</v>
       </c>
       <c r="X7" s="12">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.7435228939221128</v>
+      </c>
+      <c r="Y7" s="12">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.7435228939221128</v>
+      </c>
+      <c r="Z7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>1.7435228939221128</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="AA7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.28719435273908256</v>
       </c>
-      <c r="Z7" s="12">
+      <c r="AB7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.2495626822157434</v>
       </c>
-      <c r="AA7" s="13">
+      <c r="AC7" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.4497878359264504</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AD7" s="13">
         <f t="shared" si="3"/>
         <v>5.4497878359264504</v>
       </c>
-      <c r="AC7" s="12"/>
+      <c r="AE7" s="12"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3416,28 +3495,36 @@
         <v>1.7552528646217742</v>
       </c>
       <c r="X8" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.4092492478823588</v>
+      </c>
+      <c r="Y8" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.4092492478823588</v>
+      </c>
+      <c r="Z8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>2.1715985008962049</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="AA8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.35770727648495582</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AB8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.31083615160349853</v>
       </c>
-      <c r="AA8">
+      <c r="AC8">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.6129352718994148</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <f t="shared" si="3"/>
         <v>5.6129352718994152</v>
       </c>
-      <c r="AC8" s="2"/>
+      <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3523,28 +3610,36 @@
         <v>1.7890432377172418</v>
       </c>
       <c r="X9" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.1724748660836468</v>
+      </c>
+      <c r="Y9" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.1724748660836468</v>
+      </c>
+      <c r="Z9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>2.6603878116343513</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="AA9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.43822100544864057</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AB9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.38080000000000003</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>2.8065573770491818</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <f t="shared" si="3"/>
         <v>5.8065573770491818</v>
       </c>
-      <c r="AC9" s="2"/>
+      <c r="AE9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -3630,28 +3725,36 @@
         <v>1.8339357460128376</v>
       </c>
       <c r="X10" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.9977836892990366</v>
+      </c>
+      <c r="Y10" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.9977836892990366</v>
+      </c>
+      <c r="Z10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>3.2046113736353288</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="AA10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.52786590439380521</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AB10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.45869854227405249</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3.0216533855673777</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <f t="shared" si="3"/>
         <v>6.0216533855673777</v>
       </c>
-      <c r="AC10" s="2"/>
+      <c r="AE10" s="2"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -3737,28 +3840,36 @@
         <v>1.8842447962632431</v>
       </c>
       <c r="X11" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.8647625210177704</v>
+      </c>
+      <c r="Y11" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.8647625210177704</v>
+      </c>
+      <c r="Z11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>3.7989897343979164</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AA11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.62577233808411825</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AB11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.54377609329446064</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3.2518812377333277</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <f t="shared" si="3"/>
         <v>6.2518812377333273</v>
       </c>
-      <c r="AC11" s="2"/>
+      <c r="AE11" s="2"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -3844,28 +3955,36 @@
         <v>1.9368888888888889</v>
       </c>
       <c r="X12" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.76088888888888895</v>
+      </c>
+      <c r="Y12" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.76088888888888895</v>
+      </c>
+      <c r="Z12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>4.4382434414208927</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="AA12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.73107067128324876</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AB12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.63527696793002919</v>
       </c>
-      <c r="AA12">
+      <c r="AC12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3.4926108374384235</v>
       </c>
-      <c r="AB12">
+      <c r="AD12">
         <f t="shared" si="3"/>
         <v>6.4926108374384235</v>
       </c>
-      <c r="AC12" s="2"/>
+      <c r="AE12" s="2"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -3951,28 +4070,36 @@
         <v>1.9901518801052953</v>
       </c>
       <c r="X13" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.6780950310514291</v>
+      </c>
+      <c r="Y13" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.6780950310514291</v>
+      </c>
+      <c r="Z13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>5.1170930422030345</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="AA13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.84289126875486475</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AB13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.73244548104956264</v>
       </c>
-      <c r="AA13">
+      <c r="AC13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3.740352189030546</v>
       </c>
-      <c r="AB13">
+      <c r="AD13">
         <f t="shared" si="3"/>
         <v>6.7403521890305456</v>
       </c>
-      <c r="AC13" s="2"/>
+      <c r="AE13" s="2"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4058,28 +4185,36 @@
         <v>2.0430653552969358</v>
       </c>
       <c r="X14" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.61097305784683775</v>
+      </c>
+      <c r="Y14" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.61097305784683775</v>
+      </c>
+      <c r="Z14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>5.830259084243119</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="AA14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>0.96036449526263512</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AB14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.83452594752186593</v>
       </c>
-      <c r="AA14">
+      <c r="AC14">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>3.9923956811459935</v>
       </c>
-      <c r="AB14">
+      <c r="AD14">
         <f t="shared" si="3"/>
         <v>6.9923956811459931</v>
       </c>
-      <c r="AC14" s="2"/>
+      <c r="AE14" s="2"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4165,28 +4300,36 @@
         <v>2.0950830890198597</v>
       </c>
       <c r="X15" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.55577731243461037</v>
+      </c>
+      <c r="Y15" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.55577731243461037</v>
+      </c>
+      <c r="Z15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>6.5724621150399276</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="AA15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.0826207155702283</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AB15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>0.94076268221574355</v>
       </c>
-      <c r="AA15">
+      <c r="AC15">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>4.2465777717150361</v>
       </c>
-      <c r="AB15">
+      <c r="AD15">
         <f t="shared" si="3"/>
         <v>7.2465777717150361</v>
       </c>
-      <c r="AC15" s="2"/>
+      <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4272,28 +4415,36 @@
         <v>2.1459017036465626</v>
       </c>
       <c r="X16" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.50984099860374088</v>
+      </c>
+      <c r="Y16" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.50984099860374088</v>
+      </c>
+      <c r="Z16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>7.3384226820922347</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="AA16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.2087902944413134</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AB16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.0504000000000002</v>
       </c>
-      <c r="AA16">
+      <c r="AC16">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>4.5011235955056188</v>
       </c>
-      <c r="AB16">
+      <c r="AD16">
         <f t="shared" si="3"/>
         <v>7.5011235955056188</v>
       </c>
-      <c r="AC16" s="2"/>
+      <c r="AE16" s="2"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -4379,28 +4530,36 @@
         <v>2.1953582595675334</v>
       </c>
       <c r="X17" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.47122032853305129</v>
+      </c>
+      <c r="Y17" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.47122032853305129</v>
+      </c>
+      <c r="Z17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>8.1228613328988146</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="AA17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.3380035966395574</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AB17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.16268221574344</v>
       </c>
-      <c r="AA17">
+      <c r="AC17">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>4.7545382794001574</v>
       </c>
-      <c r="AB17">
+      <c r="AD17">
         <f t="shared" si="3"/>
         <v>7.7545382794001574</v>
       </c>
-      <c r="AC17" s="2"/>
+      <c r="AE17" s="2"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -4486,28 +4645,36 @@
         <v>2.2433700044673088</v>
       </c>
       <c r="X18" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.43846954426606577</v>
+      </c>
+      <c r="Y18" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.43846954426606577</v>
+      </c>
+      <c r="Z18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>8.9204986149584542</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="AA18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.4693909869286308</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="AB18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.2768536443148688</v>
       </c>
-      <c r="AA18">
+      <c r="AC18">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>5.0055299539170512</v>
       </c>
-      <c r="AB18">
+      <c r="AD18">
         <f t="shared" si="3"/>
         <v>8.0055299539170512</v>
       </c>
-      <c r="AC18" s="2"/>
+      <c r="AE18" s="2"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -4593,28 +4760,36 @@
         <v>2.2898979991636041</v>
       </c>
       <c r="X19" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.41049423997551571</v>
+      </c>
+      <c r="Y19" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.41049423997551571</v>
+      </c>
+      <c r="Z19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>9.726055075769926</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="AA19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.602082830072201</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AB19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.3921586005830904</v>
       </c>
-      <c r="AA19">
+      <c r="AC19">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>5.2529538798331501</v>
       </c>
-      <c r="AB19">
+      <c r="AD19">
         <f t="shared" si="3"/>
         <v>8.2529538798331501</v>
       </c>
-      <c r="AC19" s="2"/>
+      <c r="AE19" s="2"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -4700,28 +4875,36 @@
         <v>2.3349246245893016</v>
       </c>
       <c r="X20" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.38645314574160849</v>
+      </c>
+      <c r="Y20" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.38645314574160849</v>
+      </c>
+      <c r="Z20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>10.53425126283201</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="AA20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.7352094908339373</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AB20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.5078413994169098</v>
       </c>
-      <c r="AA20">
+      <c r="AC20">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>5.4957709225771207</v>
       </c>
-      <c r="AB20">
+      <c r="AD20">
         <f t="shared" si="3"/>
         <v>8.4957709225771207</v>
       </c>
-      <c r="AC20" s="2"/>
+      <c r="AE20" s="2"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -4807,28 +4990,36 @@
         <v>2.3784393185940393</v>
       </c>
       <c r="X21" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.36569080400957893</v>
+      </c>
+      <c r="Y21" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.36569080400957893</v>
+      </c>
+      <c r="Z21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>11.339807723643482</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="AA21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.8679013339775077</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AB21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.6231463556851311</v>
       </c>
-      <c r="AA21">
+      <c r="AC21">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>5.7330159352507906</v>
       </c>
-      <c r="AB21">
+      <c r="AD21">
         <f t="shared" si="3"/>
         <v>8.7330159352507906</v>
       </c>
-      <c r="AC21" s="2"/>
+      <c r="AE21" s="2"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -4914,28 +5105,36 @@
         <v>2.4204292514906816</v>
       </c>
       <c r="X22" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.34769045800906584</v>
+      </c>
+      <c r="Y22" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.34769045800906584</v>
+      </c>
+      <c r="Z22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>12.137445005703121</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="AA22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>1.9992887242665804</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="AB22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.7373177842565597</v>
       </c>
-      <c r="AA22">
+      <c r="AC22">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>5.9637730690362263</v>
       </c>
-      <c r="AB22">
+      <c r="AD22">
         <f t="shared" si="3"/>
         <v>8.9637730690362254</v>
       </c>
-      <c r="AC22" s="2"/>
+      <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -5021,28 +5220,36 @@
         <v>2.4608729712699469</v>
       </c>
       <c r="X23" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.33204047323872954</v>
+      </c>
+      <c r="Y23" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.33204047323872954</v>
+      </c>
+      <c r="Z23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>12.921883656509703</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="AA23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.1285020264648251</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AB23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.8495999999999999</v>
       </c>
-      <c r="AA23">
+      <c r="AC23">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>6.187155963302752</v>
       </c>
-      <c r="AB23">
+      <c r="AD23">
         <f t="shared" si="3"/>
         <v>9.187155963302752</v>
       </c>
-      <c r="AC23" s="2"/>
+      <c r="AE23" s="2"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -5128,28 +5335,36 @@
         <v>2.4997358089658017</v>
       </c>
       <c r="X24" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.31841000967752164</v>
+      </c>
+      <c r="Y24" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.31841000967752164</v>
+      </c>
+      <c r="Z24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>13.68784422356201</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="AA24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.2546716053359095</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="AB24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>1.9592373177842564</v>
       </c>
-      <c r="AA24">
+      <c r="AC24">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>6.4022913771858532</v>
       </c>
-      <c r="AB24">
+      <c r="AD24">
         <f t="shared" si="3"/>
         <v>9.4022913771858541</v>
       </c>
-      <c r="AC24" s="2"/>
+      <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -5235,28 +5450,36 @@
         <v>2.5369662800165029</v>
       </c>
       <c r="X25" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.30653113689430761</v>
+      </c>
+      <c r="Y25" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.30653113689430761</v>
+      </c>
+      <c r="Z25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>14.430047254358817</v>
       </c>
-      <c r="Y25" s="2">
+      <c r="AA25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.3769278256435031</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AB25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.0654740524781343</v>
       </c>
-      <c r="AA25">
+      <c r="AC25">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>6.6083052287413429</v>
       </c>
-      <c r="AB25">
+      <c r="AD25">
         <f t="shared" si="3"/>
         <v>9.6083052287413437</v>
       </c>
-      <c r="AC25" s="2"/>
+      <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -5342,28 +5565,36 @@
         <v>2.5724929822856257</v>
       </c>
       <c r="X26" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.29618551368721419</v>
+      </c>
+      <c r="Y26" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.29618551368721419</v>
+      </c>
+      <c r="Z26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>15.143213296398901</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="AA26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.4944010521512734</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="AB26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.1675545189504373</v>
       </c>
-      <c r="AA26">
+      <c r="AC26">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>6.8043102793324381</v>
       </c>
-      <c r="AB26">
+      <c r="AD26">
         <f t="shared" si="3"/>
         <v>9.8043102793324373</v>
       </c>
-      <c r="AC26" s="2"/>
+      <c r="AE26" s="2"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -5449,28 +5680,36 @@
         <v>2.6062216496228894</v>
       </c>
       <c r="X27" s="12">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.28719435273908256</v>
+      </c>
+      <c r="Y27" s="12">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.28719435273908256</v>
+      </c>
+      <c r="Z27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>15.822062897181041</v>
       </c>
-      <c r="Y27" s="12">
+      <c r="AA27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.6062216496228894</v>
       </c>
-      <c r="Z27" s="12">
+      <c r="AB27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.2647230320699707</v>
       </c>
-      <c r="AA27" s="13">
+      <c r="AC27" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>6.9893948845913902</v>
       </c>
-      <c r="AB27" s="13">
+      <c r="AD27" s="13">
         <f t="shared" si="3"/>
         <v>9.9893948845913911</v>
       </c>
-      <c r="AC27" s="12"/>
+      <c r="AE27" s="12"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -5556,28 +5795,36 @@
         <v>2.6380321132924975</v>
       </c>
       <c r="X28" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.27941078438723144</v>
+      </c>
+      <c r="Y28" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.27941078438723144</v>
+      </c>
+      <c r="Z28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>16.461316604204022</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="AA28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.7115199828220202</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="AB28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.3562239067055395</v>
       </c>
-      <c r="AA28">
+      <c r="AC28">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.1626123574753118</v>
       </c>
-      <c r="AB28">
+      <c r="AD28">
         <f t="shared" si="3"/>
         <v>10.162612357475311</v>
       </c>
-      <c r="AC28" s="2"/>
+      <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -5663,28 +5910,36 @@
         <v>2.6677749763508545</v>
       </c>
       <c r="X29" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.27271399709330718</v>
+      </c>
+      <c r="Y29" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.27271399709330718</v>
+      </c>
+      <c r="Z29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>17.055694964966609</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="AA29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.8094264165123333</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="AB29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.4413014577259475</v>
       </c>
-      <c r="AA29">
+      <c r="AC29">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.3229705717693445</v>
       </c>
-      <c r="AB29">
+      <c r="AD29">
         <f t="shared" si="3"/>
         <v>10.322970571769345</v>
       </c>
-      <c r="AC29" s="2"/>
+      <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -5770,28 +6025,36 @@
         <v>2.6952678320768548</v>
       </c>
       <c r="X30" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.26700471160007611</v>
+      </c>
+      <c r="Y30" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.26700471160007611</v>
+      </c>
+      <c r="Z30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>17.599918526967588</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="AA30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.8990713154574985</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="AB30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.5192000000000005</v>
       </c>
-      <c r="AA30">
+      <c r="AC30">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.4694214876033067</v>
       </c>
-      <c r="AB30">
+      <c r="AD30">
         <f t="shared" si="3"/>
         <v>10.469421487603306</v>
       </c>
-      <c r="AC30" s="2"/>
+      <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -5877,28 +6140,36 @@
         <v>2.7202908648702975</v>
       </c>
       <c r="X31" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.26220166988058935</v>
+      </c>
+      <c r="Y31" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.26220166988058935</v>
+      </c>
+      <c r="Z31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>18.088707837705734</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="AA31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>2.9795850444211829</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="AB31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.5891638483965016</v>
       </c>
-      <c r="AA31">
+      <c r="AC31">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.6008503117013406</v>
       </c>
-      <c r="AB31">
+      <c r="AD31">
         <f t="shared" si="3"/>
         <v>10.60085031170134</v>
       </c>
-      <c r="AC31" s="2"/>
+      <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -5984,28 +6255,36 @@
         <v>2.7425816650375898</v>
       </c>
       <c r="X32" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25823890719086751</v>
+      </c>
+      <c r="Y32" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25823890719086751</v>
+      </c>
+      <c r="Z32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>18.516783444679824</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="AA32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.0500979681670559</v>
       </c>
-      <c r="Z32" s="2">
+      <c r="AB32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.6504373177842568</v>
       </c>
-      <c r="AA32">
+      <c r="AC32">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.7160640189685834</v>
       </c>
-      <c r="AB32">
+      <c r="AD32">
         <f t="shared" si="3"/>
         <v>10.716064018968584</v>
       </c>
-      <c r="AC32" s="2"/>
+      <c r="AE32" s="2"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -6091,28 +6370,36 @@
         <v>2.7618290696418897</v>
       </c>
       <c r="X33" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.2550636377578398</v>
+      </c>
+      <c r="Y33" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.2550636377578398</v>
+      </c>
+      <c r="Z33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>18.878865895388643</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="AA33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.1097404514587863</v>
       </c>
-      <c r="Z33" s="2">
+      <c r="AB33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.7022647230320702</v>
       </c>
-      <c r="AA33">
+      <c r="AC33">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.8137789615103594</v>
       </c>
-      <c r="AB33">
+      <c r="AD33">
         <f t="shared" si="3"/>
         <v>10.813778961510359</v>
       </c>
-      <c r="AC33" s="2"/>
+      <c r="AE33" s="2"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -6198,28 +6485,36 @@
         <v>2.7776658105296184</v>
       </c>
       <c r="X34" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25263462974973644</v>
+      </c>
+      <c r="Y34" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25263462974973644</v>
+      </c>
+      <c r="Z34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>19.169675737330955</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="AA34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.1576428590600418</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="AB34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.7438903790087461</v>
       </c>
-      <c r="AA34">
+      <c r="AC34">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.8926072777608329</v>
       </c>
-      <c r="AB34">
+      <c r="AD34">
         <f t="shared" si="3"/>
         <v>10.892607277760833</v>
       </c>
-      <c r="AC34" s="2"/>
+      <c r="AE34" s="2"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -6305,28 +6600,36 @@
         <v>2.7896597068785223</v>
       </c>
       <c r="X35" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25092097848338069</v>
+      </c>
+      <c r="Y35" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.25092097848338069</v>
+      </c>
+      <c r="Z35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>19.383933518005556</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="AA35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.1929355557344929</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="AB35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.7745586005830907</v>
       </c>
-      <c r="AA35">
+      <c r="AC35">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.9510417884619891</v>
       </c>
-      <c r="AB35">
+      <c r="AD35">
         <f t="shared" si="3"/>
         <v>10.951041788461989</v>
       </c>
-      <c r="AC35" s="2"/>
+      <c r="AE35" s="2"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -6412,28 +6715,36 @@
         <v>2.7973030810680095</v>
       </c>
       <c r="X36" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.24990121194894377</v>
+      </c>
+      <c r="Y36" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.24990121194894377</v>
+      </c>
+      <c r="Z36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>19.516359784911209</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="AA36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.2147489062458061</v>
       </c>
-      <c r="Z36" s="2">
+      <c r="AB36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.793513702623907</v>
       </c>
-      <c r="AA36">
+      <c r="AC36">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>7.9874390272364471</v>
       </c>
-      <c r="AB36">
+      <c r="AD36">
         <f t="shared" si="3"/>
         <v>10.987439027236448</v>
       </c>
-      <c r="AC36" s="2"/>
+      <c r="AE36" s="2"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -6519,28 +6830,36 @@
         <v>2.8</v>
       </c>
       <c r="X37" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.2495626822157434</v>
+      </c>
+      <c r="Y37" s="2">
+        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>0.2495626822157434</v>
+      </c>
+      <c r="Z37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
         <v>19.561675085546696</v>
       </c>
-      <c r="Y37" s="2">
+      <c r="AA37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
         <v>3.2222132753576509</v>
       </c>
-      <c r="Z37" s="2">
+      <c r="AB37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
         <v>2.8</v>
       </c>
-      <c r="AA37">
+      <c r="AC37">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
         <v>8</v>
       </c>
-      <c r="AB37">
+      <c r="AD37">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="AC37" s="2"/>
+      <c r="AE37" s="2"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G39" s="8" t="s">
         <v>7</v>
       </c>
@@ -6581,7 +6900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
         <v>8</v>
       </c>
@@ -6622,12 +6941,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="T42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="T43" t="s">
         <v>25</v>
       </c>
@@ -6637,7 +6956,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="3">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Did some balance changes
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -116,13 +116,13 @@
     <t>Time to Kill StatMax</t>
   </si>
   <si>
-    <t>Time to Kill AbsMax</t>
-  </si>
-  <si>
     <t>Time for Vanilla to Kill</t>
   </si>
   <si>
     <t>Time for StatMax to Kill</t>
+  </si>
+  <si>
+    <t>Time for AbsMax to Kill</t>
   </si>
 </sst>
 </file>
@@ -2268,19 +2268,19 @@
     <tableColumn id="3" name="Time to Kill" dataDxfId="6">
       <calculatedColumnFormula>U2 + V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Time to Kill Vanilla" dataDxfId="1">
+    <tableColumn id="8" name="Time to Kill Vanilla" dataDxfId="2">
       <calculatedColumnFormula xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Time to Kill StatMax" dataDxfId="0">
-      <calculatedColumnFormula xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" name="Time for Vanilla to Kill" dataDxfId="5">
+    <tableColumn id="12" name="Time for Vanilla to Kill" dataDxfId="0">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Time for StatMax to Kill" dataDxfId="4">
+    <tableColumn id="11" name="Time to Kill StatMax" dataDxfId="1">
+      <calculatedColumnFormula xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Time for StatMax to Kill" dataDxfId="5">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Time to Kill AbsMax" dataDxfId="3">
+    <tableColumn id="10" name="Time for AbsMax to Kill" dataDxfId="4">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Time to Regen Shield">
@@ -2289,7 +2289,7 @@
     <tableColumn id="5" name="Time to Regen after Combat">
       <calculatedColumnFormula>AC2 + $U$43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Time to Top Speed" dataDxfId="2"/>
+    <tableColumn id="6" name="Time to Top Speed" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2594,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,10 +2624,11 @@
     <col min="23" max="23" width="13.140625" customWidth="1"/>
     <col min="24" max="25" width="22.5703125" customWidth="1"/>
     <col min="26" max="26" width="26.140625" customWidth="1"/>
-    <col min="27" max="27" width="20.85546875" customWidth="1"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1"/>
-    <col min="29" max="29" width="27.85546875" customWidth="1"/>
-    <col min="30" max="30" width="21" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" customWidth="1"/>
+    <col min="28" max="28" width="27.85546875" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="30" max="30" width="32" customWidth="1"/>
+    <col min="31" max="31" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -2698,16 +2699,16 @@
         <v>28</v>
       </c>
       <c r="Y1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>32</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>30</v>
       </c>
       <c r="AC1" t="s">
         <v>23</v>
@@ -2778,7 +2779,7 @@
       </c>
       <c r="P2" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q2" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
@@ -2798,31 +2799,31 @@
       </c>
       <c r="V2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.3333333333333335</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="W2" s="2">
         <f>U2 + V2</f>
-        <v>8.3333333333333339</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="X2" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>20.796890184645285</v>
+        <v>31.545189504373177</v>
       </c>
       <c r="Y2" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>20.796890184645285</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>1.816441257943622</v>
       </c>
       <c r="Z2" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>0.69863125305523921</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>164.64528668610302</v>
       </c>
       <c r="AA2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.11507904554848752</v>
+        <v>0.29920551842606757</v>
       </c>
       <c r="AB2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="AC2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
@@ -2893,11 +2894,11 @@
       </c>
       <c r="P3" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>22.354285714285716</v>
+        <v>102.16209912536443</v>
       </c>
       <c r="Q3" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>30.888862973760933</v>
+        <v>30.408396501457727</v>
       </c>
       <c r="R3" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2909,43 +2910,43 @@
       </c>
       <c r="U3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9347121568572454</v>
+        <v>1.9046183225287703</v>
       </c>
       <c r="V3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4001521637759056</v>
+        <v>6.3988841323100258</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" ref="W3:W37" si="2">U3 + V3</f>
-        <v>3.3348643206331507</v>
+        <v>8.3035024548387959</v>
       </c>
       <c r="X3" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>7.8156317309389145</v>
+        <v>11.854925513377438</v>
       </c>
       <c r="Y3" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>7.8156317309389145</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>1.8523578295584175</v>
       </c>
       <c r="Z3" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>0.74394655369072893</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>61.874968591386498</v>
       </c>
       <c r="AA3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.12254341466033228</v>
+        <v>0.30512172209249266</v>
       </c>
       <c r="AB3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.1064862973760933</v>
+        <v>0.26514099125364432</v>
       </c>
       <c r="AC3">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.5209098696107355</v>
+        <v>2.4816979156752641</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD37" si="3">AC3 + $U$43</f>
-        <v>5.520909869610735</v>
+        <v>5.4816979156752641</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
@@ -3008,11 +3009,11 @@
       </c>
       <c r="P4" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>29.234285714285711</v>
+        <v>108.48046647230321</v>
       </c>
       <c r="Q4" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>33.486413994169098</v>
+        <v>31.601865889212828</v>
       </c>
       <c r="R4" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3024,43 +3025,43 @@
       </c>
       <c r="U4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2096555405733769</v>
+        <v>1.141578556963416</v>
       </c>
       <c r="V4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0560526336187734</v>
+        <v>3.9187234958946546</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="2"/>
-        <v>2.2657081741921505</v>
+        <v>5.0603020528580709</v>
       </c>
       <c r="X4" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.5075725533822961</v>
+        <v>6.8371871534013717</v>
       </c>
       <c r="Y4" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.5075725533822961</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>1.9573179077725287</v>
       </c>
       <c r="Z4" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>0.87637282059638322</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>35.68565149504807</v>
       </c>
       <c r="AA4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.14435676517164558</v>
+        <v>0.32241082212738548</v>
       </c>
       <c r="AB4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.12544139941690963</v>
+        <v>0.28016466472303209</v>
       </c>
       <c r="AC4">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.3188726479851409</v>
+        <v>2.1883711540014534</v>
       </c>
       <c r="AD4">
         <f t="shared" si="3"/>
-        <v>5.3188726479851409</v>
+        <v>5.1883711540014534</v>
       </c>
       <c r="AE4" s="2"/>
     </row>
@@ -3123,11 +3124,11 @@
       </c>
       <c r="P5" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>40.36571428571429</v>
+        <v>118.70320699708455</v>
       </c>
       <c r="Q5" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>37.689096209912535</v>
+        <v>33.532827988338191</v>
       </c>
       <c r="R5" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3139,43 +3140,43 @@
       </c>
       <c r="U5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.91989796824555337</v>
+        <v>0.81845370247660587</v>
       </c>
       <c r="V5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.98522761998317643</v>
+        <v>2.8972527845369322</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="2"/>
-        <v>1.9051255882287297</v>
+        <v>3.7157064870135379</v>
       </c>
       <c r="X5" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.0456050609644727</v>
+        <v>4.6196420691077931</v>
       </c>
       <c r="Y5" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.0456050609644727</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.1271370376405425</v>
       </c>
       <c r="Z5" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.0906306012709801</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>24.111514459280418</v>
       </c>
       <c r="AA5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.17964946184609604</v>
+        <v>0.35038355208417205</v>
       </c>
       <c r="AB5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.15610962099125364</v>
+        <v>0.30447206997084547</v>
       </c>
       <c r="AC5">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.2754629303668232</v>
+        <v>2.0245300288671402</v>
       </c>
       <c r="AD5">
         <f t="shared" si="3"/>
-        <v>5.2754629303668228</v>
+        <v>5.0245300288671402</v>
       </c>
       <c r="AE5" s="2"/>
     </row>
@@ -3238,11 +3239,11 @@
       </c>
       <c r="P6" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>55.474285714285713</v>
+        <v>132.57842565597667</v>
       </c>
       <c r="Q6" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>43.393352769679296</v>
+        <v>36.153702623906703</v>
       </c>
       <c r="R6" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3254,43 +3255,43 @@
       </c>
       <c r="U6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.77967050917849545</v>
+        <v>0.6495920212269316</v>
       </c>
       <c r="V6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.99673479527473108</v>
+        <v>2.3821042173423788</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="2"/>
-        <v>1.7764053044532266</v>
+        <v>3.0316962385693103</v>
       </c>
       <c r="X6" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.242010021072379</v>
+        <v>3.4007310880378236</v>
       </c>
       <c r="Y6" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.242010021072379</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.3576307642170455</v>
       </c>
       <c r="Z6" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.3814404432132972</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>17.74959522290105</v>
       </c>
       <c r="AA6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.22755186944735215</v>
+        <v>0.38835064551627879</v>
       </c>
       <c r="AB6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.19773527696793003</v>
+        <v>0.33746425655976675</v>
       </c>
       <c r="AC6">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.3304189891651528</v>
+        <v>1.9416170852383039</v>
       </c>
       <c r="AD6">
         <f t="shared" si="3"/>
-        <v>5.3304189891651532</v>
+        <v>4.9416170852383043</v>
       </c>
       <c r="AE6" s="2"/>
     </row>
@@ -3353,11 +3354,11 @@
       </c>
       <c r="P7" s="5">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>74.285714285714278</v>
+        <v>149.8542274052478</v>
       </c>
       <c r="Q7" s="5">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>50.495626822157433</v>
+        <v>39.416909620991255</v>
       </c>
       <c r="R7" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3369,43 +3370,43 @@
       </c>
       <c r="U7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.70555646081147183</v>
+        <v>0.5507576992015647</v>
       </c>
       <c r="V7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0379664331106411</v>
+        <v>2.0938569333550605</v>
       </c>
       <c r="W7" s="12">
         <f t="shared" si="2"/>
-        <v>1.7435228939221128</v>
+        <v>2.6446146325566251</v>
       </c>
       <c r="X7" s="12">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.7435228939221128</v>
+        <v>2.6446146325566251</v>
       </c>
       <c r="Y7" s="12">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.7435228939221128</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.6446146325566251</v>
       </c>
       <c r="Z7" s="12">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.7435228939221128</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>13.803161153658147</v>
       </c>
       <c r="AA7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.28719435273908256</v>
+        <v>0.43562283597713175</v>
       </c>
       <c r="AB7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.2495626822157434</v>
+        <v>0.37854227405247809</v>
       </c>
       <c r="AC7" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.4497878359264504</v>
+        <v>1.9123055162659128</v>
       </c>
       <c r="AD7" s="13">
         <f t="shared" si="3"/>
-        <v>5.4497878359264504</v>
+        <v>4.9123055162659126</v>
       </c>
       <c r="AE7" s="12"/>
     </row>
@@ -3468,11 +3469,11 @@
       </c>
       <c r="P8" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>96.525714285714287</v>
+        <v>170.27871720116616</v>
       </c>
       <c r="Q8" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>58.892361516034981</v>
+        <v>43.27486880466472</v>
       </c>
       <c r="R8" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3484,43 +3485,43 @@
       </c>
       <c r="U8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.66511559689634292</v>
+        <v>0.48873554149783316</v>
       </c>
       <c r="V8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.0901372677254313</v>
+        <v>1.9230852306569601</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="2"/>
-        <v>1.7552528646217742</v>
+        <v>2.4118207721547931</v>
       </c>
       <c r="X8" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.4092492478823588</v>
+        <v>2.1375808685168862</v>
       </c>
       <c r="Y8" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.4092492478823588</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>2.9839041877138688</v>
       </c>
       <c r="Z8" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.1715985008962049</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>11.156776054963983</v>
       </c>
       <c r="AA8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.35770727648495582</v>
+        <v>0.49151085702015718</v>
       </c>
       <c r="AB8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.31083615160349853</v>
+        <v>0.42710717201166176</v>
       </c>
       <c r="AC8">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.6129352718994148</v>
+        <v>1.9200186267915347</v>
       </c>
       <c r="AD8">
         <f t="shared" si="3"/>
-        <v>5.6129352718994152</v>
+        <v>4.9200186267915349</v>
       </c>
       <c r="AE8" s="2"/>
     </row>
@@ -3583,11 +3584,11 @@
       </c>
       <c r="P9" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>121.92000000000002</v>
+        <v>193.60000000000002</v>
       </c>
       <c r="Q9" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>68.480000000000018</v>
+        <v>47.680000000000007</v>
       </c>
       <c r="R9" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3599,43 +3600,43 @@
       </c>
       <c r="U9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.64345420650670559</v>
+        <v>0.44801250826868744</v>
       </c>
       <c r="V9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.1455890312105363</v>
+        <v>1.8191111912923215</v>
       </c>
       <c r="W9" s="2">
         <f t="shared" si="2"/>
-        <v>1.7890432377172418</v>
+        <v>2.2671236995610089</v>
       </c>
       <c r="X9" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.1724748660836468</v>
+        <v>1.7784361753773448</v>
       </c>
       <c r="Y9" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.1724748660836468</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>3.3713149747433624</v>
       </c>
       <c r="Z9" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.6603878116343513</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>9.2822753183126832</v>
       </c>
       <c r="AA9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.43822100544864057</v>
+        <v>0.55532544219878144</v>
       </c>
       <c r="AB9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.38080000000000003</v>
+        <v>0.48256000000000004</v>
       </c>
       <c r="AC9">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>2.8065573770491818</v>
+        <v>1.9540983606557383</v>
       </c>
       <c r="AD9">
         <f t="shared" si="3"/>
-        <v>5.8065573770491818</v>
+        <v>4.9540983606557383</v>
       </c>
       <c r="AE9" s="2"/>
     </row>
@@ -3698,11 +3699,11 @@
       </c>
       <c r="P10" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>150.19428571428571</v>
+        <v>219.56618075801748</v>
       </c>
       <c r="Q10" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>79.154985422740523</v>
+        <v>52.584723032069974</v>
       </c>
       <c r="R10" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3714,43 +3715,43 @@
       </c>
       <c r="U10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.63294361705278346</v>
+        <v>0.42048096680054753</v>
       </c>
       <c r="V10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2009921289600543</v>
+        <v>1.7557076397555516</v>
       </c>
       <c r="W10" s="2">
         <f t="shared" si="2"/>
-        <v>1.8339357460128376</v>
+        <v>2.1761886065560989</v>
       </c>
       <c r="X10" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.9977836892990366</v>
+        <v>1.513460680123679</v>
       </c>
       <c r="Y10" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.9977836892990366</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>3.8026625386996931</v>
       </c>
       <c r="Z10" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.2046113736353288</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>7.8992762916375128</v>
       </c>
       <c r="AA10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.52786590439380521</v>
+        <v>0.6263773250664304</v>
       </c>
       <c r="AB10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.45869854227405249</v>
+        <v>0.54430180758017488</v>
       </c>
       <c r="AC10">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.0216533855673777</v>
+        <v>2.0073632195165385</v>
       </c>
       <c r="AD10">
         <f t="shared" si="3"/>
-        <v>6.0216533855673777</v>
+        <v>5.0073632195165381</v>
       </c>
       <c r="AE10" s="2"/>
     </row>
@@ -3813,11 +3814,11 @@
       </c>
       <c r="P11" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>181.07428571428568</v>
+        <v>247.92536443148686</v>
       </c>
       <c r="Q11" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>90.813760932944604</v>
+        <v>57.941457725947515</v>
       </c>
       <c r="R11" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3829,43 +3830,43 @@
       </c>
       <c r="U11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.62935961538983765</v>
+        <v>0.4015472234043338</v>
       </c>
       <c r="V11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.2548851808734056</v>
+        <v>1.7181780646569522</v>
       </c>
       <c r="W11" s="2">
         <f t="shared" si="2"/>
-        <v>1.8842447962632431</v>
+        <v>2.1197252880612858</v>
       </c>
       <c r="X11" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.8647625210177704</v>
+        <v>1.3116911884222815</v>
       </c>
       <c r="Y11" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.8647625210177704</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>4.2737624246374475</v>
       </c>
       <c r="Z11" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.7989897343979164</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>6.8461713229360113</v>
       </c>
       <c r="AA11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.62577233808411825</v>
+        <v>0.70397723917653043</v>
       </c>
       <c r="AB11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.54377609329446064</v>
+        <v>0.61173364431486876</v>
       </c>
       <c r="AC11">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.2518812377333277</v>
+        <v>2.074781809830041</v>
       </c>
       <c r="AD11">
         <f t="shared" si="3"/>
-        <v>6.2518812377333273</v>
+        <v>5.074781809830041</v>
       </c>
       <c r="AE11" s="2"/>
     </row>
@@ -3928,11 +3929,11 @@
       </c>
       <c r="P12" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>214.28571428571428</v>
+        <v>278.42565597667635</v>
       </c>
       <c r="Q12" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>103.35276967930029</v>
+        <v>63.70262390670554</v>
       </c>
       <c r="R12" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3944,43 +3945,43 @@
       </c>
       <c r="U12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.63022222222222224</v>
+        <v>0.38844444444444448</v>
       </c>
       <c r="V12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.3066666666666666</v>
+        <v>1.6977777777777776</v>
       </c>
       <c r="W12" s="2">
         <f t="shared" si="2"/>
-        <v>1.9368888888888889</v>
+        <v>2.0862222222222222</v>
       </c>
       <c r="X12" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.76088888888888895</v>
+        <v>1.1541333333333332</v>
       </c>
       <c r="Y12" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.76088888888888895</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>4.7804301776112137</v>
       </c>
       <c r="Z12" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>4.4382434414208927</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>6.023822222222222</v>
       </c>
       <c r="AA12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.73107067128324876</v>
+        <v>0.7874359180825079</v>
       </c>
       <c r="AB12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.63527696793002919</v>
+        <v>0.68425655976676381</v>
       </c>
       <c r="AC12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.4926108374384235</v>
+        <v>2.1527093596059115</v>
       </c>
       <c r="AD12">
         <f t="shared" si="3"/>
-        <v>6.4926108374384235</v>
+        <v>5.152709359605911</v>
       </c>
       <c r="AE12" s="2"/>
     </row>
@@ -4043,11 +4044,11 @@
       </c>
       <c r="P13" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>249.5542857142857</v>
+        <v>310.81516034985418</v>
       </c>
       <c r="Q13" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>116.66845481049562</v>
+        <v>69.8206413994169</v>
       </c>
       <c r="R13" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4059,43 +4060,43 @@
       </c>
       <c r="U13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.63400744682695642</v>
+        <v>0.37942395535594692</v>
       </c>
       <c r="V13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.356144433278339</v>
+        <v>1.6890523369715054</v>
       </c>
       <c r="W13" s="2">
         <f t="shared" si="2"/>
-        <v>1.9901518801052953</v>
+        <v>2.0684762923274524</v>
       </c>
       <c r="X13" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.6780950310514291</v>
+        <v>1.0285497527069807</v>
       </c>
       <c r="Y13" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.6780950310514291</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>5.318481342675577</v>
       </c>
       <c r="Z13" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>5.1170930422030345</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>5.3683579514361277</v>
       </c>
       <c r="AA13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.84289126875486475</v>
+        <v>0.87606409533778873</v>
       </c>
       <c r="AB13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.73244548104956264</v>
+        <v>0.76127160349854217</v>
       </c>
       <c r="AC13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.740352189030546</v>
+        <v>2.2384267394474149</v>
       </c>
       <c r="AD13">
         <f t="shared" si="3"/>
-        <v>6.7403521890305456</v>
+        <v>5.2384267394474149</v>
       </c>
       <c r="AE13" s="2"/>
     </row>
@@ -4158,11 +4159,11 @@
       </c>
       <c r="P14" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>286.60571428571427</v>
+        <v>344.84198250728861</v>
       </c>
       <c r="Q14" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>130.65725947521867</v>
+        <v>76.247930029154517</v>
       </c>
       <c r="R14" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4174,43 +4175,43 @@
       </c>
       <c r="U14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.63974360783998818</v>
+        <v>0.37333651450445476</v>
       </c>
       <c r="V14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4033217474569475</v>
+        <v>1.6884668705740713</v>
       </c>
       <c r="W14" s="2">
         <f t="shared" si="2"/>
-        <v>2.0430653552969358</v>
+        <v>2.0618033850785262</v>
       </c>
       <c r="X14" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.61097305784683775</v>
+        <v>0.92673763821067079</v>
       </c>
       <c r="Y14" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.61097305784683775</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>5.8837314648851269</v>
       </c>
       <c r="Z14" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>5.830259084243119</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>4.8369652084304322</v>
       </c>
       <c r="AA14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.96036449526263512</v>
+        <v>0.96917250449579928</v>
       </c>
       <c r="AB14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.83452594752186593</v>
+        <v>0.84217982507288625</v>
       </c>
       <c r="AC14">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>3.9923956811459935</v>
+        <v>2.3298506930834195</v>
       </c>
       <c r="AD14">
         <f t="shared" si="3"/>
-        <v>6.9923956811459931</v>
+        <v>5.3298506930834195</v>
       </c>
       <c r="AE14" s="2"/>
     </row>
@@ -4273,11 +4274,11 @@
       </c>
       <c r="P15" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>325.16571428571433</v>
+        <v>380.25422740524783</v>
       </c>
       <c r="Q15" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>145.21562682215745</v>
+        <v>82.936909620991258</v>
       </c>
       <c r="R15" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4289,43 +4290,43 @@
       </c>
       <c r="U15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.64679182065334151</v>
+        <v>0.3694018057630804</v>
       </c>
       <c r="V15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4482912683665183</v>
+        <v>1.6936560440273698</v>
       </c>
       <c r="W15" s="2">
         <f t="shared" si="2"/>
-        <v>2.0950830890198597</v>
+        <v>2.0630578497904501</v>
       </c>
       <c r="X15" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.55577731243461037</v>
+        <v>0.84301549353399308</v>
       </c>
       <c r="Y15" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.55577731243461037</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>6.4719960892944481</v>
       </c>
       <c r="Z15" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>6.5724621150399276</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>4.3999902931154997</v>
       </c>
       <c r="AA15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.0826207155702283</v>
+        <v>1.0660718791099659</v>
       </c>
       <c r="AB15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>0.94076268221574355</v>
+        <v>0.92638227405247819</v>
       </c>
       <c r="AC15">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>4.2465777717150361</v>
+        <v>2.4253452920915324</v>
       </c>
       <c r="AD15">
         <f t="shared" si="3"/>
-        <v>7.2465777717150361</v>
+        <v>5.4253452920915324</v>
       </c>
       <c r="AE15" s="2"/>
     </row>
@@ -4388,11 +4389,11 @@
       </c>
       <c r="P16" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>364.96000000000009</v>
+        <v>416.80000000000007</v>
       </c>
       <c r="Q16" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>160.24000000000004</v>
+        <v>89.840000000000018</v>
       </c>
       <c r="R16" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4404,43 +4405,43 @@
       </c>
       <c r="U16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.65472065687799919</v>
+        <v>0.36707503628257265</v>
       </c>
       <c r="V16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.4911810467685633</v>
+        <v>1.7029928219342862</v>
       </c>
       <c r="W16" s="2">
         <f t="shared" si="2"/>
-        <v>2.1459017036465626</v>
+        <v>2.0700678582168588</v>
       </c>
       <c r="X16" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.50984099860374088</v>
+        <v>0.7733382623681041</v>
       </c>
       <c r="Y16" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.50984099860374088</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>7.0790907609581293</v>
       </c>
       <c r="Z16" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>7.3384226820922347</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>4.0363206534320453</v>
       </c>
       <c r="AA16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.2087902944413134</v>
+        <v>1.1660729527337146</v>
       </c>
       <c r="AB16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.0504000000000002</v>
+        <v>1.0132800000000002</v>
       </c>
       <c r="AC16">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>4.5011235955056188</v>
+        <v>2.523595505617978</v>
       </c>
       <c r="AD16">
         <f t="shared" si="3"/>
-        <v>7.5011235955056188</v>
+        <v>5.523595505617978</v>
       </c>
       <c r="AE16" s="2"/>
     </row>
@@ -4503,11 +4504,11 @@
       </c>
       <c r="P17" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>405.71428571428567</v>
+        <v>454.22740524781335</v>
       </c>
       <c r="Q17" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>175.62682215743439</v>
+        <v>96.909620991253632</v>
       </c>
       <c r="R17" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4519,43 +4520,43 @@
       </c>
       <c r="U17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.66323160258950964</v>
+        <v>0.36596644206632301</v>
       </c>
       <c r="V17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5321266569780239</v>
+        <v>1.7153300744263875</v>
       </c>
       <c r="W17" s="2">
         <f t="shared" si="2"/>
-        <v>2.1953582595675334</v>
+        <v>2.0812965164927104</v>
       </c>
       <c r="X17" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.47122032853305129</v>
+        <v>0.71475756374686195</v>
       </c>
       <c r="Y17" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.47122032853305129</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>7.7008310249307526</v>
       </c>
       <c r="Z17" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>8.1228613328988146</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.7305676663583904</v>
       </c>
       <c r="AA17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.3380035966395574</v>
+        <v>1.2684864589204712</v>
       </c>
       <c r="AB17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.16268221574344</v>
+        <v>1.102274052478134</v>
       </c>
       <c r="AC17">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>4.7545382794001574</v>
+        <v>2.6235201262825569</v>
       </c>
       <c r="AD17">
         <f t="shared" si="3"/>
-        <v>7.7545382794001574</v>
+        <v>5.6235201262825569</v>
       </c>
       <c r="AE17" s="2"/>
     </row>
@@ -4618,11 +4619,11 @@
       </c>
       <c r="P18" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>447.15428571428572</v>
+        <v>492.28454810495629</v>
       </c>
       <c r="Q18" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>191.27253644314868</v>
+        <v>104.09819241982507</v>
       </c>
       <c r="R18" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4634,43 +4635,43 @@
       </c>
       <c r="U18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.67211316323599912</v>
+        <v>0.36579096348855095</v>
       </c>
       <c r="V18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.5712568412313095</v>
+        <v>1.7298402112075837</v>
       </c>
       <c r="W18" s="2">
         <f t="shared" si="2"/>
-        <v>2.2433700044673088</v>
+        <v>2.0956311746961345</v>
       </c>
       <c r="X18" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.43846954426606577</v>
+        <v>0.66508043957366803</v>
       </c>
       <c r="Y18" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.43846954426606577</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>8.3330324262669109</v>
       </c>
       <c r="Z18" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>8.9204986149584542</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.4712855228764892</v>
       </c>
       <c r="AA18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.4693909869286308</v>
+        <v>1.3726231312236625</v>
       </c>
       <c r="AB18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.2768536443148688</v>
+        <v>1.1927654810495627</v>
       </c>
       <c r="AC18">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.0055299539170512</v>
+        <v>2.7242103335673087</v>
       </c>
       <c r="AD18">
         <f t="shared" si="3"/>
-        <v>8.0055299539170512</v>
+        <v>5.7242103335673082</v>
       </c>
       <c r="AE18" s="2"/>
     </row>
@@ -4733,11 +4734,11 @@
       </c>
       <c r="P19" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>489.00571428571425</v>
+        <v>530.71953352769674</v>
       </c>
       <c r="Q19" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>207.07358600583089</v>
+        <v>111.35813411078716</v>
       </c>
       <c r="R19" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4749,43 +4750,43 @@
       </c>
       <c r="U19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.68121173848407879</v>
+        <v>0.36633580165949536</v>
       </c>
       <c r="V19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6086862606795251</v>
+        <v>1.745912566905957</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="2"/>
-        <v>2.2898979991636041</v>
+        <v>2.1122483685654525</v>
       </c>
       <c r="X19" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.41049423997551571</v>
+        <v>0.62264687054230095</v>
       </c>
       <c r="Y19" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.41049423997551571</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>8.9715105100211883</v>
       </c>
       <c r="Z19" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>9.726055075769926</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.2498100063856015</v>
       </c>
       <c r="AA19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.602082830072201</v>
+        <v>1.4777937031967143</v>
       </c>
       <c r="AB19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.3921586005830904</v>
+        <v>1.2841553352769679</v>
       </c>
       <c r="AC19">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.2529538798331501</v>
+        <v>2.8248853652042714</v>
       </c>
       <c r="AD19">
         <f t="shared" si="3"/>
-        <v>8.2529538798331501</v>
+        <v>5.8248853652042714</v>
       </c>
       <c r="AE19" s="2"/>
     </row>
@@ -4848,11 +4849,11 @@
       </c>
       <c r="P20" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>530.99428571428575</v>
+        <v>569.28046647230326</v>
       </c>
       <c r="Q20" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>222.92641399416908</v>
+        <v>118.64186588921282</v>
       </c>
       <c r="R20" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4864,43 +4865,43 @@
       </c>
       <c r="U20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.69041263054278912</v>
+        <v>0.3674389286287929</v>
       </c>
       <c r="V20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6445119940465125</v>
+        <v>1.7630859319526369</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" si="2"/>
-        <v>2.3349246245893016</v>
+        <v>2.1305248605814295</v>
       </c>
       <c r="X20" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.38645314574160849</v>
+        <v>0.58618079956881364</v>
       </c>
       <c r="Y20" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.38645314574160849</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>9.6120808212481741</v>
       </c>
       <c r="Z20" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>10.53425126283201</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>3.059480932315108</v>
       </c>
       <c r="AA20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.7352094908339373</v>
+        <v>1.5833089083930538</v>
       </c>
       <c r="AB20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.5078413994169098</v>
+        <v>1.375844664723032</v>
       </c>
       <c r="AC20">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.4957709225771207</v>
+        <v>2.9248598453267403</v>
       </c>
       <c r="AD20">
         <f t="shared" si="3"/>
-        <v>8.4957709225771207</v>
+        <v>5.9248598453267398</v>
       </c>
       <c r="AE20" s="2"/>
     </row>
@@ -4963,11 +4964,11 @@
       </c>
       <c r="P21" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>572.84571428571428</v>
+        <v>607.71545189504377</v>
       </c>
       <c r="Q21" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>238.72746355685129</v>
+        <v>125.90180758017492</v>
       </c>
       <c r="R21" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4979,43 +4980,43 @@
       </c>
       <c r="U21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.69962734261529058</v>
+        <v>0.368974502369321</v>
       </c>
       <c r="V21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6788119759787488</v>
+        <v>1.7810030749743528</v>
       </c>
       <c r="W21" s="2">
         <f t="shared" si="2"/>
-        <v>2.3784393185940393</v>
+        <v>2.149977577343674</v>
       </c>
       <c r="X21" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.36569080400957893</v>
+        <v>0.55468801393228651</v>
       </c>
       <c r="Y21" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.36569080400957893</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>10.250558905002451</v>
       </c>
       <c r="Z21" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>11.339807723643482</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.8951091595935918</v>
       </c>
       <c r="AA21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.8679013339775077</v>
+        <v>1.6884794803661056</v>
       </c>
       <c r="AB21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.6231463556851311</v>
+        <v>1.4672345189504372</v>
       </c>
       <c r="AC21">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.7330159352507906</v>
+        <v>3.0235191979163747</v>
       </c>
       <c r="AD21">
         <f t="shared" si="3"/>
-        <v>8.7330159352507906</v>
+        <v>6.0235191979163751</v>
       </c>
       <c r="AE21" s="2"/>
     </row>
@@ -5078,11 +5079,11 @@
       </c>
       <c r="P22" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>614.28571428571422</v>
+        <v>645.77259475218648</v>
       </c>
       <c r="Q22" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>254.37317784256558</v>
+        <v>133.09037900874634</v>
       </c>
       <c r="R22" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5094,43 +5095,43 @@
       </c>
       <c r="U22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.70878487059091111</v>
+        <v>0.37084274318023031</v>
       </c>
       <c r="V22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7116443808997706</v>
+        <v>1.7993793562852356</v>
       </c>
       <c r="W22" s="2">
         <f t="shared" si="2"/>
-        <v>2.4204292514906816</v>
+        <v>2.170222099465466</v>
       </c>
       <c r="X22" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.34769045800906584</v>
+        <v>0.52738468537262984</v>
       </c>
       <c r="Y22" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.34769045800906584</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>10.882760306338607</v>
       </c>
       <c r="Z22" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>12.137445005703121</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.7526036166306516</v>
       </c>
       <c r="AA22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.9992887242665804</v>
+        <v>1.7926161526692967</v>
       </c>
       <c r="AB22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.7373177842565597</v>
+        <v>1.5577259475218657</v>
       </c>
       <c r="AC22">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>5.9637730690362263</v>
+        <v>3.1203007518796988</v>
       </c>
       <c r="AD22">
         <f t="shared" si="3"/>
-        <v>8.9637730690362254</v>
+        <v>6.1203007518796984</v>
       </c>
       <c r="AE22" s="2"/>
     </row>
@@ -5193,11 +5194,11 @@
       </c>
       <c r="P23" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>655.04</v>
+        <v>683.2</v>
       </c>
       <c r="Q23" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>269.76</v>
+        <v>140.16</v>
       </c>
       <c r="R23" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5209,43 +5210,43 @@
       </c>
       <c r="U23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.7178255760486385</v>
+        <v>0.37296275481530683</v>
       </c>
       <c r="V23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7430473952213084</v>
+        <v>1.817980551439909</v>
       </c>
       <c r="W23" s="2">
         <f t="shared" si="2"/>
-        <v>2.4608729712699469</v>
+        <v>2.1909433062552157</v>
       </c>
       <c r="X23" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.33204047323872954</v>
+        <v>0.50364643744528781</v>
       </c>
       <c r="Y23" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.33204047323872954</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>11.504500570311237</v>
       </c>
       <c r="Z23" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>12.921883656509703</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.6287054661731561</v>
       </c>
       <c r="AA23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.1285020264648251</v>
+        <v>1.8950296588560538</v>
       </c>
       <c r="AB23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.8495999999999999</v>
+        <v>1.6467200000000002</v>
       </c>
       <c r="AC23">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.187155963302752</v>
+        <v>3.2146788990825685</v>
       </c>
       <c r="AD23">
         <f t="shared" si="3"/>
-        <v>9.187155963302752</v>
+        <v>6.2146788990825685</v>
       </c>
       <c r="AE23" s="2"/>
     </row>
@@ -5308,11 +5309,11 @@
       </c>
       <c r="P24" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>694.83428571428567</v>
+        <v>719.74577259475211</v>
       </c>
       <c r="Q24" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>284.78437317784255</v>
+        <v>147.06309037900871</v>
       </c>
       <c r="R24" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5324,43 +5325,43 @@
       </c>
       <c r="U24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.72669674980631738</v>
+        <v>0.37526732454578832</v>
       </c>
       <c r="V24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7730390591594845</v>
+        <v>1.8366067905868428</v>
       </c>
       <c r="W24" s="2">
         <f t="shared" si="2"/>
-        <v>2.4997358089658017</v>
+        <v>2.2118741151326313</v>
       </c>
       <c r="X24" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.31841000967752164</v>
+        <v>0.48297144458562402</v>
       </c>
       <c r="Y24" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.31841000967752164</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>12.111595241974912</v>
       </c>
       <c r="Z24" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>13.68784422356201</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.5207955065217629</v>
       </c>
       <c r="AA24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.2546716053359095</v>
+        <v>1.9950307324798022</v>
       </c>
       <c r="AB24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>1.9592373177842564</v>
+        <v>1.7336177259475218</v>
       </c>
       <c r="AC24">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.4022913771858532</v>
+        <v>3.3061531604750534</v>
       </c>
       <c r="AD24">
         <f t="shared" si="3"/>
-        <v>9.4022913771858541</v>
+        <v>6.3061531604750538</v>
       </c>
       <c r="AE24" s="2"/>
     </row>
@@ -5423,11 +5424,11 @@
       </c>
       <c r="P25" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>733.39428571428573</v>
+        <v>755.15801749271134</v>
       </c>
       <c r="Q25" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>299.34274052478133</v>
+        <v>153.75206997084547</v>
       </c>
       <c r="R25" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5439,43 +5440,43 @@
       </c>
       <c r="U25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.73534928988137382</v>
+        <v>0.37769907255022483</v>
       </c>
       <c r="V25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8016169901351289</v>
+        <v>1.8550806040526644</v>
       </c>
       <c r="W25" s="2">
         <f t="shared" si="2"/>
-        <v>2.5369662800165029</v>
+        <v>2.2327796766028891</v>
       </c>
       <c r="X25" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.30653113689430761</v>
+        <v>0.46495330390603856</v>
       </c>
       <c r="Y25" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.30653113689430761</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>12.699859866384234</v>
       </c>
       <c r="Z25" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>14.430047254358817</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.426752580029607</v>
       </c>
       <c r="AA25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.3769278256435031</v>
+        <v>2.0919301070939689</v>
       </c>
       <c r="AB25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.0654740524781343</v>
+        <v>1.8178201749271137</v>
       </c>
       <c r="AC25">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.6083052287413429</v>
+        <v>3.3942383441031843</v>
       </c>
       <c r="AD25">
         <f t="shared" si="3"/>
-        <v>9.6083052287413437</v>
+        <v>6.3942383441031847</v>
       </c>
       <c r="AE25" s="2"/>
     </row>
@@ -5538,11 +5539,11 @@
       </c>
       <c r="P26" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>770.4457142857143</v>
+        <v>789.18483965014582</v>
       </c>
       <c r="Q26" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>313.33154518950437</v>
+        <v>160.1793586005831</v>
       </c>
       <c r="R26" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5554,43 +5555,43 @@
       </c>
       <c r="U26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.74373511169537709</v>
+        <v>0.38020753093355969</v>
       </c>
       <c r="V26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8287578705902487</v>
+        <v>1.8732377377148948</v>
       </c>
       <c r="W26" s="2">
         <f t="shared" si="2"/>
-        <v>2.5724929822856257</v>
+        <v>2.2534452686484543</v>
       </c>
       <c r="X26" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.29618551368721419</v>
+        <v>0.44926083057415761</v>
       </c>
       <c r="Y26" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.29618551368721419</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>13.265109988593785</v>
       </c>
       <c r="Z26" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.143213296398901</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.3448481181723282</v>
       </c>
       <c r="AA26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.4944010521512734</v>
+        <v>2.1850385162519794</v>
       </c>
       <c r="AB26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.1675545189504373</v>
+        <v>1.8987283965014579</v>
       </c>
       <c r="AC26">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.8043102793324381</v>
+        <v>3.4784562007749389</v>
       </c>
       <c r="AD26">
         <f t="shared" si="3"/>
-        <v>9.8043102793324373</v>
+        <v>6.4784562007749393</v>
       </c>
       <c r="AE26" s="2"/>
     </row>
@@ -5653,11 +5654,11 @@
       </c>
       <c r="P27" s="5">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>805.71428571428567</v>
+        <v>821.57434402332353</v>
       </c>
       <c r="Q27" s="5">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>326.64723032069969</v>
+        <v>166.29737609329445</v>
       </c>
       <c r="R27" s="5">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5669,43 +5670,43 @@
       </c>
       <c r="U27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.75180502992726195</v>
+        <v>0.38274686636068384</v>
       </c>
       <c r="V27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8544166196956275</v>
+        <v>1.8909198271465761</v>
       </c>
       <c r="W27" s="12">
         <f t="shared" si="2"/>
-        <v>2.6062216496228894</v>
+        <v>2.27366669350726</v>
       </c>
       <c r="X27" s="12">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.28719435273908256</v>
+        <v>0.43562283597713175</v>
       </c>
       <c r="Y27" s="12">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.28719435273908256</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>13.803161153658147</v>
       </c>
       <c r="Z27" s="12">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.822062897181041</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.27366669350726</v>
       </c>
       <c r="AA27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.6062216496228894</v>
+        <v>2.27366669350726</v>
       </c>
       <c r="AB27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.2647230320699707</v>
+        <v>1.9757434402332359</v>
       </c>
       <c r="AC27" s="13">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>6.9893948845913902</v>
+        <v>3.5583281347473483</v>
       </c>
       <c r="AD27" s="13">
         <f t="shared" si="3"/>
-        <v>9.9893948845913911</v>
+        <v>6.5583281347473488</v>
       </c>
       <c r="AE27" s="12"/>
     </row>
@@ -5768,11 +5769,11 @@
       </c>
       <c r="P28" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>838.92571428571432</v>
+        <v>852.07463556851314</v>
       </c>
       <c r="Q28" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>339.1862390670554</v>
+        <v>172.05854227405248</v>
       </c>
       <c r="R28" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5784,43 +5785,43 @@
       </c>
       <c r="U28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.7595069284369339</v>
+        <v>0.38527404682849542</v>
       </c>
       <c r="V28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8785251848555637</v>
+        <v>1.9079682921090488</v>
       </c>
       <c r="W28" s="2">
         <f t="shared" si="2"/>
-        <v>2.6380321132924975</v>
+        <v>2.293242338937544</v>
       </c>
       <c r="X28" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.27941078438723144</v>
+        <v>0.4238165449163333</v>
       </c>
       <c r="Y28" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.27941078438723144</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>14.309828906631916</v>
       </c>
       <c r="Z28" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.461316604204022</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.2120455649946145</v>
       </c>
       <c r="AA28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.7115199828220202</v>
+        <v>2.3571253724132375</v>
       </c>
       <c r="AB28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.3562239067055395</v>
+        <v>2.048266355685131</v>
       </c>
       <c r="AC28">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.1626123574753118</v>
+        <v>3.6333686310242079</v>
       </c>
       <c r="AD28">
         <f t="shared" si="3"/>
-        <v>10.162612357475311</v>
+        <v>6.6333686310242079</v>
       </c>
       <c r="AE28" s="2"/>
     </row>
@@ -5883,11 +5884,11 @@
       </c>
       <c r="P29" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>869.80571428571432</v>
+        <v>880.43381924198252</v>
       </c>
       <c r="Q29" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>350.84501457725946</v>
+        <v>177.41527696793003</v>
       </c>
       <c r="R29" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5899,43 +5900,43 @@
       </c>
       <c r="U29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.76678408355067884</v>
+        <v>0.38774730979620897</v>
       </c>
       <c r="V29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9009908928001755</v>
+        <v>1.9242189889114798</v>
       </c>
       <c r="W29" s="2">
         <f t="shared" si="2"/>
-        <v>2.6677749763508545</v>
+        <v>2.3119662987076888</v>
       </c>
       <c r="X29" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.27271399709330718</v>
+        <v>0.41365870774059582</v>
       </c>
       <c r="Y29" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.27271399709330718</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>14.78092879256967</v>
       </c>
       <c r="Z29" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>17.055694964966609</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.1590282891377619</v>
       </c>
       <c r="AA29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.8094264165123333</v>
+        <v>2.4347252865233378</v>
       </c>
       <c r="AB29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.4413014577259475</v>
+        <v>2.115698192419825</v>
       </c>
       <c r="AC29">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.3229705717693445</v>
+        <v>3.7030791324878902</v>
       </c>
       <c r="AD29">
         <f t="shared" si="3"/>
-        <v>10.322970571769345</v>
+        <v>6.7030791324878898</v>
       </c>
       <c r="AE29" s="2"/>
     </row>
@@ -5998,11 +5999,11 @@
       </c>
       <c r="P30" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>898.08000000000015</v>
+        <v>906.40000000000009</v>
       </c>
       <c r="Q30" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>361.52000000000004</v>
+        <v>182.32000000000002</v>
       </c>
       <c r="R30" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6014,43 +6015,43 @@
       </c>
       <c r="U30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.77357353656114991</v>
+        <v>0.39012482624980321</v>
       </c>
       <c r="V30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9216942955157048</v>
+        <v>1.9394972713515886</v>
       </c>
       <c r="W30" s="2">
         <f t="shared" si="2"/>
-        <v>2.6952678320768548</v>
+        <v>2.3296220976013919</v>
       </c>
       <c r="X30" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.26700471160007611</v>
+        <v>0.4049987354457229</v>
       </c>
       <c r="Y30" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.26700471160007611</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>15.212276356526001</v>
       </c>
       <c r="Z30" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>17.599918526967588</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.1138288896862099</v>
       </c>
       <c r="AA30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.8990713154574985</v>
+        <v>2.5057771693909872</v>
       </c>
       <c r="AB30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.5192000000000005</v>
+        <v>2.1774400000000003</v>
       </c>
       <c r="AC30">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.4694214876033067</v>
+        <v>3.766942148760331</v>
       </c>
       <c r="AD30">
         <f t="shared" si="3"/>
-        <v>10.469421487603306</v>
+        <v>6.7669421487603305</v>
       </c>
       <c r="AE30" s="2"/>
     </row>
@@ -6113,11 +6114,11 @@
       </c>
       <c r="P31" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>923.47428571428577</v>
+        <v>929.72128279883384</v>
       </c>
       <c r="Q31" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>371.10763848396505</v>
+        <v>186.72513119533528</v>
       </c>
       <c r="R31" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6129,43 +6130,43 @@
       </c>
       <c r="U31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.77980442950856621</v>
+        <v>0.39236347977510611</v>
       </c>
       <c r="V31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.940486435361731</v>
+        <v>1.9536131821394538</v>
       </c>
       <c r="W31" s="2">
         <f t="shared" si="2"/>
-        <v>2.7202908648702975</v>
+        <v>2.3459766619145599</v>
       </c>
       <c r="X31" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.26220166988058935</v>
+        <v>0.3977133740338285</v>
       </c>
       <c r="Y31" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.26220166988058935</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>15.599687143555494</v>
       </c>
       <c r="Z31" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>18.088707837705734</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.0758040612696003</v>
       </c>
       <c r="AA31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.9795850444211829</v>
+        <v>2.5695917545696112</v>
       </c>
       <c r="AB31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.5891638483965016</v>
+        <v>2.232892827988338</v>
       </c>
       <c r="AC31">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.6008503117013406</v>
+        <v>3.824415410705329</v>
       </c>
       <c r="AD31">
         <f t="shared" si="3"/>
-        <v>10.60085031170134</v>
+        <v>6.8244154107053294</v>
       </c>
       <c r="AE31" s="2"/>
     </row>
@@ -6228,11 +6229,11 @@
       </c>
       <c r="P32" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>945.71428571428578</v>
+        <v>950.1457725947522</v>
       </c>
       <c r="Q32" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>379.50437317784258</v>
+        <v>190.58309037900875</v>
       </c>
       <c r="R32" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6244,43 +6245,43 @@
       </c>
       <c r="U32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.78539622778119689</v>
+        <v>0.39441769539876192</v>
       </c>
       <c r="V32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9571854372563928</v>
+        <v>1.9663565386332647</v>
       </c>
       <c r="W32" s="2">
         <f t="shared" si="2"/>
-        <v>2.7425816650375898</v>
+        <v>2.3607742340320268</v>
       </c>
       <c r="X32" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25823890719086751</v>
+        <v>0.39170256670166165</v>
       </c>
       <c r="Y32" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25823890719086751</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>15.938976698712738</v>
       </c>
       <c r="Z32" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>18.516783444679824</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.0444315727232136</v>
       </c>
       <c r="AA32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.0500979681670559</v>
+        <v>2.6254797756126362</v>
       </c>
       <c r="AB32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.6504373177842568</v>
+        <v>2.2814577259475217</v>
       </c>
       <c r="AC32">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.7160640189685834</v>
+        <v>3.8749259039715471</v>
       </c>
       <c r="AD32">
         <f t="shared" si="3"/>
-        <v>10.716064018968584</v>
+        <v>6.8749259039715476</v>
       </c>
       <c r="AE32" s="2"/>
     </row>
@@ -6343,11 +6344,11 @@
       </c>
       <c r="P33" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>964.52571428571434</v>
+        <v>967.42157434402338</v>
       </c>
       <c r="Q33" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>386.60664723032073</v>
+        <v>193.8462973760933</v>
       </c>
       <c r="R33" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6359,43 +6360,43 @@
       </c>
       <c r="U33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.79025675592540023</v>
+        <v>0.39623826235279402</v>
       </c>
       <c r="V33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9715723137164893</v>
+        <v>1.9774916971303236</v>
       </c>
       <c r="W33" s="2">
         <f t="shared" si="2"/>
-        <v>2.7618290696418897</v>
+        <v>2.3737299594831178</v>
       </c>
       <c r="X33" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.2550636377578398</v>
+        <v>0.38688624680464861</v>
       </c>
       <c r="Y33" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.2550636377578398</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.225960567052319</v>
       </c>
       <c r="Z33" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>18.878865895388643</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.0192935284548232</v>
       </c>
       <c r="AA33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.1097404514587863</v>
+        <v>2.6727519660734895</v>
       </c>
       <c r="AB33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.7022647230320702</v>
+        <v>2.3225357434402336</v>
       </c>
       <c r="AC33">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.8137789615103594</v>
+        <v>3.9178636245786884</v>
       </c>
       <c r="AD33">
         <f t="shared" si="3"/>
-        <v>10.813778961510359</v>
+        <v>6.917863624578688</v>
       </c>
       <c r="AE33" s="2"/>
     </row>
@@ -6458,11 +6459,11 @@
       </c>
       <c r="P34" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>979.63428571428562</v>
+        <v>981.29679300291536</v>
       </c>
       <c r="Q34" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>392.31090379008742</v>
+        <v>196.4671720116618</v>
       </c>
       <c r="R34" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6474,43 +6475,43 @@
       </c>
       <c r="U34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.79427997043334286</v>
+        <v>0.39777109957678458</v>
       </c>
       <c r="V34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9833858400962756</v>
+        <v>1.9867517833502122</v>
       </c>
       <c r="W34" s="2">
         <f t="shared" si="2"/>
-        <v>2.7776658105296184</v>
+        <v>2.3845228829269969</v>
       </c>
       <c r="X34" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25263462974973644</v>
+        <v>0.38320187297553482</v>
       </c>
       <c r="Y34" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25263462974973644</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.45645429362882</v>
       </c>
       <c r="Z34" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>19.169675737330955</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>2.0000635033738479</v>
       </c>
       <c r="AA34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.1576428590600418</v>
+        <v>2.7107190595055961</v>
       </c>
       <c r="AB34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.7438903790087461</v>
+        <v>2.3555279300291545</v>
       </c>
       <c r="AC34">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.8926072777608329</v>
+        <v>3.9525749008751143</v>
       </c>
       <c r="AD34">
         <f t="shared" si="3"/>
-        <v>10.892607277760833</v>
+        <v>6.9525749008751143</v>
       </c>
       <c r="AE34" s="2"/>
     </row>
@@ -6573,11 +6574,11 @@
       </c>
       <c r="P35" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>990.76571428571435</v>
+        <v>991.51953352769681</v>
       </c>
       <c r="Q35" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>396.51358600583092</v>
+        <v>198.39813411078717</v>
       </c>
       <c r="R35" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6589,43 +6590,43 @@
       </c>
       <c r="U35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.79734338563108109</v>
+        <v>0.3989559135874301</v>
       </c>
       <c r="V35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9923163212474411</v>
+        <v>1.9938321653641853</v>
       </c>
       <c r="W35" s="2">
         <f t="shared" si="2"/>
-        <v>2.7896597068785223</v>
+        <v>2.3927880789516154</v>
       </c>
       <c r="X35" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25092097848338069</v>
+        <v>0.38060256829768868</v>
       </c>
       <c r="Y35" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.25092097848338069</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.626273423496833</v>
       </c>
       <c r="Z35" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>19.383933518005556</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.9864968305913253</v>
       </c>
       <c r="AA35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.1929355557344929</v>
+        <v>2.7386917894623828</v>
       </c>
       <c r="AB35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.7745586005830907</v>
+        <v>2.3798353352769679</v>
       </c>
       <c r="AC35">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.9510417884619891</v>
+        <v>3.9783551200804435</v>
       </c>
       <c r="AD35">
         <f t="shared" si="3"/>
-        <v>10.951041788461989</v>
+        <v>6.9783551200804439</v>
       </c>
       <c r="AE35" s="2"/>
     </row>
@@ -6688,11 +6689,11 @@
       </c>
       <c r="P36" s="2">
         <f>P$39 + ((P$40 - P$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>997.64571428571435</v>
+        <v>997.83790087463558</v>
       </c>
       <c r="Q36" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>399.11113702623908</v>
+        <v>199.59160349854227</v>
       </c>
       <c r="R36" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6704,43 +6705,43 @@
       </c>
       <c r="U36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.79930505602560964</v>
+        <v>0.39972469574597513</v>
       </c>
       <c r="V36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9979980250423997</v>
+        <v>1.9983829196193079</v>
       </c>
       <c r="W36" s="2">
         <f t="shared" si="2"/>
-        <v>2.7973030810680095</v>
+        <v>2.3981076153652832</v>
       </c>
       <c r="X36" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.24990121194894377</v>
+        <v>0.3790557635449866</v>
       </c>
       <c r="Y36" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.24990121194894377</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.731233501710946</v>
       </c>
       <c r="Z36" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>19.516359784911209</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.9784235200182265</v>
       </c>
       <c r="AA36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.2147489062458061</v>
+        <v>2.7559808894972755</v>
       </c>
       <c r="AB36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.793513702623907</v>
+        <v>2.3948590087463555</v>
       </c>
       <c r="AC36">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>7.9874390272364471</v>
+        <v>3.9944406842952835</v>
       </c>
       <c r="AD36">
         <f t="shared" si="3"/>
-        <v>10.987439027236448</v>
+        <v>6.9944406842952835</v>
       </c>
       <c r="AE36" s="2"/>
     </row>
@@ -6807,7 +6808,7 @@
       </c>
       <c r="Q37" s="2">
         <f>Q$39 + ((Q$40 - Q$39) * ((Table1[[#This Row],[Smooth Step]]) / (1)))</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="R37" s="2">
         <f>R$39 + ((R$40 - R$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6819,7 +6820,7 @@
       </c>
       <c r="U37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="V37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
@@ -6827,35 +6828,35 @@
       </c>
       <c r="W37" s="2">
         <f t="shared" si="2"/>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="X37" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.2495626822157434</v>
+        <v>0.37854227405247809</v>
       </c>
       <c r="Y37" s="2">
-        <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.2495626822157434</v>
+        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
+        <v>16.767150073325741</v>
       </c>
       <c r="Z37" s="2">
-        <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>19.561675085546696</v>
+        <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
+        <v>1.9757434402332359</v>
       </c>
       <c r="AA37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>3.2222132753576509</v>
+        <v>2.761897093163701</v>
       </c>
       <c r="AB37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="AC37">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]]/Table2[[#This Row],[Shield Regen]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AD37">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AE37" s="2"/>
     </row>
@@ -6888,7 +6889,7 @@
         <v>3</v>
       </c>
       <c r="P39" s="9">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q39" s="9">
         <v>30</v>
@@ -6932,7 +6933,7 @@
         <v>1000</v>
       </c>
       <c r="Q40" s="11">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="R40" s="11">
         <v>50</v>

</xml_diff>

<commit_message>
Made some playtesting tweaks
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -2268,19 +2268,19 @@
     <tableColumn id="3" name="Time to Kill" dataDxfId="6">
       <calculatedColumnFormula>U2 + V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Time to Kill Vanilla" dataDxfId="2">
+    <tableColumn id="8" name="Time to Kill Vanilla" dataDxfId="5">
       <calculatedColumnFormula xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Time for Vanilla to Kill" dataDxfId="0">
+    <tableColumn id="12" name="Time for Vanilla to Kill" dataDxfId="4">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Time to Kill StatMax" dataDxfId="1">
+    <tableColumn id="11" name="Time to Kill StatMax" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Time for StatMax to Kill" dataDxfId="5">
+    <tableColumn id="9" name="Time for StatMax to Kill" dataDxfId="2">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Time for AbsMax to Kill" dataDxfId="4">
+    <tableColumn id="10" name="Time for AbsMax to Kill" dataDxfId="1">
       <calculatedColumnFormula xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Time to Regen Shield">
@@ -2289,7 +2289,7 @@
     <tableColumn id="5" name="Time to Regen after Combat">
       <calculatedColumnFormula>AC2 + $U$43</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Time to Top Speed" dataDxfId="3"/>
+    <tableColumn id="6" name="Time to Top Speed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2594,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="L2" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M2" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2795,31 +2795,31 @@
       </c>
       <c r="U2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>16.666666666666668</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="W2" s="2">
         <f>U2 + V2</f>
-        <v>21.666666666666668</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="X2" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>31.545189504373177</v>
+        <v>6.3090379008746353</v>
       </c>
       <c r="Y2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.816441257943622</v>
+        <v>1.2984857309260345</v>
       </c>
       <c r="Z2" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>164.64528668610302</v>
+        <v>32.929057337220598</v>
       </c>
       <c r="AA2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.29920551842606757</v>
+        <v>0.29502448061400022</v>
       </c>
       <c r="AB2" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="L3" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>4.7036734693877555</v>
+        <v>12.253061224489796</v>
       </c>
       <c r="M3" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -2910,31 +2910,31 @@
       </c>
       <c r="U3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9046183225287703</v>
+        <v>0.73113995832183709</v>
       </c>
       <c r="V3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>6.3988841323100258</v>
+        <v>2.4563870999580528</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" ref="W3:W37" si="2">U3 + V3</f>
-        <v>8.3035024548387959</v>
+        <v>3.18752705827989</v>
       </c>
       <c r="X3" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>11.854925513377438</v>
+        <v>4.5508381617642106</v>
       </c>
       <c r="Y3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.8523578295584175</v>
+        <v>1.324160745486314</v>
       </c>
       <c r="Z3" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>61.874968591386498</v>
+        <v>23.752402999571551</v>
       </c>
       <c r="AA3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.30512172209249266</v>
+        <v>0.30085801243879839</v>
       </c>
       <c r="AB3" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="L4" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>7.3289795918367346</v>
+        <v>14.440816326530612</v>
       </c>
       <c r="M4" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3025,31 +3025,31 @@
       </c>
       <c r="U4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.141578556963416</v>
+        <v>0.57937209069630013</v>
       </c>
       <c r="V4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>3.9187234958946546</v>
+        <v>1.9888241688039687</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="2"/>
-        <v>5.0603020528580709</v>
+        <v>2.5681962595002688</v>
       </c>
       <c r="X4" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>6.8371871534013717</v>
+        <v>3.4699980928907586</v>
       </c>
       <c r="Y4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>1.9573179077725287</v>
+        <v>1.3991916132789757</v>
       </c>
       <c r="Z4" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>35.68565149504807</v>
+        <v>18.111123749154412</v>
       </c>
       <c r="AA4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.32241082212738548</v>
+        <v>0.31790551806272327</v>
       </c>
       <c r="AB4" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="L5" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>9.8759183673469426</v>
+        <v>16.563265306122453</v>
       </c>
       <c r="M5" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3140,31 +3140,31 @@
       </c>
       <c r="U5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.81845370247660587</v>
+        <v>0.48800654965805706</v>
       </c>
       <c r="V5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.8972527845369322</v>
+        <v>1.7274994670935342</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="2"/>
-        <v>3.7157064870135379</v>
+        <v>2.2155060167515912</v>
       </c>
       <c r="X5" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.6196420691077931</v>
+        <v>2.7544815057696441</v>
       </c>
       <c r="Y5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.1271370376405425</v>
+        <v>1.5205870704717539</v>
       </c>
       <c r="Z5" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>24.111514459280418</v>
+        <v>14.376594476509339</v>
       </c>
       <c r="AA5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.35038355208417205</v>
+        <v>0.34548736271007008</v>
       </c>
       <c r="AB5" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="L6" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>12.344489795918369</v>
+        <v>18.620408163265306</v>
       </c>
       <c r="M6" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3255,31 +3255,31 @@
       </c>
       <c r="U6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.6495920212269316</v>
+        <v>0.43065017733422456</v>
       </c>
       <c r="V6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.3821042173423788</v>
+        <v>1.5792275306730144</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="2"/>
-        <v>3.0316962385693103</v>
+        <v>2.009877708007239</v>
       </c>
       <c r="X6" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.4007310880378236</v>
+        <v>2.254531149202454</v>
       </c>
       <c r="Y6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.3576307642170455</v>
+        <v>1.6853558532323829</v>
       </c>
       <c r="Z6" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>17.74959522290105</v>
+        <v>11.767180138566845</v>
       </c>
       <c r="AA6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.38835064551627879</v>
+        <v>0.38292391160513428</v>
       </c>
       <c r="AB6" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="L7" s="5">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>14.734693877551013</v>
+        <v>20.612244897959179</v>
       </c>
       <c r="M7" s="5">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3370,31 +3370,31 @@
       </c>
       <c r="U7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.5507576992015647</v>
+        <v>0.39370995923121749</v>
       </c>
       <c r="V7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>2.0938569333550605</v>
+        <v>1.4967967384973797</v>
       </c>
       <c r="W7" s="12">
         <f t="shared" si="2"/>
-        <v>2.6446146325566251</v>
+        <v>1.8905066977285971</v>
       </c>
       <c r="X7" s="12">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.6446146325566251</v>
+        <v>1.8905066977285971</v>
       </c>
       <c r="Y7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.6446146325566251</v>
+        <v>1.8905066977285971</v>
       </c>
       <c r="Z7" s="12">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>13.803161153658147</v>
+        <v>9.8672102504368127</v>
       </c>
       <c r="AA7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.43562283597713175</v>
+        <v>0.42953552997221112</v>
       </c>
       <c r="AB7" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="L8" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>17.046530612244901</v>
+        <v>22.538775510204086</v>
       </c>
       <c r="M8" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3485,31 +3485,31 @@
       </c>
       <c r="U8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.48873554149783316</v>
+        <v>0.36964054971234162</v>
       </c>
       <c r="V8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9230852306569601</v>
+        <v>1.4544681559789439</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="2"/>
-        <v>2.4118207721547931</v>
+        <v>1.8241087056912855</v>
       </c>
       <c r="X8" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.1375808685168862</v>
+        <v>1.6166955340952416</v>
       </c>
       <c r="Y8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>2.9839041877138688</v>
+        <v>2.1330483401281315</v>
       </c>
       <c r="Z8" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>11.156776054963983</v>
+        <v>8.4380948054964833</v>
       </c>
       <c r="AA8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.49151085702015718</v>
+        <v>0.48464258303559599</v>
       </c>
       <c r="AB8" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="L9" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>19.279999999999994</v>
+        <v>24.399999999999995</v>
       </c>
       <c r="M9" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3600,31 +3600,31 @@
       </c>
       <c r="U9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.44801250826868744</v>
+        <v>0.35400332620574976</v>
       </c>
       <c r="V9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8191111912923215</v>
+        <v>1.4373960560703261</v>
       </c>
       <c r="W9" s="2">
         <f t="shared" si="2"/>
-        <v>2.2671236995610089</v>
+        <v>1.7913993822760759</v>
       </c>
       <c r="X9" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.7784361753773448</v>
+        <v>1.4052561254620985</v>
       </c>
       <c r="Y9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.3713149747433624</v>
+        <v>2.4099895165987202</v>
       </c>
       <c r="Z9" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>9.2822753183126832</v>
+        <v>7.3345191859454317</v>
       </c>
       <c r="AA9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.55532544219878144</v>
+        <v>0.54756543601958452</v>
       </c>
       <c r="AB9" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="L10" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>21.435102040816325</v>
+        <v>26.195918367346938</v>
       </c>
       <c r="M10" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3715,31 +3715,31 @@
       </c>
       <c r="U10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.42048096680054753</v>
+        <v>0.34406323547051343</v>
       </c>
       <c r="V10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7557076397555516</v>
+        <v>1.4366273357650754</v>
       </c>
       <c r="W10" s="2">
         <f t="shared" si="2"/>
-        <v>2.1761886065560989</v>
+        <v>1.7806905712355889</v>
       </c>
       <c r="X10" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.513460680123679</v>
+        <v>1.2384060622838129</v>
       </c>
       <c r="Y10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>3.8026625386996931</v>
+        <v>2.718338963308097</v>
       </c>
       <c r="Z10" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>7.8992762916375128</v>
+        <v>6.463670827853468</v>
       </c>
       <c r="AA10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.6263773250664304</v>
+        <v>0.61762445414847156</v>
       </c>
       <c r="AB10" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="L11" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>23.511836734693873</v>
+        <v>27.926530612244896</v>
       </c>
       <c r="M11" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3830,31 +3830,31 @@
       </c>
       <c r="U11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.4015472234043338</v>
+        <v>0.33806966175070502</v>
       </c>
       <c r="V11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7181780646569522</v>
+        <v>1.4465642975226405</v>
       </c>
       <c r="W11" s="2">
         <f t="shared" si="2"/>
-        <v>2.1197252880612858</v>
+        <v>1.7846339592733456</v>
       </c>
       <c r="X11" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.3116911884222815</v>
+        <v>1.1043358552744387</v>
       </c>
       <c r="Y11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>4.2737624246374475</v>
+        <v>3.0551054164239968</v>
       </c>
       <c r="Z11" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>6.8461713229360113</v>
+        <v>5.7639119100614717</v>
       </c>
       <c r="AA11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.70397723917653043</v>
+        <v>0.69414000264655273</v>
       </c>
       <c r="AB11" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="L12" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>25.510204081632651</v>
+        <v>29.591836734693878</v>
       </c>
       <c r="M12" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -3945,31 +3945,31 @@
       </c>
       <c r="U12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.38844444444444448</v>
+        <v>0.33486590038314173</v>
       </c>
       <c r="V12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6977777777777776</v>
+        <v>1.4636015325670495</v>
       </c>
       <c r="W12" s="2">
         <f t="shared" si="2"/>
-        <v>2.0862222222222222</v>
+        <v>1.7984674329501913</v>
       </c>
       <c r="X12" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.1541333333333332</v>
+        <v>0.99494252873563205</v>
       </c>
       <c r="Y12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>4.7804301776112137</v>
+        <v>3.4172976121141541</v>
       </c>
       <c r="Z12" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>6.023822222222222</v>
+        <v>5.1929501915708798</v>
       </c>
       <c r="AA12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.7874359180825079</v>
+        <v>0.77643244673812339</v>
       </c>
       <c r="AB12" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="L13" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>27.430204081632649</v>
+        <v>31.191836734693872</v>
       </c>
       <c r="M13" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4060,31 +4060,31 @@
       </c>
       <c r="U13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37942395535594692</v>
+        <v>0.33366667751558571</v>
       </c>
       <c r="V13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6890523369715054</v>
+        <v>1.4853581948944394</v>
       </c>
       <c r="W13" s="2">
         <f t="shared" si="2"/>
-        <v>2.0684762923274524</v>
+        <v>1.8190248724100251</v>
       </c>
       <c r="X13" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.0285497527069807</v>
+        <v>0.90451004424129744</v>
       </c>
       <c r="Y13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>5.318481342675577</v>
+        <v>3.8019242865463028</v>
       </c>
       <c r="Z13" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>5.3683579514361277</v>
+        <v>4.7209516850080284</v>
       </c>
       <c r="AA13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.87606409533778873</v>
+        <v>0.86382215164747889</v>
       </c>
       <c r="AB13" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="L14" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>29.271836734693874</v>
+        <v>32.726530612244893</v>
       </c>
       <c r="M14" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4175,31 +4175,31 @@
       </c>
       <c r="U14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37333651450445476</v>
+        <v>0.33392618451236566</v>
       </c>
       <c r="V14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6884668705740713</v>
+        <v>1.510228112872164</v>
       </c>
       <c r="W14" s="2">
         <f t="shared" si="2"/>
-        <v>2.0618033850785262</v>
+        <v>1.8441542973845295</v>
       </c>
       <c r="X14" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.92673763821067079</v>
+        <v>0.82890891072482498</v>
       </c>
       <c r="Y14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>5.8837314648851269</v>
+        <v>4.2059941758881791</v>
       </c>
       <c r="Z14" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.8369652084304322</v>
+        <v>4.3263631440234089</v>
       </c>
       <c r="AA14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>0.96917250449579928</v>
+        <v>0.95562948259891467</v>
       </c>
       <c r="AB14" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="L15" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>31.035102040816327</v>
+        <v>34.195918367346941</v>
       </c>
       <c r="M15" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4290,31 +4290,31 @@
       </c>
       <c r="U15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.3694018057630804</v>
+        <v>0.33525705064456407</v>
       </c>
       <c r="V15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.6936560440273698</v>
+        <v>1.5371070776278954</v>
       </c>
       <c r="W15" s="2">
         <f t="shared" si="2"/>
-        <v>2.0630578497904501</v>
+        <v>1.8723641282724595</v>
       </c>
       <c r="X15" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.84301549353399308</v>
+        <v>0.76509341210731319</v>
       </c>
       <c r="Y15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>6.4719960892944481</v>
+        <v>4.6265160163075159</v>
       </c>
       <c r="Z15" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.3999902931154997</v>
+        <v>3.9932879198774183</v>
       </c>
       <c r="AA15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.0660718791099659</v>
+        <v>1.0511748048167262</v>
       </c>
       <c r="AB15" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="L16" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>32.72</v>
+        <v>35.6</v>
       </c>
       <c r="M16" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4405,31 +4405,31 @@
       </c>
       <c r="U16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.36707503628257265</v>
+        <v>0.33737907829117353</v>
       </c>
       <c r="V16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7029928219342862</v>
+        <v>1.5652226161148832</v>
       </c>
       <c r="W16" s="2">
         <f t="shared" si="2"/>
-        <v>2.0700678582168588</v>
+        <v>1.9026016944060569</v>
       </c>
       <c r="X16" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.7733382623681041</v>
+        <v>0.71077606586192033</v>
       </c>
       <c r="Y16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>7.0790907609581293</v>
+        <v>5.0604985439720469</v>
       </c>
       <c r="Z16" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>4.0363206534320453</v>
+        <v>3.709786847761138</v>
       </c>
       <c r="AA16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.1660729527337146</v>
+        <v>1.1497784835252085</v>
       </c>
       <c r="AB16" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="L17" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>34.326530612244902</v>
+        <v>36.938775510204081</v>
       </c>
       <c r="M17" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4520,31 +4520,31 @@
       </c>
       <c r="U17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.36596644206632301</v>
+        <v>0.34008594229588701</v>
       </c>
       <c r="V17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7153300744263875</v>
+        <v>1.5940249641907098</v>
       </c>
       <c r="W17" s="2">
         <f t="shared" si="2"/>
-        <v>2.0812965164927104</v>
+        <v>1.9341109064865969</v>
       </c>
       <c r="X17" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.71475756374686195</v>
+        <v>0.66421117249846529</v>
       </c>
       <c r="Y17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>7.7008310249307526</v>
+        <v>5.5049504950495072</v>
       </c>
       <c r="Z17" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.7305676663583904</v>
+        <v>3.4667485164722729</v>
       </c>
       <c r="AA17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.2684864589204712</v>
+        <v>1.2507608839486566</v>
       </c>
       <c r="AB17" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="L18" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>35.854693877551014</v>
+        <v>38.212244897959181</v>
       </c>
       <c r="M18" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4635,31 +4635,31 @@
       </c>
       <c r="U18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.36579096348855095</v>
+        <v>0.34322304418594601</v>
       </c>
       <c r="V18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7298402112075837</v>
+        <v>1.6231156111228258</v>
       </c>
       <c r="W18" s="2">
         <f t="shared" si="2"/>
-        <v>2.0956311746961345</v>
+        <v>1.9663386553087718</v>
       </c>
       <c r="X18" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.66508043957366803</v>
+        <v>0.62404749128294479</v>
       </c>
       <c r="Y18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>8.3330324262669109</v>
+        <v>5.9568806057076324</v>
       </c>
       <c r="Z18" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.4712855228764892</v>
+        <v>3.2571203318902184</v>
       </c>
       <c r="AA18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.3726231312236625</v>
+        <v>1.3534423713113668</v>
       </c>
       <c r="AB18" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="L19" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>37.304489795918371</v>
+        <v>39.420408163265307</v>
       </c>
       <c r="M19" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4750,31 +4750,31 @@
       </c>
       <c r="U19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.36633580165949536</v>
+        <v>0.34667246767934601</v>
       </c>
       <c r="V19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.745912566905957</v>
+        <v>1.6521994715773125</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="2"/>
-        <v>2.1122483685654525</v>
+        <v>1.9988719392566585</v>
       </c>
       <c r="X19" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.62264687054230095</v>
+        <v>0.58922585814955619</v>
       </c>
       <c r="Y19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>8.9715105100211883</v>
+        <v>6.4132976121141549</v>
       </c>
       <c r="Z19" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.2498100063856015</v>
+        <v>3.0753741493437405</v>
       </c>
       <c r="AA19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.4777937031967143</v>
+        <v>1.4571433108376337</v>
       </c>
       <c r="AB19" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="L20" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>38.675918367346938</v>
+        <v>40.563265306122446</v>
       </c>
       <c r="M20" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4865,31 +4865,31 @@
       </c>
       <c r="U20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.3674389286287929</v>
+        <v>0.35034255505282652</v>
       </c>
       <c r="V20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7630859319526369</v>
+        <v>1.6810522295039654</v>
       </c>
       <c r="W20" s="2">
         <f t="shared" si="2"/>
-        <v>2.1305248605814295</v>
+        <v>2.0313947845567917</v>
       </c>
       <c r="X20" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.58618079956881364</v>
+        <v>0.55890669997929676</v>
       </c>
       <c r="Y20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>9.6120808212481741</v>
+        <v>6.8712102504368122</v>
       </c>
       <c r="Z20" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>3.059480932315108</v>
+        <v>2.9171279454865204</v>
       </c>
       <c r="AA20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.5833089083930538</v>
+        <v>1.5611840677517532</v>
       </c>
       <c r="AB20" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="L21" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>39.968979591836728</v>
+        <v>41.640816326530611</v>
       </c>
       <c r="M21" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -4980,31 +4980,31 @@
       </c>
       <c r="U21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.368974502369321</v>
+        <v>0.35416054861804924</v>
       </c>
       <c r="V21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7810030749743528</v>
+        <v>1.7094975996254509</v>
       </c>
       <c r="W21" s="2">
         <f t="shared" si="2"/>
-        <v>2.149977577343674</v>
+        <v>2.0636581482435004</v>
       </c>
       <c r="X21" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.55468801393228651</v>
+        <v>0.53241785018922971</v>
       </c>
       <c r="Y21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>10.250558905002451</v>
+        <v>7.3276272568433356</v>
       </c>
       <c r="Z21" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.8951091595935918</v>
+        <v>2.7788734497553698</v>
       </c>
       <c r="AA21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.6884794803661056</v>
+        <v>1.6648850072780201</v>
       </c>
       <c r="AB21" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="L22" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>41.183673469387756</v>
+        <v>42.653061224489797</v>
       </c>
       <c r="M22" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5095,31 +5095,31 @@
       </c>
       <c r="U22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37084274318023031</v>
+        <v>0.35806729939603099</v>
       </c>
       <c r="V22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.7993793562852356</v>
+        <v>1.7373911679347396</v>
       </c>
       <c r="W22" s="2">
         <f t="shared" si="2"/>
-        <v>2.170222099465466</v>
+        <v>2.0954584673307703</v>
       </c>
       <c r="X22" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.52738468537262984</v>
+        <v>0.50921640913012778</v>
       </c>
       <c r="Y22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>10.882760306338607</v>
+        <v>7.7795573675014591</v>
       </c>
       <c r="Z22" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.7526036166306516</v>
+        <v>2.6577770805553373</v>
       </c>
       <c r="AA22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.7926161526692967</v>
+        <v>1.7675664946407301</v>
       </c>
       <c r="AB22" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5178,7 +5178,7 @@
       </c>
       <c r="L23" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>42.32</v>
+        <v>43.6</v>
       </c>
       <c r="M23" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5210,31 +5210,31 @@
       </c>
       <c r="U23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37296275481530683</v>
+        <v>0.36201338953632534</v>
       </c>
       <c r="V23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.817980551439909</v>
+        <v>1.7646086453425907</v>
       </c>
       <c r="W23" s="2">
         <f t="shared" si="2"/>
-        <v>2.1909433062552157</v>
+        <v>2.126622034878916</v>
       </c>
       <c r="X23" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.50364643744528781</v>
+        <v>0.48886048698817847</v>
       </c>
       <c r="Y23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>11.504500570311237</v>
+        <v>8.224009318578922</v>
       </c>
       <c r="Z23" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.6287054661731561</v>
+        <v>2.551532461661651</v>
       </c>
       <c r="AA23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.8950296588560538</v>
+        <v>1.8685488950641789</v>
       </c>
       <c r="AB23" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5293,7 +5293,7 @@
       </c>
       <c r="L24" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>43.377959183673468</v>
+        <v>44.481632653061226</v>
       </c>
       <c r="M24" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5325,31 +5325,31 @@
       </c>
       <c r="U24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37526732454578832</v>
+        <v>0.36595623218414569</v>
       </c>
       <c r="V24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8366067905868428</v>
+        <v>1.7910371010865047</v>
       </c>
       <c r="W24" s="2">
         <f t="shared" si="2"/>
-        <v>2.2118741151326313</v>
+        <v>2.1569933332706506</v>
       </c>
       <c r="X24" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.48297144458562402</v>
+        <v>0.47098800921987316</v>
       </c>
       <c r="Y24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>12.111595241974912</v>
+        <v>8.6579918462434513</v>
       </c>
       <c r="Z24" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.5207955065217629</v>
+        <v>2.4582498004322524</v>
       </c>
       <c r="AA24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>1.9950307324798022</v>
+        <v>1.9671525737726605</v>
       </c>
       <c r="AB24" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="L25" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>44.357551020408167</v>
+        <v>45.29795918367347</v>
       </c>
       <c r="M25" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5440,31 +5440,31 @@
       </c>
       <c r="U25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.37769907255022483</v>
+        <v>0.36985785194150511</v>
       </c>
       <c r="V25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8550806040526644</v>
+        <v>1.8165682080197094</v>
       </c>
       <c r="W25" s="2">
         <f t="shared" si="2"/>
-        <v>2.2327796766028891</v>
+        <v>2.1864260599612146</v>
       </c>
       <c r="X25" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.46495330390603856</v>
+        <v>0.455300642055259</v>
       </c>
       <c r="Y25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>12.699859866384234</v>
+        <v>9.078513686662788</v>
       </c>
       <c r="Z25" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.426752580029607</v>
+        <v>2.3763719894332094</v>
       </c>
       <c r="AA25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.0919301070939689</v>
+        <v>2.062697895990472</v>
       </c>
       <c r="AB25" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5523,7 +5523,7 @@
       </c>
       <c r="L26" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>45.258775510204082</v>
+        <v>46.048979591836734</v>
       </c>
       <c r="M26" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5555,31 +5555,31 @@
       </c>
       <c r="U26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.38020753093355969</v>
+        <v>0.37368314004641762</v>
       </c>
       <c r="V26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8732377377148948</v>
+        <v>1.8410928320224995</v>
       </c>
       <c r="W26" s="2">
         <f t="shared" si="2"/>
-        <v>2.2534452686484543</v>
+        <v>2.2147759720689173</v>
       </c>
       <c r="X26" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.44926083057415761</v>
+        <v>0.44155147967900099</v>
       </c>
       <c r="Y26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>13.265109988593785</v>
+        <v>9.4825835760046644</v>
       </c>
       <c r="Z26" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.3448481181723282</v>
+        <v>2.3046103415655068</v>
       </c>
       <c r="AA26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.1850385162519794</v>
+        <v>2.1545052269419083</v>
       </c>
       <c r="AB26" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5638,7 +5638,7 @@
       </c>
       <c r="L27" s="5">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>46.081632653061227</v>
+        <v>46.734693877551024</v>
       </c>
       <c r="M27" s="5">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5670,31 +5670,31 @@
       </c>
       <c r="U27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.38274686636068384</v>
+        <v>0.37739843853380961</v>
       </c>
       <c r="V27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.8909198271465761</v>
+        <v>1.8644964933174535</v>
       </c>
       <c r="W27" s="12">
         <f t="shared" si="2"/>
-        <v>2.27366669350726</v>
+        <v>2.2418949318512631</v>
       </c>
       <c r="X27" s="12">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.43562283597713175</v>
+        <v>0.42953552997221112</v>
       </c>
       <c r="Y27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>13.803161153658147</v>
+        <v>9.8672102504368127</v>
       </c>
       <c r="Z27" s="12">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.27366669350726</v>
+        <v>2.2418949318512631</v>
       </c>
       <c r="AA27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.27366669350726</v>
+        <v>2.2418949318512631</v>
       </c>
       <c r="AB27" s="12">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="L28" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>46.826122448979589</v>
+        <v>47.355102040816327</v>
       </c>
       <c r="M28" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5785,31 +5785,31 @@
       </c>
       <c r="U28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.38527404682849542</v>
+        <v>0.38097034777066291</v>
       </c>
       <c r="V28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9079682921090488</v>
+        <v>1.8866553554897303</v>
       </c>
       <c r="W28" s="2">
         <f t="shared" si="2"/>
-        <v>2.293242338937544</v>
+        <v>2.2676257032603933</v>
       </c>
       <c r="X28" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.4238165449163333</v>
+        <v>0.41908230735202057</v>
       </c>
       <c r="Y28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>14.309828906631916</v>
+        <v>10.229402446126972</v>
       </c>
       <c r="Z28" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.2120455649946145</v>
+        <v>2.1873359368940024</v>
       </c>
       <c r="AA28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.3571253724132375</v>
+        <v>2.3241873759428344</v>
       </c>
       <c r="AB28" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5868,7 +5868,7 @@
       </c>
       <c r="L29" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>47.492244897959182</v>
+        <v>47.910204081632656</v>
       </c>
       <c r="M29" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -5900,31 +5900,31 @@
       </c>
       <c r="U29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.38774730979620897</v>
+        <v>0.38436467863901591</v>
       </c>
       <c r="V29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9242189889114798</v>
+        <v>1.9074324814600794</v>
       </c>
       <c r="W29" s="2">
         <f t="shared" si="2"/>
-        <v>2.3119662987076888</v>
+        <v>2.2917971600990952</v>
       </c>
       <c r="X29" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.41365870774059582</v>
+        <v>0.4100500306514292</v>
       </c>
       <c r="Y29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>14.78092879256967</v>
+        <v>10.566168899242872</v>
       </c>
       <c r="Z29" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.1590282891377619</v>
+        <v>2.1401933516008977</v>
       </c>
       <c r="AA29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.4347252865233378</v>
+        <v>2.4007029244409153</v>
       </c>
       <c r="AB29" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="L30" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>48.08</v>
+        <v>48.4</v>
       </c>
       <c r="M30" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6015,31 +6015,31 @@
       </c>
       <c r="U30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39012482624980321</v>
+        <v>0.38754548855558968</v>
       </c>
       <c r="V30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9394972713515886</v>
+        <v>1.9266741488963717</v>
       </c>
       <c r="W30" s="2">
         <f t="shared" si="2"/>
-        <v>2.3296220976013919</v>
+        <v>2.3142196374519615</v>
       </c>
       <c r="X30" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.4049987354457229</v>
+        <v>0.40232105785599914</v>
       </c>
       <c r="Y30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.212276356526001</v>
+        <v>10.87451834595225</v>
       </c>
       <c r="Z30" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.1138288896862099</v>
+        <v>2.0998531614899374</v>
       </c>
       <c r="AA30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.5057771693909872</v>
+        <v>2.4707619425698026</v>
       </c>
       <c r="AB30" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6098,7 +6098,7 @@
       </c>
       <c r="L31" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>48.589387755102038</v>
+        <v>48.824489795918367</v>
       </c>
       <c r="M31" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6130,31 +6130,31 @@
       </c>
       <c r="U31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39236347977510611</v>
+        <v>0.39047415220153592</v>
       </c>
       <c r="V31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9536131821394538</v>
+        <v>1.9442060496121814</v>
       </c>
       <c r="W31" s="2">
         <f t="shared" si="2"/>
-        <v>2.3459766619145599</v>
+        <v>2.3346802018137174</v>
       </c>
       <c r="X31" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.3977133740338285</v>
+        <v>0.39579828539109746</v>
       </c>
       <c r="Y31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.599687143555494</v>
+        <v>11.151459522422837</v>
       </c>
       <c r="Z31" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.0758040612696003</v>
+        <v>2.0658085493210021</v>
       </c>
       <c r="AA31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.5695917545696112</v>
+        <v>2.5336847955537909</v>
       </c>
       <c r="AB31" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="L32" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.020408163265301</v>
+        <v>49.183673469387756</v>
       </c>
       <c r="M32" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6245,31 +6245,31 @@
       </c>
       <c r="U32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39441769539876192</v>
+        <v>0.39310842504059168</v>
       </c>
       <c r="V32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9663565386332647</v>
+        <v>1.9598292140236933</v>
       </c>
       <c r="W32" s="2">
         <f t="shared" si="2"/>
-        <v>2.3607742340320268</v>
+        <v>2.3529376390642849</v>
       </c>
       <c r="X32" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.39170256670166165</v>
+        <v>0.39040230921883445</v>
       </c>
       <c r="Y32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>15.938976698712738</v>
+        <v>11.39400116482237</v>
       </c>
       <c r="Z32" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.0444315727232136</v>
+        <v>2.0376450778759994</v>
       </c>
       <c r="AA32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.6254797756126362</v>
+        <v>2.5887918486171757</v>
       </c>
       <c r="AB32" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6328,7 +6328,7 @@
       </c>
       <c r="L33" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.373061224489796</v>
+        <v>49.477551020408164</v>
       </c>
       <c r="M33" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6360,31 +6360,31 @@
       </c>
       <c r="U33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39623826235279402</v>
+        <v>0.39540146153475808</v>
       </c>
       <c r="V33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9774916971303236</v>
+        <v>1.9733155061184</v>
       </c>
       <c r="W33" s="2">
         <f t="shared" si="2"/>
-        <v>2.3737299594831178</v>
+        <v>2.3687169676531581</v>
       </c>
       <c r="X33" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.38688624680464861</v>
+        <v>0.38606919615968904</v>
       </c>
       <c r="Y33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.225960567052319</v>
+        <v>11.599152009318585</v>
       </c>
       <c r="Z33" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.0192935284548232</v>
+        <v>2.0150290577133245</v>
       </c>
       <c r="AA33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.6727519660734895</v>
+        <v>2.6354034669842528</v>
       </c>
       <c r="AB33" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="L34" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.647346938775513</v>
+        <v>49.706122448979592</v>
       </c>
       <c r="M34" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6475,31 +6475,31 @@
       </c>
       <c r="U34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39777109957678458</v>
+        <v>0.39730075109313323</v>
       </c>
       <c r="V34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9867517833502122</v>
+        <v>1.9844025284906095</v>
       </c>
       <c r="W34" s="2">
         <f t="shared" si="2"/>
-        <v>2.3845228829269969</v>
+        <v>2.3817032795837427</v>
       </c>
       <c r="X34" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.38320187297553482</v>
+        <v>0.38274875202210668</v>
       </c>
       <c r="Y34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.45645429362882</v>
+        <v>11.763920792079212</v>
       </c>
       <c r="Z34" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>2.0000635033738479</v>
+        <v>1.9976985079354685</v>
       </c>
       <c r="AA34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.7107190595055961</v>
+        <v>2.6728400158793169</v>
       </c>
       <c r="AB34" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="L35" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.843265306122447</v>
+        <v>49.869387755102039</v>
       </c>
       <c r="M35" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6590,31 +6590,31 @@
       </c>
       <c r="U35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.3989559135874301</v>
+        <v>0.39874693357049118</v>
       </c>
       <c r="V35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9938321653641853</v>
+        <v>1.9927877615453662</v>
       </c>
       <c r="W35" s="2">
         <f t="shared" si="2"/>
-        <v>2.3927880789516154</v>
+        <v>2.3915346951158574</v>
       </c>
       <c r="X35" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.38060256829768868</v>
+        <v>0.38040320208086881</v>
       </c>
       <c r="Y35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.626273423496833</v>
+        <v>11.885316249271993</v>
       </c>
       <c r="Z35" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.9864968305913253</v>
+        <v>1.9854562691478987</v>
       </c>
       <c r="AA35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.7386917894623828</v>
+        <v>2.7004218605266637</v>
       </c>
       <c r="AB35" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="L36" s="2">
         <f>L$39 + ((L$40 - L$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
-        <v>49.960816326530612</v>
+        <v>49.967346938775506</v>
       </c>
       <c r="M36" s="2">
         <f>M$39 + ((M$40 - M$39) * ((Table1[[#This Row],[Selected Blend]]) / (1)))</f>
@@ -6705,31 +6705,31 @@
       </c>
       <c r="U36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>0.39972469574597513</v>
+        <v>0.39967245268820734</v>
       </c>
       <c r="V36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[HP]] / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])</f>
-        <v>1.9983829196193079</v>
+        <v>1.9981217357709671</v>
       </c>
       <c r="W36" s="2">
         <f t="shared" si="2"/>
-        <v>2.3981076153652832</v>
+        <v>2.3977941884591742</v>
       </c>
       <c r="X36" s="2">
         <f xml:space="preserve"> ($Q$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$7 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>0.3790557635449866</v>
+        <v>0.37900622186701971</v>
       </c>
       <c r="Y36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.731233501710946</v>
+        <v>11.960347117064654</v>
       </c>
       <c r="Z36" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
-        <v>1.9784235200182265</v>
+        <v>1.9781649448154797</v>
       </c>
       <c r="AA36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.7559808894972755</v>
+        <v>2.7174693661505884</v>
       </c>
       <c r="AB36" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6836,7 +6836,7 @@
       </c>
       <c r="Y37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$7 * $O$7) + Table2[[#This Row],[HP]] / ($L$7 * $O$7)</f>
-        <v>16.767150073325741</v>
+        <v>11.986022131624933</v>
       </c>
       <c r="Z37" s="2">
         <f xml:space="preserve"> ($Q$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]])) + ($P$27 / (Table2[[#This Row],[Damage]] * Table2[[#This Row],[Rate of Fire]]))</f>
@@ -6844,7 +6844,7 @@
       </c>
       <c r="AA37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$27 * $O$27) + Table2[[#This Row],[HP]] / ($L$27 * $O$27)</f>
-        <v>2.761897093163701</v>
+        <v>2.7233028979753868</v>
       </c>
       <c r="AB37" s="2">
         <f xml:space="preserve"> Table2[[#This Row],[Shield Capacity]] / ($L$37 * $O$37) + Table2[[#This Row],[HP]] / ($L$37 * $O$37)</f>
@@ -6877,7 +6877,7 @@
         <v>0.97</v>
       </c>
       <c r="L39" s="9">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M39" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Ready to consider this my 3rd draft!
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Acceleration</t>
   </si>
@@ -124,12 +125,30 @@
   <si>
     <t>Time for AbsMax to Kill</t>
   </si>
+  <si>
+    <t>X killing Vanilla</t>
+  </si>
+  <si>
+    <t>X killing X</t>
+  </si>
+  <si>
+    <t>Vanilla killing X</t>
+  </si>
+  <si>
+    <t>X killing StatMax</t>
+  </si>
+  <si>
+    <t>StatMax killing X</t>
+  </si>
+  <si>
+    <t>AbsoluteMax killing X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +164,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +230,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -207,11 +326,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -226,6 +411,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1601,7 +1826,1224 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PvP Kill Times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X killing X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$7:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>4.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.18752705827989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5681962595002688</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2155060167515912</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.009877708007239</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8905066977285971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8241087056912855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7913993822760759</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7806905712355889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7846339592733456</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7984674329501913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8190248724100251</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8441542973845295</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8723641282724595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9026016944060569</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9341109064865969</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9663386553087718</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9988719392566585</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0313947845567917</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0636581482435004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0954584673307703</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.126622034878916</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.1569933332706506</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.1864260599612146</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.2147759720689173</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.2418949318512631</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2676257032603933</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2917971600990952</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.3142196374519615</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.3346802018137174</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.3529376390642849</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.3687169676531581</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.3817032795837427</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.3915346951158574</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.3977941884591742</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-16B0-4C6F-A50B-EB59E481AED9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X killing Vanilla</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$7:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>6.3090379008746353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5508381617642106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4699980928907586</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7544815057696441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.254531149202454</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8905066977285971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6166955340952416</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4052561254620985</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2384060622838129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1043358552744387</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99494252873563205</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90451004424129744</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82890891072482498</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.76509341210731319</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.71077606586192033</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.66421117249846529</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.62404749128294479</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58922585814955619</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.55890669997929676</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.53241785018922971</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.50921640913012778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.48886048698817847</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47098800921987316</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.455300642055259</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.44155147967900099</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.42953552997221112</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.41908230735202057</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.4100500306514292</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.40232105785599914</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.39579828539109746</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.39040230921883445</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.38606919615968904</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.38274875202210668</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.38040320208086881</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.37900622186701971</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.37854227405247809</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-16B0-4C6F-A50B-EB59E481AED9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vanilla killing X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$7:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1.2984857309260345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.324160745486314</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3991916132789757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5205870704717539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6853558532323829</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8905066977285971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1330483401281315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4099895165987202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.718338963308097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0551054164239968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4172976121141541</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8019242865463028</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2059941758881791</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6265160163075159</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0604985439720469</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5049504950495072</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.9568806057076324</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4132976121141549</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8712102504368122</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.3276272568433356</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7795573675014591</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.224009318578922</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.6579918462434513</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.078513686662788</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.4825835760046644</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.8672102504368127</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.229402446126972</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.566168899242872</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.87451834595225</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.151459522422837</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.39400116482237</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.599152009318585</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.763920792079212</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.885316249271993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.960347117064654</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11.986022131624933</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-16B0-4C6F-A50B-EB59E481AED9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StatMax killing X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$7:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.29502448061400022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30085801243879839</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31790551806272327</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34548736271007008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38292391160513428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42953552997221112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48464258303559599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54756543601958452</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.61762445414847156</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69414000264655273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.77643244673812339</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86382215164747889</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95562948259891467</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0511748048167262</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1497784835252085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2507608839486566</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3534423713113668</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4571433108376337</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5611840677517532</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6648850072780201</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7675664946407301</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8685488950641789</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.9671525737726605</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.062697895990472</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.1545052269419083</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.2418949318512631</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3241873759428344</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.4007029244409153</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4707619425698026</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5336847955537909</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5887918486171757</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6354034669842528</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6728400158793169</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.7004218605266637</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.7174693661505884</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.7233028979753868</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-16B0-4C6F-A50B-EB59E481AED9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AbsoluteMax killing X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$I$7:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26514099125364432</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28016466472303209</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30447206997084547</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33746425655976675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37854227405247809</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42710717201166176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48256000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54430180758017488</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61173364431486876</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68425655976676381</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76127160349854217</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84217982507288625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92638227405247819</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0132800000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.102274052478134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1927654810495627</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2841553352769679</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.375844664723032</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4672345189504372</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5577259475218657</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.6467200000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7336177259475218</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.8178201749271137</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.8987283965014579</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9757434402332359</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.048266355685131</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.115698192419825</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.1774400000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.232892827988338</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.2814577259475217</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.3225357434402336</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.3555279300291545</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.3798353352769679</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.3948590087463555</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-16B0-4C6F-A50B-EB59E481AED9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1778400256"/>
+        <c:axId val="1772807552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1778400256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stat Levels</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1772807552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1772807552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds to Kill</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1778400256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2144,6 +3586,502 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2165,6 +4103,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDDCE86-B095-4ABE-AF56-CACA4F647574}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2594,8 +4573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6965,4 +8944,1160 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:I74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="26">
+        <v>1</v>
+      </c>
+      <c r="D7" s="27">
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="E7">
+        <v>6.3090379008746353</v>
+      </c>
+      <c r="F7">
+        <v>1.2984857309260345</v>
+      </c>
+      <c r="G7">
+        <v>32.929057337220598</v>
+      </c>
+      <c r="H7">
+        <v>0.29502448061400022</v>
+      </c>
+      <c r="I7">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="28">
+        <v>2</v>
+      </c>
+      <c r="D8" s="29">
+        <v>3.18752705827989</v>
+      </c>
+      <c r="E8">
+        <v>4.5508381617642106</v>
+      </c>
+      <c r="F8">
+        <v>1.324160745486314</v>
+      </c>
+      <c r="G8">
+        <v>23.752402999571551</v>
+      </c>
+      <c r="H8">
+        <v>0.30085801243879839</v>
+      </c>
+      <c r="I8">
+        <v>0.26514099125364432</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="26">
+        <v>3</v>
+      </c>
+      <c r="D9" s="27">
+        <v>2.5681962595002688</v>
+      </c>
+      <c r="E9">
+        <v>3.4699980928907586</v>
+      </c>
+      <c r="F9">
+        <v>1.3991916132789757</v>
+      </c>
+      <c r="G9">
+        <v>18.111123749154412</v>
+      </c>
+      <c r="H9">
+        <v>0.31790551806272327</v>
+      </c>
+      <c r="I9">
+        <v>0.28016466472303209</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="28">
+        <v>4</v>
+      </c>
+      <c r="D10" s="29">
+        <v>2.2155060167515912</v>
+      </c>
+      <c r="E10">
+        <v>2.7544815057696441</v>
+      </c>
+      <c r="F10">
+        <v>1.5205870704717539</v>
+      </c>
+      <c r="G10">
+        <v>14.376594476509339</v>
+      </c>
+      <c r="H10">
+        <v>0.34548736271007008</v>
+      </c>
+      <c r="I10">
+        <v>0.30447206997084547</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="26">
+        <v>5</v>
+      </c>
+      <c r="D11" s="27">
+        <v>2.009877708007239</v>
+      </c>
+      <c r="E11">
+        <v>2.254531149202454</v>
+      </c>
+      <c r="F11">
+        <v>1.6853558532323829</v>
+      </c>
+      <c r="G11">
+        <v>11.767180138566845</v>
+      </c>
+      <c r="H11">
+        <v>0.38292391160513428</v>
+      </c>
+      <c r="I11">
+        <v>0.33746425655976675</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="30">
+        <v>6</v>
+      </c>
+      <c r="D12" s="31">
+        <v>1.8905066977285971</v>
+      </c>
+      <c r="E12">
+        <v>1.8905066977285971</v>
+      </c>
+      <c r="F12">
+        <v>1.8905066977285971</v>
+      </c>
+      <c r="G12">
+        <v>9.8672102504368127</v>
+      </c>
+      <c r="H12">
+        <v>0.42953552997221112</v>
+      </c>
+      <c r="I12">
+        <v>0.37854227405247809</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="26">
+        <v>7</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1.8241087056912855</v>
+      </c>
+      <c r="E13">
+        <v>1.6166955340952416</v>
+      </c>
+      <c r="F13">
+        <v>2.1330483401281315</v>
+      </c>
+      <c r="G13">
+        <v>8.4380948054964833</v>
+      </c>
+      <c r="H13">
+        <v>0.48464258303559599</v>
+      </c>
+      <c r="I13">
+        <v>0.42710717201166176</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="28">
+        <v>8</v>
+      </c>
+      <c r="D14" s="29">
+        <v>1.7913993822760759</v>
+      </c>
+      <c r="E14">
+        <v>1.4052561254620985</v>
+      </c>
+      <c r="F14">
+        <v>2.4099895165987202</v>
+      </c>
+      <c r="G14">
+        <v>7.3345191859454317</v>
+      </c>
+      <c r="H14">
+        <v>0.54756543601958452</v>
+      </c>
+      <c r="I14">
+        <v>0.48256000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="26">
+        <v>9</v>
+      </c>
+      <c r="D15" s="27">
+        <v>1.7806905712355889</v>
+      </c>
+      <c r="E15">
+        <v>1.2384060622838129</v>
+      </c>
+      <c r="F15">
+        <v>2.718338963308097</v>
+      </c>
+      <c r="G15">
+        <v>6.463670827853468</v>
+      </c>
+      <c r="H15">
+        <v>0.61762445414847156</v>
+      </c>
+      <c r="I15">
+        <v>0.54430180758017488</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="28">
+        <v>10</v>
+      </c>
+      <c r="D16" s="29">
+        <v>1.7846339592733456</v>
+      </c>
+      <c r="E16">
+        <v>1.1043358552744387</v>
+      </c>
+      <c r="F16">
+        <v>3.0551054164239968</v>
+      </c>
+      <c r="G16">
+        <v>5.7639119100614717</v>
+      </c>
+      <c r="H16">
+        <v>0.69414000264655273</v>
+      </c>
+      <c r="I16">
+        <v>0.61173364431486876</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="26">
+        <v>11</v>
+      </c>
+      <c r="D17" s="27">
+        <v>1.7984674329501913</v>
+      </c>
+      <c r="E17">
+        <v>0.99494252873563205</v>
+      </c>
+      <c r="F17">
+        <v>3.4172976121141541</v>
+      </c>
+      <c r="G17">
+        <v>5.1929501915708798</v>
+      </c>
+      <c r="H17">
+        <v>0.77643244673812339</v>
+      </c>
+      <c r="I17">
+        <v>0.68425655976676381</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="28">
+        <v>12</v>
+      </c>
+      <c r="D18" s="29">
+        <v>1.8190248724100251</v>
+      </c>
+      <c r="E18">
+        <v>0.90451004424129744</v>
+      </c>
+      <c r="F18">
+        <v>3.8019242865463028</v>
+      </c>
+      <c r="G18">
+        <v>4.7209516850080284</v>
+      </c>
+      <c r="H18">
+        <v>0.86382215164747889</v>
+      </c>
+      <c r="I18">
+        <v>0.76127160349854217</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="26">
+        <v>13</v>
+      </c>
+      <c r="D19" s="27">
+        <v>1.8441542973845295</v>
+      </c>
+      <c r="E19">
+        <v>0.82890891072482498</v>
+      </c>
+      <c r="F19">
+        <v>4.2059941758881791</v>
+      </c>
+      <c r="G19">
+        <v>4.3263631440234089</v>
+      </c>
+      <c r="H19">
+        <v>0.95562948259891467</v>
+      </c>
+      <c r="I19">
+        <v>0.84217982507288625</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="28">
+        <v>14</v>
+      </c>
+      <c r="D20" s="29">
+        <v>1.8723641282724595</v>
+      </c>
+      <c r="E20">
+        <v>0.76509341210731319</v>
+      </c>
+      <c r="F20">
+        <v>4.6265160163075159</v>
+      </c>
+      <c r="G20">
+        <v>3.9932879198774183</v>
+      </c>
+      <c r="H20">
+        <v>1.0511748048167262</v>
+      </c>
+      <c r="I20">
+        <v>0.92638227405247819</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="26">
+        <v>15</v>
+      </c>
+      <c r="D21" s="27">
+        <v>1.9026016944060569</v>
+      </c>
+      <c r="E21">
+        <v>0.71077606586192033</v>
+      </c>
+      <c r="F21">
+        <v>5.0604985439720469</v>
+      </c>
+      <c r="G21">
+        <v>3.709786847761138</v>
+      </c>
+      <c r="H21">
+        <v>1.1497784835252085</v>
+      </c>
+      <c r="I21">
+        <v>1.0132800000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="28">
+        <v>16</v>
+      </c>
+      <c r="D22" s="29">
+        <v>1.9341109064865969</v>
+      </c>
+      <c r="E22">
+        <v>0.66421117249846529</v>
+      </c>
+      <c r="F22">
+        <v>5.5049504950495072</v>
+      </c>
+      <c r="G22">
+        <v>3.4667485164722729</v>
+      </c>
+      <c r="H22">
+        <v>1.2507608839486566</v>
+      </c>
+      <c r="I22">
+        <v>1.102274052478134</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="26">
+        <v>17</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1.9663386553087718</v>
+      </c>
+      <c r="E23">
+        <v>0.62404749128294479</v>
+      </c>
+      <c r="F23">
+        <v>5.9568806057076324</v>
+      </c>
+      <c r="G23">
+        <v>3.2571203318902184</v>
+      </c>
+      <c r="H23">
+        <v>1.3534423713113668</v>
+      </c>
+      <c r="I23">
+        <v>1.1927654810495627</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="28">
+        <v>18</v>
+      </c>
+      <c r="D24" s="29">
+        <v>1.9988719392566585</v>
+      </c>
+      <c r="E24">
+        <v>0.58922585814955619</v>
+      </c>
+      <c r="F24">
+        <v>6.4132976121141549</v>
+      </c>
+      <c r="G24">
+        <v>3.0753741493437405</v>
+      </c>
+      <c r="H24">
+        <v>1.4571433108376337</v>
+      </c>
+      <c r="I24">
+        <v>1.2841553352769679</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="26">
+        <v>19</v>
+      </c>
+      <c r="D25" s="27">
+        <v>2.0313947845567917</v>
+      </c>
+      <c r="E25">
+        <v>0.55890669997929676</v>
+      </c>
+      <c r="F25">
+        <v>6.8712102504368122</v>
+      </c>
+      <c r="G25">
+        <v>2.9171279454865204</v>
+      </c>
+      <c r="H25">
+        <v>1.5611840677517532</v>
+      </c>
+      <c r="I25">
+        <v>1.375844664723032</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="28">
+        <v>20</v>
+      </c>
+      <c r="D26" s="29">
+        <v>2.0636581482435004</v>
+      </c>
+      <c r="E26">
+        <v>0.53241785018922971</v>
+      </c>
+      <c r="F26">
+        <v>7.3276272568433356</v>
+      </c>
+      <c r="G26">
+        <v>2.7788734497553698</v>
+      </c>
+      <c r="H26">
+        <v>1.6648850072780201</v>
+      </c>
+      <c r="I26">
+        <v>1.4672345189504372</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="26">
+        <v>21</v>
+      </c>
+      <c r="D27" s="27">
+        <v>2.0954584673307703</v>
+      </c>
+      <c r="E27">
+        <v>0.50921640913012778</v>
+      </c>
+      <c r="F27">
+        <v>7.7795573675014591</v>
+      </c>
+      <c r="G27">
+        <v>2.6577770805553373</v>
+      </c>
+      <c r="H27">
+        <v>1.7675664946407301</v>
+      </c>
+      <c r="I27">
+        <v>1.5577259475218657</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="28">
+        <v>22</v>
+      </c>
+      <c r="D28" s="29">
+        <v>2.126622034878916</v>
+      </c>
+      <c r="E28">
+        <v>0.48886048698817847</v>
+      </c>
+      <c r="F28">
+        <v>8.224009318578922</v>
+      </c>
+      <c r="G28">
+        <v>2.551532461661651</v>
+      </c>
+      <c r="H28">
+        <v>1.8685488950641789</v>
+      </c>
+      <c r="I28">
+        <v>1.6467200000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="26">
+        <v>23</v>
+      </c>
+      <c r="D29" s="27">
+        <v>2.1569933332706506</v>
+      </c>
+      <c r="E29">
+        <v>0.47098800921987316</v>
+      </c>
+      <c r="F29">
+        <v>8.6579918462434513</v>
+      </c>
+      <c r="G29">
+        <v>2.4582498004322524</v>
+      </c>
+      <c r="H29">
+        <v>1.9671525737726605</v>
+      </c>
+      <c r="I29">
+        <v>1.7336177259475218</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="28">
+        <v>24</v>
+      </c>
+      <c r="D30" s="29">
+        <v>2.1864260599612146</v>
+      </c>
+      <c r="E30">
+        <v>0.455300642055259</v>
+      </c>
+      <c r="F30">
+        <v>9.078513686662788</v>
+      </c>
+      <c r="G30">
+        <v>2.3763719894332094</v>
+      </c>
+      <c r="H30">
+        <v>2.062697895990472</v>
+      </c>
+      <c r="I30">
+        <v>1.8178201749271137</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="26">
+        <v>25</v>
+      </c>
+      <c r="D31" s="27">
+        <v>2.2147759720689173</v>
+      </c>
+      <c r="E31">
+        <v>0.44155147967900099</v>
+      </c>
+      <c r="F31">
+        <v>9.4825835760046644</v>
+      </c>
+      <c r="G31">
+        <v>2.3046103415655068</v>
+      </c>
+      <c r="H31">
+        <v>2.1545052269419083</v>
+      </c>
+      <c r="I31">
+        <v>1.8987283965014579</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="30">
+        <v>26</v>
+      </c>
+      <c r="D32" s="31">
+        <v>2.2418949318512631</v>
+      </c>
+      <c r="E32">
+        <v>0.42953552997221112</v>
+      </c>
+      <c r="F32">
+        <v>9.8672102504368127</v>
+      </c>
+      <c r="G32">
+        <v>2.2418949318512631</v>
+      </c>
+      <c r="H32">
+        <v>2.2418949318512631</v>
+      </c>
+      <c r="I32">
+        <v>1.9757434402332359</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="26">
+        <v>27</v>
+      </c>
+      <c r="D33" s="27">
+        <v>2.2676257032603933</v>
+      </c>
+      <c r="E33">
+        <v>0.41908230735202057</v>
+      </c>
+      <c r="F33">
+        <v>10.229402446126972</v>
+      </c>
+      <c r="G33">
+        <v>2.1873359368940024</v>
+      </c>
+      <c r="H33">
+        <v>2.3241873759428344</v>
+      </c>
+      <c r="I33">
+        <v>2.048266355685131</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="28">
+        <v>28</v>
+      </c>
+      <c r="D34" s="29">
+        <v>2.2917971600990952</v>
+      </c>
+      <c r="E34">
+        <v>0.4100500306514292</v>
+      </c>
+      <c r="F34">
+        <v>10.566168899242872</v>
+      </c>
+      <c r="G34">
+        <v>2.1401933516008977</v>
+      </c>
+      <c r="H34">
+        <v>2.4007029244409153</v>
+      </c>
+      <c r="I34">
+        <v>2.115698192419825</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="26">
+        <v>29</v>
+      </c>
+      <c r="D35" s="27">
+        <v>2.3142196374519615</v>
+      </c>
+      <c r="E35">
+        <v>0.40232105785599914</v>
+      </c>
+      <c r="F35">
+        <v>10.87451834595225</v>
+      </c>
+      <c r="G35">
+        <v>2.0998531614899374</v>
+      </c>
+      <c r="H35">
+        <v>2.4707619425698026</v>
+      </c>
+      <c r="I35">
+        <v>2.1774400000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="28">
+        <v>30</v>
+      </c>
+      <c r="D36" s="29">
+        <v>2.3346802018137174</v>
+      </c>
+      <c r="E36">
+        <v>0.39579828539109746</v>
+      </c>
+      <c r="F36">
+        <v>11.151459522422837</v>
+      </c>
+      <c r="G36">
+        <v>2.0658085493210021</v>
+      </c>
+      <c r="H36">
+        <v>2.5336847955537909</v>
+      </c>
+      <c r="I36">
+        <v>2.232892827988338</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="26">
+        <v>31</v>
+      </c>
+      <c r="D37" s="27">
+        <v>2.3529376390642849</v>
+      </c>
+      <c r="E37">
+        <v>0.39040230921883445</v>
+      </c>
+      <c r="F37">
+        <v>11.39400116482237</v>
+      </c>
+      <c r="G37">
+        <v>2.0376450778759994</v>
+      </c>
+      <c r="H37">
+        <v>2.5887918486171757</v>
+      </c>
+      <c r="I37">
+        <v>2.2814577259475217</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="28">
+        <v>32</v>
+      </c>
+      <c r="D38" s="29">
+        <v>2.3687169676531581</v>
+      </c>
+      <c r="E38">
+        <v>0.38606919615968904</v>
+      </c>
+      <c r="F38">
+        <v>11.599152009318585</v>
+      </c>
+      <c r="G38">
+        <v>2.0150290577133245</v>
+      </c>
+      <c r="H38">
+        <v>2.6354034669842528</v>
+      </c>
+      <c r="I38">
+        <v>2.3225357434402336</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="26">
+        <v>33</v>
+      </c>
+      <c r="D39" s="27">
+        <v>2.3817032795837427</v>
+      </c>
+      <c r="E39">
+        <v>0.38274875202210668</v>
+      </c>
+      <c r="F39">
+        <v>11.763920792079212</v>
+      </c>
+      <c r="G39">
+        <v>1.9976985079354685</v>
+      </c>
+      <c r="H39">
+        <v>2.6728400158793169</v>
+      </c>
+      <c r="I39">
+        <v>2.3555279300291545</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="28">
+        <v>34</v>
+      </c>
+      <c r="D40" s="29">
+        <v>2.3915346951158574</v>
+      </c>
+      <c r="E40">
+        <v>0.38040320208086881</v>
+      </c>
+      <c r="F40">
+        <v>11.885316249271993</v>
+      </c>
+      <c r="G40">
+        <v>1.9854562691478987</v>
+      </c>
+      <c r="H40">
+        <v>2.7004218605266637</v>
+      </c>
+      <c r="I40">
+        <v>2.3798353352769679</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="26">
+        <v>35</v>
+      </c>
+      <c r="D41" s="27">
+        <v>2.3977941884591742</v>
+      </c>
+      <c r="E41">
+        <v>0.37900622186701971</v>
+      </c>
+      <c r="F41">
+        <v>11.960347117064654</v>
+      </c>
+      <c r="G41">
+        <v>1.9781649448154797</v>
+      </c>
+      <c r="H41">
+        <v>2.7174693661505884</v>
+      </c>
+      <c r="I41">
+        <v>2.3948590087463555</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="32">
+        <v>36</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2.4</v>
+      </c>
+      <c r="E42">
+        <v>0.37854227405247809</v>
+      </c>
+      <c r="F42">
+        <v>11.986022131624933</v>
+      </c>
+      <c r="G42">
+        <v>1.9757434402332359</v>
+      </c>
+      <c r="H42">
+        <v>2.7233028979753868</v>
+      </c>
+      <c r="I42">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="20">
+        <v>1</v>
+      </c>
+      <c r="D54" s="15">
+        <v>2</v>
+      </c>
+      <c r="E54" s="20">
+        <v>19</v>
+      </c>
+      <c r="F54" s="15">
+        <v>8.7784956268221563</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="21">
+        <v>2</v>
+      </c>
+      <c r="D55" s="16">
+        <v>2.0312303206997084</v>
+      </c>
+      <c r="E55" s="21">
+        <v>20</v>
+      </c>
+      <c r="F55" s="16">
+        <v>9.3336676384839645</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="20">
+        <v>3</v>
+      </c>
+      <c r="D56" s="15">
+        <v>2.1224956268221575</v>
+      </c>
+      <c r="E56" s="20">
+        <v>21</v>
+      </c>
+      <c r="F56" s="15">
+        <v>9.8833819241982503</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="21">
+        <v>4</v>
+      </c>
+      <c r="D57" s="16">
+        <v>2.2701574344023325</v>
+      </c>
+      <c r="E57" s="21">
+        <v>22</v>
+      </c>
+      <c r="F57" s="16">
+        <v>10.423999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="20">
+        <v>5</v>
+      </c>
+      <c r="D58" s="15">
+        <v>2.4705772594752187</v>
+      </c>
+      <c r="E58" s="20">
+        <v>23</v>
+      </c>
+      <c r="F58" s="15">
+        <v>10.951883381924198</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="22">
+        <v>6</v>
+      </c>
+      <c r="D59" s="17">
+        <v>2.7201166180758016</v>
+      </c>
+      <c r="E59" s="21">
+        <v>24</v>
+      </c>
+      <c r="F59" s="16">
+        <v>11.46339358600583</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="20">
+        <v>7</v>
+      </c>
+      <c r="D60" s="15">
+        <v>3.0151370262390671</v>
+      </c>
+      <c r="E60" s="20">
+        <v>25</v>
+      </c>
+      <c r="F60" s="15">
+        <v>11.954892128279884</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="21">
+        <v>8</v>
+      </c>
+      <c r="D61" s="16">
+        <v>3.3520000000000003</v>
+      </c>
+      <c r="E61" s="22">
+        <v>26</v>
+      </c>
+      <c r="F61" s="17">
+        <v>12.422740524781341</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="20">
+        <v>9</v>
+      </c>
+      <c r="D62" s="15">
+        <v>3.7270670553935856</v>
+      </c>
+      <c r="E62" s="20">
+        <v>27</v>
+      </c>
+      <c r="F62" s="15">
+        <v>12.86330029154519</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="21">
+        <v>10</v>
+      </c>
+      <c r="D63" s="16">
+        <v>4.1366997084548096</v>
+      </c>
+      <c r="E63" s="21">
+        <v>28</v>
+      </c>
+      <c r="F63" s="16">
+        <v>13.272932944606413</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="20">
+        <v>11</v>
+      </c>
+      <c r="D64" s="15">
+        <v>4.5772594752186588</v>
+      </c>
+      <c r="E64" s="20">
+        <v>29</v>
+      </c>
+      <c r="F64" s="15">
+        <v>13.648000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="21">
+        <v>12</v>
+      </c>
+      <c r="D65" s="16">
+        <v>5.0451078717201163</v>
+      </c>
+      <c r="E65" s="21">
+        <v>30</v>
+      </c>
+      <c r="F65" s="16">
+        <v>13.984862973760933</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="20">
+        <v>13</v>
+      </c>
+      <c r="D66" s="15">
+        <v>5.5366064139941686</v>
+      </c>
+      <c r="E66" s="20">
+        <v>31</v>
+      </c>
+      <c r="F66" s="15">
+        <v>14.279883381924199</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="21">
+        <v>14</v>
+      </c>
+      <c r="D67" s="16">
+        <v>6.0481166180758024</v>
+      </c>
+      <c r="E67" s="21">
+        <v>32</v>
+      </c>
+      <c r="F67" s="16">
+        <v>14.529422740524781</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="20">
+        <v>15</v>
+      </c>
+      <c r="D68" s="15">
+        <v>6.5760000000000014</v>
+      </c>
+      <c r="E68" s="20">
+        <v>33</v>
+      </c>
+      <c r="F68" s="15">
+        <v>14.729842565597666</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="21">
+        <v>16</v>
+      </c>
+      <c r="D69" s="16">
+        <v>7.1166180758017488</v>
+      </c>
+      <c r="E69" s="21">
+        <v>34</v>
+      </c>
+      <c r="F69" s="16">
+        <v>14.877504373177842</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="20">
+        <v>17</v>
+      </c>
+      <c r="D70" s="15">
+        <v>7.6663323615160346</v>
+      </c>
+      <c r="E70" s="20">
+        <v>35</v>
+      </c>
+      <c r="F70" s="15">
+        <v>14.968769679300292</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="21">
+        <v>18</v>
+      </c>
+      <c r="D71" s="16">
+        <v>8.2215043731778419</v>
+      </c>
+      <c r="E71" s="23">
+        <v>36</v>
+      </c>
+      <c r="F71" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D73" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="11">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Coins now scale based on value
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -3003,6 +3003,1242 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stat Growth Curves</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0-1 Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8571428571428571E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7142857142857141E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25714285714285712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.34285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.37142857142857144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42857142857142855</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.45714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.48571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.51428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.54285714285714282</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.62857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.65714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.74285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.77142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.82857142857142863</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.8571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.88571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.94285714285714284</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.97142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D91B-463A-9357-B6D58483131C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Smooth Stop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6326530612244907E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11102040816326531</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1640816326530613</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21551020408163268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26530612244897944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31346938775510214</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35999999999999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40489795918367344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44816326530612238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48979591836734693</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52979591836734685</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.56816326530612238</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.60489795918367351</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.67346938775510212</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.7053061224489795</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7355102040816327</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.76408163265306117</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79102040816326524</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.81632653061224492</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86204081632653062</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.88244897959183677</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9012244897959184</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.91836734693877553</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.93387755102040815</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.94775510204081637</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.97061224489795916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.97959183673469385</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98693877551020404</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99265306122448982</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.99673469387755098</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99918367346938775</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D91B-463A-9357-B6D58483131C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Smooth Start</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1632653061224482E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2653061224489793E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3469387755102046E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3061224489795917E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0408163265306121E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9387755102040818E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0000000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2244897959183668E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6122448979591825E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1632653061224483E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.8775510204081624E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11755102040816327</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1379591836734694</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18367346938775508</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.20897959183673467</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.23591836734693877</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2644897959183673</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.29469387755102039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.32653061224489793</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.39510204081632649</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.43183673469387757</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.47020408163265309</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.51020408163265307</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.55183673469387762</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.59510204081632656</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.64000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.68653061224489809</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.73469387755102034</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.78448979591836732</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.8359183673469387</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.88897959183673469</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.94367346938775509</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D91B-463A-9357-B6D58483131C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Smooth Step</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4023323615160351E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4227405247813405E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0781341107871724E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6198250728862971E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.53935860058309E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.8087463556851311E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13285131195335276</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16436151603498539</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19825072886297376</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23423906705539357</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27204664723032068</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.31139358600583095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.35200000000000009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.39358600583090375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.43587172011661807</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47857725947521862</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.52142274052478133</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.56412827988338188</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.60641399416909614</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.64800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.688606413994169</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.72795335276967932</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.76576093294460645</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.80174927113702621</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.83563848396501461</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.86714868804664724</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.89600000000000013</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.92191253644314874</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94460641399416911</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.96380174927113704</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.97921865889212822</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.99057725947521869</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99759766763848401</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D91B-463A-9357-B6D58483131C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="133813567"/>
+        <c:axId val="133812319"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Stat Level</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="34925" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                        <a:srgbClr val="000000">
+                          <a:alpha val="63000"/>
+                        </a:srgbClr>
+                      </a:outerShdw>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$37</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="36"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>36</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-D91B-463A-9357-B6D58483131C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="133813567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stat Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133812319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133812319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Blend Weight</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133813567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3044,6 +4280,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4082,6 +5358,502 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4156,6 +5928,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>376517</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>13135</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EB60420-A163-477E-9727-50FC6218076E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4573,7 +6383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G38" sqref="G38:H40"/>
     </sheetView>
   </sheetViews>
@@ -8950,8 +10760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Thesis paper is up to Revision 7!
</commit_message>
<xml_diff>
--- a/Docs/StatBalanceSheet.xlsx
+++ b/Docs/StatBalanceSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Acceleration</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>AbsoluteMax killing X</t>
+  </si>
+  <si>
+    <t>Control Points</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -450,6 +453,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10758,10 +10770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:I74"/>
+  <dimension ref="C6:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73:G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11905,6 +11917,39 @@
         <v>15</v>
       </c>
     </row>
+    <row r="76" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" s="36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="20">
+        <v>1</v>
+      </c>
+      <c r="E77" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="21">
+        <v>36</v>
+      </c>
+      <c r="E78" s="16">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>